<commit_message>
Dynamics First Manual GUI
</commit_message>
<xml_diff>
--- a/0 DyTech Informations/Dytech Balance.xlsx
+++ b/0 DyTech Informations/Dytech Balance.xlsx
@@ -4622,8 +4622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35:P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5251,7 +5251,7 @@
         <v>0.9</v>
       </c>
       <c r="G18" s="86">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H18" s="87" t="s">
         <v>53</v>
@@ -5292,7 +5292,7 @@
         <v>0.8</v>
       </c>
       <c r="G19" s="86">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="H19" s="87" t="s">
         <v>53</v>
@@ -5333,7 +5333,7 @@
         <v>0.7</v>
       </c>
       <c r="G20" s="86">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H20" s="87" t="s">
         <v>53</v>
@@ -5417,11 +5417,11 @@
       </c>
       <c r="G22" s="89">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="H22" s="90">
         <f t="shared" ref="H22:H24" si="10">IFERROR(60/F22*G22,"")</f>
-        <v>16.666666666666668</v>
+        <v>25</v>
       </c>
       <c r="I22" s="91">
         <f t="shared" ref="I22:L22" si="11">I$6*I18</f>
@@ -5445,7 +5445,7 @@
       </c>
       <c r="N22" s="89">
         <f t="shared" ref="N22:N24" si="12">IFERROR(K22/M22*H22,"")</f>
-        <v>5.0250000000000004</v>
+        <v>7.5374999999999996</v>
       </c>
       <c r="O22" s="89"/>
       <c r="P22" s="92">
@@ -5468,11 +5468,11 @@
       </c>
       <c r="G23" s="89">
         <f t="shared" si="14"/>
-        <v>6.25</v>
+        <v>8.75</v>
       </c>
       <c r="H23" s="90">
         <f t="shared" si="10"/>
-        <v>23.4375</v>
+        <v>32.8125</v>
       </c>
       <c r="I23" s="91">
         <f t="shared" ref="I23:L23" si="15">I$6*I19</f>
@@ -5496,7 +5496,7 @@
       </c>
       <c r="N23" s="89">
         <f t="shared" si="12"/>
-        <v>6.28125</v>
+        <v>8.7937500000000011</v>
       </c>
       <c r="O23" s="89"/>
       <c r="P23" s="92">
@@ -5519,11 +5519,11 @@
       </c>
       <c r="G24" s="89">
         <f t="shared" si="16"/>
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="H24" s="90">
         <f t="shared" si="10"/>
-        <v>32.142857142857139</v>
+        <v>42.857142857142854</v>
       </c>
       <c r="I24" s="91">
         <f t="shared" ref="I24:L24" si="17">I$6*I20</f>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="N24" s="89">
         <f t="shared" si="12"/>
-        <v>7.5374999999999996</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="O24" s="89"/>
       <c r="P24" s="92">
@@ -5607,10 +5607,10 @@
         <v>1</v>
       </c>
       <c r="F27" s="93">
+        <v>0.9</v>
+      </c>
+      <c r="G27" s="93">
         <v>1</v>
-      </c>
-      <c r="G27" s="93">
-        <v>1.5</v>
       </c>
       <c r="H27" s="94" t="s">
         <v>53</v>
@@ -5619,13 +5619,13 @@
         <v>1.5</v>
       </c>
       <c r="J27" s="93">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K27" s="93">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="L27" s="93">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="M27" s="94" t="s">
         <v>53</v>
@@ -5648,10 +5648,10 @@
         <v>2</v>
       </c>
       <c r="F28" s="93">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G28" s="93">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="H28" s="94" t="s">
         <v>53</v>
@@ -5660,13 +5660,13 @@
         <v>1.625</v>
       </c>
       <c r="J28" s="93">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="K28" s="93">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="L28" s="93">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="M28" s="94" t="s">
         <v>53</v>
@@ -5689,7 +5689,7 @@
         <v>3</v>
       </c>
       <c r="F29" s="93">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G29" s="93">
         <v>2</v>
@@ -5707,7 +5707,7 @@
         <v>0.6</v>
       </c>
       <c r="L29" s="93">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="M29" s="94" t="s">
         <v>53</v>
@@ -5772,15 +5772,15 @@
       </c>
       <c r="F31" s="97">
         <f t="shared" ref="F31:G31" si="18">F$6*F27</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G31" s="97">
         <f t="shared" si="18"/>
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="H31" s="97">
         <f t="shared" ref="H31:H33" si="19">IFERROR(60/F31*G31,"")</f>
-        <v>22.5</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="I31" s="98">
         <f t="shared" ref="I31:L31" si="20">I$6*I27</f>
@@ -5788,23 +5788,23 @@
       </c>
       <c r="J31" s="97">
         <f t="shared" si="20"/>
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="K31" s="97">
         <f t="shared" si="20"/>
-        <v>201</v>
+        <v>160.80000000000001</v>
       </c>
       <c r="L31" s="97">
         <f t="shared" si="20"/>
-        <v>4.5</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="M31" s="97">
         <f>60/F31*J31</f>
-        <v>600</v>
+        <v>533.33333333333337</v>
       </c>
       <c r="N31" s="97">
         <f t="shared" ref="N31:N33" si="21">IFERROR(K31/M31*H31,"")</f>
-        <v>7.5375000000000005</v>
+        <v>5.0250000000000004</v>
       </c>
       <c r="O31" s="97"/>
       <c r="P31" s="99">
@@ -5823,15 +5823,15 @@
       </c>
       <c r="F32" s="97">
         <f t="shared" ref="F32:G32" si="23">F$6*F28</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G32" s="97">
         <f t="shared" si="23"/>
-        <v>8.75</v>
+        <v>7.5</v>
       </c>
       <c r="H32" s="97">
         <f t="shared" si="19"/>
-        <v>26.25</v>
+        <v>25</v>
       </c>
       <c r="I32" s="98">
         <f t="shared" ref="I32:L32" si="24">I$6*I28</f>
@@ -5839,23 +5839,23 @@
       </c>
       <c r="J32" s="97">
         <f t="shared" si="24"/>
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="K32" s="97">
         <f t="shared" si="24"/>
-        <v>150.75</v>
+        <v>140.69999999999999</v>
       </c>
       <c r="L32" s="97">
         <f t="shared" si="24"/>
-        <v>4.5</v>
+        <v>4.1999999999999993</v>
       </c>
       <c r="M32" s="97">
         <f>60/F32*J32</f>
-        <v>450</v>
+        <v>466.66666666666669</v>
       </c>
       <c r="N32" s="97">
         <f t="shared" si="21"/>
-        <v>8.7937500000000011</v>
+        <v>7.5374999999999996</v>
       </c>
       <c r="O32" s="97"/>
       <c r="P32" s="99">
@@ -5874,7 +5874,7 @@
       </c>
       <c r="F33" s="97">
         <f t="shared" ref="F33:G33" si="25">F$6*F29</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G33" s="97">
         <f t="shared" si="25"/>
@@ -5882,7 +5882,7 @@
       </c>
       <c r="H33" s="97">
         <f t="shared" si="19"/>
-        <v>30</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="I33" s="98">
         <f t="shared" ref="I33:L33" si="26">I$6*I29</f>
@@ -5898,15 +5898,15 @@
       </c>
       <c r="L33" s="97">
         <f t="shared" si="26"/>
-        <v>4.5</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="M33" s="97">
         <f>60/F33*J33</f>
-        <v>360</v>
+        <v>400</v>
       </c>
       <c r="N33" s="97">
         <f t="shared" si="21"/>
-        <v>10.049999999999999</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="O33" s="97"/>
       <c r="P33" s="99">
@@ -5966,7 +5966,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="101">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G36" s="101">
         <v>5</v>
@@ -6007,7 +6007,7 @@
         <v>2</v>
       </c>
       <c r="F37" s="101">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="G37" s="101">
         <v>7.5</v>
@@ -6048,7 +6048,7 @@
         <v>3</v>
       </c>
       <c r="F38" s="101">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G38" s="101">
         <v>10</v>
@@ -6131,7 +6131,7 @@
       </c>
       <c r="F40" s="105">
         <f t="shared" ref="F40:G40" si="27">F$6*F36</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G40" s="105">
         <f t="shared" si="27"/>
@@ -6139,7 +6139,7 @@
       </c>
       <c r="H40" s="105">
         <f t="shared" ref="H40:H42" si="28">IFERROR(60/F40*G40,"")</f>
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="I40" s="106">
         <f t="shared" ref="I40:L40" si="29">I$6*I36</f>
@@ -6159,11 +6159,11 @@
       </c>
       <c r="M40" s="105">
         <f>60/F40*J40</f>
-        <v>1050</v>
+        <v>350</v>
       </c>
       <c r="N40" s="105">
         <f t="shared" ref="N40:N42" si="30">IFERROR(K40/M40*H40,"")</f>
-        <v>25.125</v>
+        <v>25.124999999999996</v>
       </c>
       <c r="O40" s="105"/>
       <c r="P40" s="107">
@@ -6182,7 +6182,7 @@
       </c>
       <c r="F41" s="105">
         <f t="shared" ref="F41:G41" si="32">F$6*F37</f>
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="G41" s="105">
         <f t="shared" si="32"/>
@@ -6190,7 +6190,7 @@
       </c>
       <c r="H41" s="105">
         <f t="shared" si="28"/>
-        <v>112.5</v>
+        <v>50</v>
       </c>
       <c r="I41" s="106">
         <f t="shared" ref="I41:L41" si="33">I$6*I37</f>
@@ -6210,11 +6210,11 @@
       </c>
       <c r="M41" s="105">
         <f>60/F41*J41</f>
-        <v>1200</v>
+        <v>533.33333333333326</v>
       </c>
       <c r="N41" s="105">
         <f t="shared" si="30"/>
-        <v>37.6875</v>
+        <v>37.687500000000007</v>
       </c>
       <c r="O41" s="105"/>
       <c r="P41" s="107">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="F42" s="105">
         <f t="shared" ref="F42:G42" si="34">F$6*F38</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G42" s="105">
         <f t="shared" si="34"/>
@@ -6241,7 +6241,7 @@
       </c>
       <c r="H42" s="105">
         <f t="shared" si="28"/>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="I42" s="106">
         <f t="shared" ref="I42:L42" si="35">I$6*I38</f>
@@ -6261,11 +6261,11 @@
       </c>
       <c r="M42" s="105">
         <f>60/F42*J42</f>
-        <v>1350</v>
+        <v>900</v>
       </c>
       <c r="N42" s="105">
         <f t="shared" si="30"/>
-        <v>50.25</v>
+        <v>50.249999999999993</v>
       </c>
       <c r="O42" s="105"/>
       <c r="P42" s="107">

</xml_diff>

<commit_message>
completed balance sheet for nuclear power
</commit_message>
<xml_diff>
--- a/0 DyTech Informations/Dytech Balance.xlsx
+++ b/0 DyTech Informations/Dytech Balance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -256,6 +256,30 @@
             <family val="2"/>
           </rPr>
           <t>Sum of energy required to create all the items for the recipe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MagicLegend:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Energy used by the chemical processor to create the fuel stated in colum A</t>
         </r>
       </text>
     </comment>
@@ -619,7 +643,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="395">
   <si>
     <t>README</t>
   </si>
@@ -1632,9 +1656,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Clean-water</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -1701,9 +1722,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>54 minuten</t>
-  </si>
-  <si>
     <t>Energy consumption</t>
   </si>
   <si>
@@ -1722,22 +1740,110 @@
     <t>(0.5 speed)</t>
   </si>
   <si>
-    <t>Water cleaner</t>
+    <t>Tier 1:</t>
+  </si>
+  <si>
+    <t>crystal</t>
+  </si>
+  <si>
+    <t>raw-ruby</t>
+  </si>
+  <si>
+    <t>raw-sapphire</t>
+  </si>
+  <si>
+    <t>raw-emerald</t>
+  </si>
+  <si>
+    <t>raw-topaz</t>
+  </si>
+  <si>
+    <t>raw-diamond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier 2: </t>
+  </si>
+  <si>
+    <t>cut-ruby</t>
+  </si>
+  <si>
+    <t>cut-sapphire</t>
+  </si>
+  <si>
+    <t>cut-emerald</t>
+  </si>
+  <si>
+    <t>cut-topaz</t>
+  </si>
+  <si>
+    <t>cut-diamond</t>
+  </si>
+  <si>
+    <t>compressed-ruby</t>
+  </si>
+  <si>
+    <t>compressed-sapphire</t>
+  </si>
+  <si>
+    <t>compressed-emerald</t>
+  </si>
+  <si>
+    <t>compressed-topaz</t>
+  </si>
+  <si>
+    <t>compressed-diamond</t>
+  </si>
+  <si>
+    <t>Tier 3:</t>
+  </si>
+  <si>
+    <t>Tier 4:</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Tier 2:</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>Total time</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>Total energy</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
     <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="175" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1845,6 +1951,18 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3D3C40"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2274,7 +2392,7 @@
     <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2565,6 +2683,7 @@
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
@@ -2612,10 +2731,14 @@
     <xf numFmtId="4" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="15" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="40" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="40" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -8414,17 +8537,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="214" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="214" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" style="214" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="214"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="215" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="215" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="215" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="215" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="215"/>
     <col min="18" max="18" width="10.7109375" customWidth="1"/>
     <col min="19" max="20" width="9.28515625" customWidth="1"/>
   </cols>
@@ -8434,7 +8561,7 @@
       <c r="Y1" s="119"/>
       <c r="Z1" s="119"/>
       <c r="AC1" s="119" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -8455,49 +8582,49 @@
       <c r="A3" s="144" t="s">
         <v>333</v>
       </c>
-      <c r="D3" s="197" t="s">
+      <c r="D3" s="198" t="s">
+        <v>344</v>
+      </c>
+      <c r="E3" s="199"/>
+      <c r="F3" s="199"/>
+      <c r="G3" s="199"/>
+      <c r="H3" s="200"/>
+      <c r="Q3" s="211" t="s">
+        <v>346</v>
+      </c>
+      <c r="R3" s="206"/>
+      <c r="S3" s="206"/>
+      <c r="T3" s="206"/>
+      <c r="U3" s="206"/>
+      <c r="V3" s="206"/>
+      <c r="W3" s="206"/>
+      <c r="X3" s="206"/>
+      <c r="Y3" s="206"/>
+      <c r="Z3" s="206"/>
+      <c r="AA3" s="150"/>
+    </row>
+    <row r="4" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="201" t="s">
         <v>345</v>
       </c>
-      <c r="E3" s="198"/>
-      <c r="F3" s="198"/>
-      <c r="G3" s="198"/>
-      <c r="H3" s="199"/>
-      <c r="Q3" s="210" t="s">
-        <v>347</v>
-      </c>
-      <c r="R3" s="205"/>
-      <c r="S3" s="205"/>
-      <c r="T3" s="205"/>
-      <c r="U3" s="205"/>
-      <c r="V3" s="205"/>
-      <c r="W3" s="205"/>
-      <c r="X3" s="205"/>
-      <c r="Y3" s="205"/>
-      <c r="Z3" s="205"/>
-      <c r="AA3" s="150"/>
-    </row>
-    <row r="4" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="200" t="s">
-        <v>346</v>
-      </c>
-      <c r="E4" s="201"/>
-      <c r="F4" s="201"/>
-      <c r="G4" s="201"/>
-      <c r="H4" s="202"/>
-      <c r="Q4" s="211"/>
-      <c r="R4" s="205"/>
-      <c r="S4" s="205"/>
-      <c r="T4" s="205"/>
-      <c r="U4" s="205"/>
-      <c r="V4" s="205"/>
-      <c r="W4" s="205"/>
-      <c r="X4" s="205"/>
-      <c r="Y4" s="205"/>
-      <c r="Z4" s="205"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="203"/>
+      <c r="Q4" s="212"/>
+      <c r="R4" s="206"/>
+      <c r="S4" s="206"/>
+      <c r="T4" s="206"/>
+      <c r="U4" s="206"/>
+      <c r="V4" s="206"/>
+      <c r="W4" s="206"/>
+      <c r="X4" s="206"/>
+      <c r="Y4" s="206"/>
+      <c r="Z4" s="206"/>
       <c r="AA4" s="150"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="Q5" s="203"/>
+      <c r="Q5" s="204"/>
       <c r="R5" s="150"/>
       <c r="S5" s="150"/>
       <c r="T5" s="150"/>
@@ -8522,42 +8649,42 @@
         <v>336</v>
       </c>
       <c r="F6" s="146"/>
-      <c r="G6" s="215" t="s">
+      <c r="G6" s="216" t="s">
         <v>335</v>
       </c>
-      <c r="H6" s="215" t="s">
+      <c r="H6" s="216" t="s">
         <v>335</v>
       </c>
       <c r="I6" s="146"/>
-      <c r="J6" s="215" t="s">
+      <c r="J6" s="216" t="s">
         <v>335</v>
       </c>
-      <c r="K6" s="215" t="s">
-        <v>344</v>
+      <c r="K6" s="216" t="s">
+        <v>343</v>
       </c>
       <c r="L6" s="146"/>
-      <c r="M6" s="215" t="s">
+      <c r="M6" s="216" t="s">
+        <v>337</v>
+      </c>
+      <c r="N6" s="216" t="s">
         <v>338</v>
       </c>
-      <c r="N6" s="215" t="s">
-        <v>339</v>
-      </c>
-      <c r="Q6" s="203"/>
-      <c r="R6" s="207" t="s">
-        <v>348</v>
-      </c>
-      <c r="S6" s="207"/>
+      <c r="Q6" s="204"/>
+      <c r="R6" s="208" t="s">
+        <v>347</v>
+      </c>
+      <c r="S6" s="208"/>
       <c r="T6" s="150"/>
-      <c r="U6" s="206" t="s">
-        <v>361</v>
-      </c>
-      <c r="V6" s="206"/>
-      <c r="W6" s="206"/>
+      <c r="U6" s="207" t="s">
+        <v>359</v>
+      </c>
+      <c r="V6" s="207"/>
+      <c r="W6" s="207"/>
       <c r="X6" s="150"/>
-      <c r="Y6" s="196" t="s">
-        <v>365</v>
-      </c>
-      <c r="Z6" s="196"/>
+      <c r="Y6" s="197" t="s">
+        <v>363</v>
+      </c>
+      <c r="Z6" s="197"/>
       <c r="AA6" s="150"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -8567,36 +8694,36 @@
       <c r="D7" s="146"/>
       <c r="E7" s="146"/>
       <c r="F7" s="186"/>
-      <c r="G7" s="215" t="s">
-        <v>343</v>
-      </c>
-      <c r="H7" s="216" t="s">
-        <v>343</v>
+      <c r="G7" s="216" t="s">
+        <v>342</v>
+      </c>
+      <c r="H7" s="217" t="s">
+        <v>342</v>
       </c>
       <c r="I7" s="186"/>
-      <c r="J7" s="215" t="s">
-        <v>343</v>
-      </c>
-      <c r="K7" s="215" t="s">
-        <v>343</v>
+      <c r="J7" s="216" t="s">
+        <v>342</v>
+      </c>
+      <c r="K7" s="216" t="s">
+        <v>342</v>
       </c>
       <c r="L7" s="186"/>
-      <c r="M7" s="216" t="s">
-        <v>340</v>
-      </c>
-      <c r="N7" s="216" t="s">
-        <v>340</v>
-      </c>
-      <c r="Q7" s="203"/>
-      <c r="R7" s="204"/>
-      <c r="S7" s="208" t="s">
-        <v>340</v>
+      <c r="M7" s="217" t="s">
+        <v>339</v>
+      </c>
+      <c r="N7" s="217" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q7" s="204"/>
+      <c r="R7" s="205"/>
+      <c r="S7" s="209" t="s">
+        <v>339</v>
       </c>
       <c r="T7" s="150"/>
-      <c r="U7" s="195"/>
-      <c r="V7" s="195"/>
-      <c r="W7" s="209" t="s">
-        <v>363</v>
+      <c r="U7" s="196"/>
+      <c r="V7" s="196"/>
+      <c r="W7" s="210" t="s">
+        <v>361</v>
       </c>
       <c r="X7" s="150"/>
       <c r="Y7" s="150"/>
@@ -8608,45 +8735,48 @@
         <v>323</v>
       </c>
       <c r="B8" s="186"/>
-      <c r="C8" s="220" t="s">
-        <v>342</v>
-      </c>
-      <c r="D8" s="220"/>
+      <c r="C8" s="222" t="s">
+        <v>341</v>
+      </c>
+      <c r="D8" s="222"/>
       <c r="E8" s="185">
         <v>1</v>
       </c>
       <c r="F8" s="186"/>
-      <c r="G8" s="213">
+      <c r="G8" s="214">
         <f>W9*Y9*S8</f>
         <v>1800</v>
       </c>
-      <c r="H8" s="217">
+      <c r="H8" s="218">
         <f>G8</f>
         <v>1800</v>
       </c>
       <c r="I8" s="186"/>
-      <c r="J8" s="213"/>
-      <c r="K8" s="213"/>
+      <c r="J8" s="214">
+        <f>G8</f>
+        <v>1800</v>
+      </c>
+      <c r="K8" s="214"/>
       <c r="L8" s="186"/>
-      <c r="M8" s="218">
+      <c r="M8" s="219">
         <f>S8</f>
         <v>10</v>
       </c>
-      <c r="N8" s="218"/>
-      <c r="Q8" s="203"/>
-      <c r="R8" s="193" t="s">
+      <c r="N8" s="219"/>
+      <c r="Q8" s="204"/>
+      <c r="R8" s="194" t="s">
         <v>323</v>
       </c>
       <c r="S8" s="189">
         <v>10</v>
       </c>
       <c r="T8" s="150"/>
-      <c r="U8" s="191" t="s">
-        <v>362</v>
-      </c>
-      <c r="V8" s="192"/>
+      <c r="U8" s="192" t="s">
+        <v>360</v>
+      </c>
+      <c r="V8" s="193"/>
       <c r="W8" s="187">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="X8" s="150"/>
       <c r="Y8" s="150"/>
@@ -8656,38 +8786,42 @@
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="149"/>
       <c r="B9" s="186"/>
-      <c r="C9" s="220" t="s">
-        <v>341</v>
-      </c>
-      <c r="D9" s="220"/>
+      <c r="C9" s="222" t="s">
+        <v>340</v>
+      </c>
+      <c r="D9" s="222"/>
       <c r="E9" s="185"/>
       <c r="F9" s="186"/>
-      <c r="G9" s="213"/>
-      <c r="H9" s="213"/>
+      <c r="G9" s="214"/>
+      <c r="H9" s="223">
+        <f>H8</f>
+        <v>1800</v>
+      </c>
       <c r="I9" s="186"/>
-      <c r="J9" s="213"/>
-      <c r="K9" s="213"/>
+      <c r="J9" s="214"/>
+      <c r="K9" s="214"/>
       <c r="L9" s="186"/>
-      <c r="M9" s="213">
+      <c r="M9" s="214">
         <f>M8</f>
         <v>10</v>
       </c>
-      <c r="N9" s="213">
+      <c r="N9" s="214">
         <f>M9</f>
         <v>10</v>
       </c>
-      <c r="Q9" s="203"/>
-      <c r="R9" s="194" t="s">
+      <c r="O9" s="227"/>
+      <c r="Q9" s="204"/>
+      <c r="R9" s="195" t="s">
         <v>324</v>
       </c>
       <c r="S9" s="188">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="T9" s="150"/>
-      <c r="U9" s="191" t="s">
-        <v>364</v>
-      </c>
-      <c r="V9" s="192"/>
+      <c r="U9" s="192" t="s">
+        <v>362</v>
+      </c>
+      <c r="V9" s="193"/>
       <c r="W9" s="187">
         <v>90</v>
       </c>
@@ -8696,7 +8830,7 @@
         <v>2</v>
       </c>
       <c r="Z9" s="119" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AA9" s="150"/>
     </row>
@@ -8707,32 +8841,28 @@
       <c r="D10" s="149"/>
       <c r="E10" s="185"/>
       <c r="F10" s="186"/>
-      <c r="G10" s="213"/>
-      <c r="H10" s="213"/>
+      <c r="G10" s="214"/>
+      <c r="H10" s="214"/>
       <c r="I10" s="186"/>
-      <c r="J10" s="213"/>
-      <c r="K10" s="219">
+      <c r="J10" s="214"/>
+      <c r="K10" s="221">
         <f>H8</f>
         <v>1800</v>
       </c>
       <c r="L10" s="186"/>
-      <c r="M10" s="213"/>
-      <c r="N10" s="213"/>
-      <c r="Q10" s="203"/>
-      <c r="R10" s="194" t="s">
+      <c r="M10" s="214"/>
+      <c r="N10" s="214"/>
+      <c r="Q10" s="204"/>
+      <c r="R10" s="195" t="s">
         <v>325</v>
       </c>
       <c r="S10" s="188">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="T10" s="150"/>
-      <c r="U10" s="191" t="s">
-        <v>367</v>
-      </c>
-      <c r="V10" s="192"/>
-      <c r="W10" s="187">
-        <v>50</v>
-      </c>
+      <c r="U10" s="192"/>
+      <c r="V10" s="193"/>
+      <c r="W10" s="187"/>
       <c r="X10" s="150"/>
       <c r="Y10" s="150"/>
       <c r="Z10" s="150"/>
@@ -8751,33 +8881,36 @@
         <v>2</v>
       </c>
       <c r="F11" s="186"/>
-      <c r="G11" s="213">
+      <c r="G11" s="214">
+        <f>J8</f>
+        <v>1800</v>
+      </c>
+      <c r="H11" s="214">
+        <f>G11*E11</f>
+        <v>3600</v>
+      </c>
+      <c r="I11" s="186"/>
+      <c r="J11" s="214">
         <f>W8*S9</f>
-        <v>30000</v>
-      </c>
-      <c r="H11" s="213">
-        <f>G11*E11</f>
-        <v>60000</v>
-      </c>
-      <c r="I11" s="186"/>
-      <c r="J11" s="213"/>
-      <c r="K11" s="213"/>
+        <v>60</v>
+      </c>
+      <c r="K11" s="214"/>
       <c r="L11" s="186"/>
-      <c r="M11" s="213">
-        <f>S9</f>
+      <c r="M11" s="214">
+        <f>S9+M8*E11</f>
+        <v>80</v>
+      </c>
+      <c r="N11" s="214"/>
+      <c r="Q11" s="204"/>
+      <c r="R11" s="195" t="s">
+        <v>326</v>
+      </c>
+      <c r="S11" s="188">
         <v>120</v>
       </c>
-      <c r="N11" s="213"/>
-      <c r="Q11" s="203"/>
-      <c r="R11" s="194" t="s">
-        <v>326</v>
-      </c>
-      <c r="S11" s="188">
-        <v>240</v>
-      </c>
       <c r="T11" s="150"/>
-      <c r="U11" s="192"/>
-      <c r="V11" s="192"/>
+      <c r="U11" s="193"/>
+      <c r="V11" s="193"/>
       <c r="W11" s="187"/>
       <c r="X11" s="150"/>
       <c r="Y11" s="150"/>
@@ -8787,41 +8920,36 @@
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="149"/>
       <c r="B12" s="186"/>
-      <c r="C12" s="148" t="s">
-        <v>337</v>
-      </c>
+      <c r="C12" s="148"/>
       <c r="D12" s="149"/>
-      <c r="E12" s="185">
-        <v>100</v>
-      </c>
+      <c r="E12" s="185"/>
       <c r="F12" s="186"/>
-      <c r="G12" s="217">
-        <f>W10*S31</f>
-        <v>10.869565217391305</v>
-      </c>
-      <c r="H12" s="218">
-        <f>E12/9.2</f>
-        <v>10.869565217391305</v>
+      <c r="G12" s="218"/>
+      <c r="H12" s="219">
+        <f>G12</f>
+        <v>0</v>
       </c>
       <c r="I12" s="186"/>
-      <c r="J12" s="213"/>
-      <c r="K12" s="213"/>
+      <c r="J12" s="214">
+        <f>J11+H13</f>
+        <v>3660</v>
+      </c>
+      <c r="K12" s="214"/>
       <c r="L12" s="186"/>
-      <c r="M12" s="218">
-        <f>S31</f>
-        <v>0.21739130434782608</v>
-      </c>
-      <c r="N12" s="218"/>
-      <c r="Q12" s="203"/>
-      <c r="R12" s="194" t="s">
+      <c r="M12" s="219">
+        <v>0</v>
+      </c>
+      <c r="N12" s="219"/>
+      <c r="Q12" s="204"/>
+      <c r="R12" s="195" t="s">
         <v>327</v>
       </c>
       <c r="S12" s="188">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="T12" s="150"/>
-      <c r="U12" s="192"/>
-      <c r="V12" s="192"/>
+      <c r="U12" s="193"/>
+      <c r="V12" s="193"/>
       <c r="W12" s="187"/>
       <c r="X12" s="150"/>
       <c r="Y12" s="150"/>
@@ -8835,36 +8963,36 @@
       <c r="D13" s="149"/>
       <c r="E13" s="185"/>
       <c r="F13" s="186"/>
-      <c r="G13" s="213"/>
-      <c r="H13" s="213">
+      <c r="G13" s="214"/>
+      <c r="H13" s="214">
         <f>H11+H12</f>
-        <v>60010.869565217392</v>
+        <v>3600</v>
       </c>
       <c r="I13" s="186"/>
       <c r="J13" s="213"/>
-      <c r="K13" s="219">
-        <f>K10+H13</f>
-        <v>61810.869565217392</v>
+      <c r="K13" s="221">
+        <f>K10+J12</f>
+        <v>5460</v>
       </c>
       <c r="L13" s="186"/>
-      <c r="M13" s="212">
+      <c r="M13" s="213">
         <f>M11+M12</f>
-        <v>120.21739130434783</v>
-      </c>
-      <c r="N13" s="213">
+        <v>80</v>
+      </c>
+      <c r="N13" s="214">
         <f>N9+M13</f>
-        <v>130.21739130434781</v>
-      </c>
-      <c r="Q13" s="203"/>
-      <c r="R13" s="194" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="204"/>
+      <c r="R13" s="195" t="s">
         <v>328</v>
       </c>
       <c r="S13" s="188">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="T13" s="150"/>
-      <c r="U13" s="192"/>
-      <c r="V13" s="192"/>
+      <c r="U13" s="193"/>
+      <c r="V13" s="193"/>
       <c r="W13" s="187"/>
       <c r="X13" s="150"/>
       <c r="Y13" s="150"/>
@@ -8878,24 +9006,24 @@
       <c r="D14" s="149"/>
       <c r="E14" s="185"/>
       <c r="F14" s="186"/>
-      <c r="G14" s="213"/>
-      <c r="H14" s="212"/>
+      <c r="G14" s="214"/>
+      <c r="H14" s="213"/>
       <c r="I14" s="186"/>
-      <c r="J14" s="213"/>
-      <c r="K14" s="213"/>
+      <c r="J14" s="214"/>
+      <c r="K14" s="214"/>
       <c r="L14" s="186"/>
-      <c r="M14" s="213"/>
-      <c r="N14" s="213"/>
-      <c r="Q14" s="203"/>
-      <c r="R14" s="194" t="s">
+      <c r="M14" s="214"/>
+      <c r="N14" s="214"/>
+      <c r="Q14" s="204"/>
+      <c r="R14" s="195" t="s">
         <v>329</v>
       </c>
       <c r="S14" s="188">
-        <v>420</v>
+        <v>210</v>
       </c>
       <c r="T14" s="150"/>
-      <c r="U14" s="192"/>
-      <c r="V14" s="192"/>
+      <c r="U14" s="193"/>
+      <c r="V14" s="193"/>
       <c r="W14" s="187"/>
       <c r="X14" s="150"/>
       <c r="Y14" s="150"/>
@@ -8903,30 +9031,48 @@
       <c r="AA14" s="150"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A15" s="149"/>
+      <c r="A15" s="149" t="s">
+        <v>325</v>
+      </c>
       <c r="B15" s="186"/>
-      <c r="C15" s="149"/>
+      <c r="C15" s="149" t="s">
+        <v>324</v>
+      </c>
       <c r="D15" s="149"/>
-      <c r="E15" s="185"/>
-      <c r="F15" s="222"/>
-      <c r="G15" s="213"/>
-      <c r="H15" s="213"/>
+      <c r="E15" s="185">
+        <v>2</v>
+      </c>
+      <c r="F15" s="186"/>
+      <c r="G15" s="214">
+        <f>J12</f>
+        <v>3660</v>
+      </c>
+      <c r="H15" s="214">
+        <f>G15*E15</f>
+        <v>7320</v>
+      </c>
       <c r="I15" s="186"/>
-      <c r="J15" s="213"/>
-      <c r="K15" s="213"/>
+      <c r="J15" s="214">
+        <f>W8*S10</f>
+        <v>90</v>
+      </c>
+      <c r="K15" s="214"/>
       <c r="L15" s="186"/>
-      <c r="M15" s="213"/>
-      <c r="N15" s="213"/>
-      <c r="Q15" s="203"/>
-      <c r="R15" s="194" t="s">
+      <c r="M15" s="214">
+        <f>S10+S9*E15</f>
+        <v>210</v>
+      </c>
+      <c r="N15" s="214"/>
+      <c r="Q15" s="204"/>
+      <c r="R15" s="195" t="s">
         <v>330</v>
       </c>
       <c r="S15" s="188">
-        <v>480</v>
+        <v>240</v>
       </c>
       <c r="T15" s="150"/>
       <c r="U15" s="192"/>
-      <c r="V15" s="192"/>
+      <c r="V15" s="193"/>
       <c r="W15" s="187"/>
       <c r="X15" s="150"/>
       <c r="Y15" s="150"/>
@@ -8934,45 +9080,38 @@
       <c r="AA15" s="150"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A16" s="149" t="s">
-        <v>325</v>
-      </c>
+      <c r="A16" s="149"/>
       <c r="B16" s="186"/>
-      <c r="C16" s="149" t="s">
-        <v>324</v>
-      </c>
+      <c r="C16" s="149"/>
       <c r="D16" s="149"/>
-      <c r="E16" s="185">
-        <v>2</v>
-      </c>
+      <c r="E16" s="185"/>
       <c r="F16" s="186"/>
-      <c r="G16" s="213">
-        <f>W8*S10</f>
-        <v>45000</v>
-      </c>
+      <c r="G16" s="218"/>
       <c r="H16" s="213">
-        <f>G16*E16</f>
-        <v>90000</v>
+        <f>G16</f>
+        <v>0</v>
       </c>
       <c r="I16" s="186"/>
-      <c r="J16" s="213"/>
-      <c r="K16" s="213"/>
+      <c r="J16" s="214">
+        <f>J15+H17</f>
+        <v>7410</v>
+      </c>
+      <c r="K16" s="214"/>
       <c r="L16" s="186"/>
-      <c r="M16" s="213">
-        <f>M13</f>
-        <v>120.21739130434783</v>
-      </c>
-      <c r="N16" s="213"/>
-      <c r="Q16" s="203"/>
-      <c r="R16" s="194" t="s">
+      <c r="M16" s="219">
+        <v>0</v>
+      </c>
+      <c r="N16" s="219"/>
+      <c r="Q16" s="204"/>
+      <c r="R16" s="195" t="s">
         <v>331</v>
       </c>
       <c r="S16" s="188">
-        <v>540</v>
+        <v>270</v>
       </c>
       <c r="T16" s="150"/>
-      <c r="U16" s="192"/>
-      <c r="V16" s="192"/>
+      <c r="U16" s="193"/>
+      <c r="V16" s="193"/>
       <c r="W16" s="187"/>
       <c r="X16" s="150"/>
       <c r="Y16" s="150"/>
@@ -8982,41 +9121,40 @@
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="149"/>
       <c r="B17" s="186"/>
-      <c r="C17" s="149" t="s">
-        <v>337</v>
-      </c>
+      <c r="C17" s="149"/>
       <c r="D17" s="149"/>
-      <c r="E17" s="185">
-        <v>100</v>
-      </c>
+      <c r="E17" s="185"/>
       <c r="F17" s="186"/>
-      <c r="G17" s="217">
-        <f>W10*S31</f>
-        <v>10.869565217391305</v>
-      </c>
-      <c r="H17" s="212">
-        <f>E17/9.2</f>
-        <v>10.869565217391305</v>
+      <c r="G17" s="214"/>
+      <c r="H17" s="223">
+        <f>H15+H16</f>
+        <v>7320</v>
       </c>
       <c r="I17" s="186"/>
-      <c r="J17" s="213"/>
-      <c r="K17" s="213"/>
+      <c r="J17" s="214"/>
+      <c r="K17" s="221">
+        <f>K13+J16</f>
+        <v>12870</v>
+      </c>
       <c r="L17" s="186"/>
-      <c r="M17" s="218">
-        <f>S31</f>
-        <v>0.21739130434782608</v>
-      </c>
-      <c r="N17" s="218"/>
-      <c r="Q17" s="203"/>
-      <c r="R17" s="194" t="s">
+      <c r="M17" s="214">
+        <f>M15+M16</f>
+        <v>210</v>
+      </c>
+      <c r="N17" s="214">
+        <f>N13+M17</f>
+        <v>300</v>
+      </c>
+      <c r="Q17" s="204"/>
+      <c r="R17" s="195" t="s">
         <v>332</v>
       </c>
       <c r="S17" s="188">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="T17" s="150"/>
-      <c r="U17" s="192"/>
-      <c r="V17" s="192"/>
+      <c r="U17" s="193"/>
+      <c r="V17" s="193"/>
       <c r="W17" s="187"/>
       <c r="X17" s="150"/>
       <c r="Y17" s="150"/>
@@ -9030,34 +9168,25 @@
       <c r="D18" s="149"/>
       <c r="E18" s="185"/>
       <c r="F18" s="186"/>
-      <c r="G18" s="213"/>
-      <c r="H18" s="221">
-        <f>H16+H17</f>
-        <v>90010.869565217392</v>
-      </c>
+      <c r="G18" s="214"/>
+      <c r="H18" s="214"/>
       <c r="I18" s="186"/>
-      <c r="J18" s="213"/>
-      <c r="K18" s="219">
-        <f>K13+H18</f>
-        <v>151821.73913043478</v>
-      </c>
+      <c r="J18" s="214"/>
+      <c r="K18" s="214"/>
       <c r="L18" s="186"/>
-      <c r="M18" s="213">
-        <f>M16+M17</f>
-        <v>120.43478260869566</v>
-      </c>
-      <c r="N18" s="213">
-        <f>N13+M18</f>
-        <v>250.65217391304347</v>
-      </c>
-      <c r="Q18" s="203"/>
-      <c r="R18" s="194"/>
-      <c r="S18" s="190" t="s">
-        <v>360</v>
-      </c>
-      <c r="T18" s="150"/>
-      <c r="U18" s="192"/>
-      <c r="V18" s="192"/>
+      <c r="M18" s="214"/>
+      <c r="N18" s="214"/>
+      <c r="Q18" s="204"/>
+      <c r="R18" s="195"/>
+      <c r="S18" s="191">
+        <f>(S9+S10+S11+S12+S13+S14+S15+S16+S17)/60</f>
+        <v>27</v>
+      </c>
+      <c r="T18" s="119" t="s">
+        <v>394</v>
+      </c>
+      <c r="U18" s="193"/>
+      <c r="V18" s="193"/>
       <c r="W18" s="187"/>
       <c r="X18" s="150"/>
       <c r="Y18" s="150"/>
@@ -9065,22 +9194,40 @@
       <c r="AA18" s="150"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19" s="149"/>
+      <c r="A19" s="148" t="s">
+        <v>326</v>
+      </c>
       <c r="B19" s="186"/>
-      <c r="C19" s="149"/>
+      <c r="C19" s="148" t="s">
+        <v>325</v>
+      </c>
       <c r="D19" s="149"/>
-      <c r="E19" s="185"/>
+      <c r="E19" s="185">
+        <v>2</v>
+      </c>
       <c r="F19" s="186"/>
-      <c r="G19" s="213"/>
-      <c r="H19" s="213"/>
+      <c r="G19" s="214">
+        <f>J16</f>
+        <v>7410</v>
+      </c>
+      <c r="H19" s="214">
+        <f>G19*E19</f>
+        <v>14820</v>
+      </c>
       <c r="I19" s="186"/>
-      <c r="J19" s="213"/>
-      <c r="K19" s="213"/>
+      <c r="J19" s="214">
+        <f>W8*S11</f>
+        <v>120</v>
+      </c>
+      <c r="K19" s="214"/>
       <c r="L19" s="186"/>
-      <c r="M19" s="213"/>
-      <c r="N19" s="213"/>
-      <c r="Q19" s="203"/>
-      <c r="R19" s="194"/>
+      <c r="M19" s="214">
+        <f>S11+S10*E19</f>
+        <v>300</v>
+      </c>
+      <c r="N19" s="214"/>
+      <c r="Q19" s="204"/>
+      <c r="R19" s="195"/>
       <c r="S19" s="189"/>
       <c r="T19" s="150"/>
       <c r="U19" s="150"/>
@@ -9092,35 +9239,31 @@
       <c r="AA19" s="150"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" s="148" t="s">
-        <v>326</v>
-      </c>
+      <c r="A20" s="149"/>
       <c r="B20" s="186"/>
-      <c r="C20" s="148" t="s">
-        <v>325</v>
-      </c>
+      <c r="C20" s="148"/>
       <c r="D20" s="149"/>
-      <c r="E20" s="185">
-        <v>2</v>
-      </c>
+      <c r="E20" s="185"/>
       <c r="F20" s="186"/>
-      <c r="G20" s="213">
-        <f>W8*S11</f>
-        <v>60000</v>
-      </c>
-      <c r="H20" s="213">
-        <f>G20*E20</f>
-        <v>120000</v>
+      <c r="G20" s="214"/>
+      <c r="H20" s="214">
+        <f>G20</f>
+        <v>0</v>
       </c>
       <c r="I20" s="186"/>
-      <c r="J20" s="213"/>
-      <c r="K20" s="213"/>
+      <c r="J20" s="214">
+        <f>J19+H21</f>
+        <v>14940</v>
+      </c>
+      <c r="K20" s="214"/>
       <c r="L20" s="186"/>
-      <c r="M20" s="213"/>
-      <c r="N20" s="213"/>
-      <c r="Q20" s="203"/>
-      <c r="R20" s="193" t="s">
-        <v>349</v>
+      <c r="M20" s="219">
+        <v>0</v>
+      </c>
+      <c r="N20" s="219"/>
+      <c r="Q20" s="204"/>
+      <c r="R20" s="194" t="s">
+        <v>348</v>
       </c>
       <c r="S20" s="189"/>
       <c r="T20" s="150"/>
@@ -9135,28 +9278,33 @@
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="149"/>
       <c r="B21" s="186"/>
-      <c r="C21" s="148" t="s">
-        <v>337</v>
-      </c>
+      <c r="C21" s="149"/>
       <c r="D21" s="149"/>
-      <c r="E21" s="185">
-        <v>100</v>
-      </c>
+      <c r="E21" s="185"/>
       <c r="F21" s="186"/>
-      <c r="G21" s="213">
-        <f>W10*S31</f>
-        <v>10.869565217391305</v>
-      </c>
-      <c r="H21" s="213"/>
+      <c r="G21" s="214"/>
+      <c r="H21" s="223">
+        <f>H19+H20</f>
+        <v>14820</v>
+      </c>
       <c r="I21" s="186"/>
-      <c r="J21" s="213"/>
-      <c r="K21" s="213"/>
+      <c r="J21" s="214"/>
+      <c r="K21" s="221">
+        <f>K17+J20</f>
+        <v>27810</v>
+      </c>
       <c r="L21" s="186"/>
-      <c r="M21" s="213"/>
-      <c r="N21" s="213"/>
-      <c r="Q21" s="203"/>
-      <c r="R21" s="193" t="s">
-        <v>350</v>
+      <c r="M21" s="213">
+        <f>M19+M20</f>
+        <v>300</v>
+      </c>
+      <c r="N21" s="213">
+        <f>M21+N17</f>
+        <v>600</v>
+      </c>
+      <c r="Q21" s="204"/>
+      <c r="R21" s="194" t="s">
+        <v>349</v>
       </c>
       <c r="S21" s="189"/>
       <c r="T21" s="150"/>
@@ -9175,17 +9323,17 @@
       <c r="D22" s="149"/>
       <c r="E22" s="185"/>
       <c r="F22" s="186"/>
-      <c r="G22" s="213"/>
-      <c r="H22" s="213"/>
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
       <c r="I22" s="186"/>
-      <c r="J22" s="213"/>
-      <c r="K22" s="213"/>
+      <c r="J22" s="214"/>
+      <c r="K22" s="214"/>
       <c r="L22" s="186"/>
-      <c r="M22" s="213"/>
-      <c r="N22" s="213"/>
-      <c r="Q22" s="203"/>
-      <c r="R22" s="193" t="s">
-        <v>351</v>
+      <c r="M22" s="214"/>
+      <c r="N22" s="214"/>
+      <c r="Q22" s="204"/>
+      <c r="R22" s="194" t="s">
+        <v>350</v>
       </c>
       <c r="S22" s="189"/>
       <c r="T22" s="150"/>
@@ -9198,23 +9346,41 @@
       <c r="AA22" s="150"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" s="149"/>
+      <c r="A23" s="148" t="s">
+        <v>327</v>
+      </c>
       <c r="B23" s="186"/>
-      <c r="C23" s="149"/>
+      <c r="C23" s="148" t="s">
+        <v>326</v>
+      </c>
       <c r="D23" s="149"/>
-      <c r="E23" s="185"/>
+      <c r="E23" s="185">
+        <v>2</v>
+      </c>
       <c r="F23" s="186"/>
-      <c r="G23" s="213"/>
-      <c r="H23" s="213"/>
+      <c r="G23" s="214">
+        <f>J20</f>
+        <v>14940</v>
+      </c>
+      <c r="H23" s="214">
+        <f>G23*E23</f>
+        <v>29880</v>
+      </c>
       <c r="I23" s="186"/>
-      <c r="J23" s="213"/>
-      <c r="K23" s="213"/>
-      <c r="L23" s="186"/>
-      <c r="M23" s="213"/>
-      <c r="N23" s="213"/>
-      <c r="Q23" s="203"/>
-      <c r="R23" s="193" t="s">
-        <v>352</v>
+      <c r="J23" s="214">
+        <f>W8*S12</f>
+        <v>150</v>
+      </c>
+      <c r="K23" s="185"/>
+      <c r="L23" s="224"/>
+      <c r="M23" s="214">
+        <f>S12+S11*E23</f>
+        <v>390</v>
+      </c>
+      <c r="N23" s="185"/>
+      <c r="Q23" s="204"/>
+      <c r="R23" s="194" t="s">
+        <v>351</v>
       </c>
       <c r="S23" s="189"/>
       <c r="T23" s="150"/>
@@ -9229,21 +9395,29 @@
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="149"/>
       <c r="B24" s="186"/>
-      <c r="C24" s="149"/>
+      <c r="C24" s="148"/>
       <c r="D24" s="149"/>
       <c r="E24" s="185"/>
       <c r="F24" s="186"/>
-      <c r="G24" s="213"/>
-      <c r="H24" s="213"/>
+      <c r="G24" s="214"/>
+      <c r="H24" s="219">
+        <f>G24</f>
+        <v>0</v>
+      </c>
       <c r="I24" s="186"/>
-      <c r="J24" s="213"/>
-      <c r="K24" s="213"/>
+      <c r="J24" s="214">
+        <f>J23+H25</f>
+        <v>30030</v>
+      </c>
+      <c r="K24" s="214"/>
       <c r="L24" s="186"/>
-      <c r="M24" s="213"/>
-      <c r="N24" s="213"/>
-      <c r="Q24" s="203"/>
-      <c r="R24" s="193" t="s">
-        <v>353</v>
+      <c r="M24" s="219">
+        <v>0</v>
+      </c>
+      <c r="N24" s="219"/>
+      <c r="Q24" s="204"/>
+      <c r="R24" s="194" t="s">
+        <v>352</v>
       </c>
       <c r="S24" s="189"/>
       <c r="T24" s="150"/>
@@ -9262,17 +9436,29 @@
       <c r="D25" s="149"/>
       <c r="E25" s="185"/>
       <c r="F25" s="186"/>
-      <c r="G25" s="213"/>
-      <c r="H25" s="213"/>
+      <c r="G25" s="214"/>
+      <c r="H25" s="214">
+        <f>H24+H23</f>
+        <v>29880</v>
+      </c>
       <c r="I25" s="186"/>
-      <c r="J25" s="213"/>
-      <c r="K25" s="213"/>
+      <c r="J25" s="214"/>
+      <c r="K25" s="221">
+        <f>K21+J24</f>
+        <v>57840</v>
+      </c>
       <c r="L25" s="186"/>
-      <c r="M25" s="213"/>
-      <c r="N25" s="213"/>
-      <c r="Q25" s="203"/>
-      <c r="R25" s="193" t="s">
-        <v>354</v>
+      <c r="M25" s="214">
+        <f>M24+M23</f>
+        <v>390</v>
+      </c>
+      <c r="N25" s="214">
+        <f>N21+M25</f>
+        <v>990</v>
+      </c>
+      <c r="Q25" s="204"/>
+      <c r="R25" s="194" t="s">
+        <v>353</v>
       </c>
       <c r="S25" s="189"/>
       <c r="T25" s="150"/>
@@ -9291,17 +9477,17 @@
       <c r="D26" s="149"/>
       <c r="E26" s="185"/>
       <c r="F26" s="186"/>
-      <c r="G26" s="213"/>
-      <c r="H26" s="213"/>
+      <c r="G26" s="214"/>
+      <c r="H26" s="214"/>
       <c r="I26" s="186"/>
-      <c r="J26" s="213"/>
-      <c r="K26" s="213"/>
+      <c r="J26" s="214"/>
+      <c r="K26" s="214"/>
       <c r="L26" s="186"/>
-      <c r="M26" s="213"/>
-      <c r="N26" s="213"/>
-      <c r="Q26" s="203"/>
-      <c r="R26" s="193" t="s">
-        <v>355</v>
+      <c r="M26" s="214"/>
+      <c r="N26" s="214"/>
+      <c r="Q26" s="204"/>
+      <c r="R26" s="194" t="s">
+        <v>354</v>
       </c>
       <c r="S26" s="189"/>
       <c r="T26" s="150"/>
@@ -9314,23 +9500,41 @@
       <c r="AA26" s="150"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A27" s="149"/>
+      <c r="A27" s="148" t="s">
+        <v>328</v>
+      </c>
       <c r="B27" s="186"/>
-      <c r="C27" s="149"/>
+      <c r="C27" s="148" t="s">
+        <v>327</v>
+      </c>
       <c r="D27" s="149"/>
-      <c r="E27" s="185"/>
+      <c r="E27" s="185">
+        <v>2</v>
+      </c>
       <c r="F27" s="186"/>
-      <c r="G27" s="213"/>
-      <c r="H27" s="213"/>
+      <c r="G27" s="214">
+        <f>H25</f>
+        <v>29880</v>
+      </c>
+      <c r="H27" s="214">
+        <f>G27*E27</f>
+        <v>59760</v>
+      </c>
       <c r="I27" s="186"/>
-      <c r="J27" s="213"/>
-      <c r="K27" s="213"/>
+      <c r="J27" s="214">
+        <f>W8*S13</f>
+        <v>180</v>
+      </c>
+      <c r="K27" s="214"/>
       <c r="L27" s="186"/>
-      <c r="M27" s="213"/>
-      <c r="N27" s="213"/>
-      <c r="Q27" s="203"/>
-      <c r="R27" s="193" t="s">
-        <v>356</v>
+      <c r="M27" s="214">
+        <f>S13+S12*E27</f>
+        <v>480</v>
+      </c>
+      <c r="N27" s="214"/>
+      <c r="Q27" s="204"/>
+      <c r="R27" s="194" t="s">
+        <v>355</v>
       </c>
       <c r="S27" s="189"/>
       <c r="T27" s="150"/>
@@ -9345,21 +9549,29 @@
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="149"/>
       <c r="B28" s="186"/>
-      <c r="C28" s="149"/>
+      <c r="C28" s="148"/>
       <c r="D28" s="149"/>
       <c r="E28" s="185"/>
       <c r="F28" s="186"/>
-      <c r="G28" s="213"/>
-      <c r="H28" s="213"/>
+      <c r="G28" s="214"/>
+      <c r="H28" s="219">
+        <f>G28</f>
+        <v>0</v>
+      </c>
       <c r="I28" s="186"/>
-      <c r="J28" s="213"/>
-      <c r="K28" s="213"/>
+      <c r="J28" s="214">
+        <f>J27+H29</f>
+        <v>59940</v>
+      </c>
+      <c r="K28" s="214"/>
       <c r="L28" s="186"/>
-      <c r="M28" s="213"/>
-      <c r="N28" s="213"/>
-      <c r="Q28" s="203"/>
-      <c r="R28" s="193" t="s">
-        <v>357</v>
+      <c r="M28" s="219">
+        <v>0</v>
+      </c>
+      <c r="N28" s="219"/>
+      <c r="Q28" s="204"/>
+      <c r="R28" s="194" t="s">
+        <v>356</v>
       </c>
       <c r="S28" s="189"/>
       <c r="T28" s="150"/>
@@ -9378,17 +9590,29 @@
       <c r="D29" s="149"/>
       <c r="E29" s="185"/>
       <c r="F29" s="186"/>
-      <c r="G29" s="213"/>
-      <c r="H29" s="213"/>
+      <c r="G29" s="214"/>
+      <c r="H29" s="214">
+        <f>H28+H27</f>
+        <v>59760</v>
+      </c>
       <c r="I29" s="186"/>
-      <c r="J29" s="213"/>
-      <c r="K29" s="213"/>
+      <c r="J29" s="214"/>
+      <c r="K29" s="221">
+        <f>K25+J28</f>
+        <v>117780</v>
+      </c>
       <c r="L29" s="186"/>
-      <c r="M29" s="213"/>
-      <c r="N29" s="213"/>
-      <c r="Q29" s="203"/>
-      <c r="R29" s="193" t="s">
-        <v>358</v>
+      <c r="M29" s="214">
+        <f>M27+M28</f>
+        <v>480</v>
+      </c>
+      <c r="N29" s="214">
+        <f>N25+M29</f>
+        <v>1470</v>
+      </c>
+      <c r="Q29" s="204"/>
+      <c r="R29" s="194" t="s">
+        <v>357</v>
       </c>
       <c r="S29" s="189"/>
       <c r="T29" s="150"/>
@@ -9407,16 +9631,16 @@
       <c r="D30" s="149"/>
       <c r="E30" s="185"/>
       <c r="F30" s="186"/>
-      <c r="G30" s="213"/>
-      <c r="H30" s="213"/>
+      <c r="G30" s="214"/>
+      <c r="H30" s="214"/>
       <c r="I30" s="186"/>
-      <c r="J30" s="213"/>
-      <c r="K30" s="213"/>
+      <c r="J30" s="214"/>
+      <c r="K30" s="214"/>
       <c r="L30" s="186"/>
-      <c r="M30" s="213"/>
-      <c r="N30" s="213"/>
-      <c r="Q30" s="203"/>
-      <c r="R30" s="194"/>
+      <c r="M30" s="214"/>
+      <c r="N30" s="214"/>
+      <c r="Q30" s="204"/>
+      <c r="R30" s="195"/>
       <c r="S30" s="189"/>
       <c r="T30" s="150"/>
       <c r="U30" s="150"/>
@@ -9428,28 +9652,41 @@
       <c r="AA30" s="150"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A31" s="149"/>
+      <c r="A31" s="148" t="s">
+        <v>329</v>
+      </c>
       <c r="B31" s="186"/>
-      <c r="C31" s="149"/>
+      <c r="C31" s="148" t="s">
+        <v>328</v>
+      </c>
       <c r="D31" s="149"/>
-      <c r="E31" s="185"/>
+      <c r="E31" s="185">
+        <v>2</v>
+      </c>
       <c r="F31" s="186"/>
-      <c r="G31" s="213"/>
-      <c r="H31" s="213"/>
+      <c r="G31" s="214">
+        <f>J28</f>
+        <v>59940</v>
+      </c>
+      <c r="H31" s="214">
+        <f>G31*E31</f>
+        <v>119880</v>
+      </c>
       <c r="I31" s="186"/>
-      <c r="J31" s="213"/>
-      <c r="K31" s="213"/>
+      <c r="J31" s="214">
+        <f>W8*S14</f>
+        <v>210</v>
+      </c>
+      <c r="K31" s="214"/>
       <c r="L31" s="186"/>
-      <c r="M31" s="213"/>
-      <c r="N31" s="213"/>
-      <c r="Q31" s="203"/>
-      <c r="R31" s="193" t="s">
-        <v>337</v>
-      </c>
-      <c r="S31" s="188">
-        <f>100/460</f>
-        <v>0.21739130434782608</v>
-      </c>
+      <c r="M31" s="214">
+        <f>S14+S13*E31</f>
+        <v>570</v>
+      </c>
+      <c r="N31" s="214"/>
+      <c r="Q31" s="204"/>
+      <c r="R31" s="194"/>
+      <c r="S31" s="188"/>
       <c r="T31" s="150"/>
       <c r="U31" s="150"/>
       <c r="V31" s="150"/>
@@ -9466,14 +9703,21 @@
       <c r="D32" s="149"/>
       <c r="E32" s="185"/>
       <c r="F32" s="186"/>
-      <c r="G32" s="213"/>
-      <c r="H32" s="213"/>
+      <c r="G32" s="214"/>
+      <c r="H32" s="219">
+        <v>0</v>
+      </c>
       <c r="I32" s="186"/>
-      <c r="J32" s="213"/>
-      <c r="K32" s="213"/>
+      <c r="J32" s="214">
+        <f>J31+H33</f>
+        <v>120090</v>
+      </c>
+      <c r="K32" s="214"/>
       <c r="L32" s="186"/>
-      <c r="M32" s="213"/>
-      <c r="N32" s="213"/>
+      <c r="M32" s="219">
+        <v>0</v>
+      </c>
+      <c r="N32" s="219"/>
       <c r="Q32" s="150"/>
       <c r="R32" s="150"/>
       <c r="S32" s="150"/>
@@ -9493,14 +9737,26 @@
       <c r="D33" s="149"/>
       <c r="E33" s="185"/>
       <c r="F33" s="186"/>
-      <c r="G33" s="213"/>
-      <c r="H33" s="213"/>
+      <c r="G33" s="214"/>
+      <c r="H33" s="214">
+        <f>H32+H31</f>
+        <v>119880</v>
+      </c>
       <c r="I33" s="186"/>
-      <c r="J33" s="213"/>
-      <c r="K33" s="213"/>
+      <c r="J33" s="214"/>
+      <c r="K33" s="221">
+        <f>K29+J32</f>
+        <v>237870</v>
+      </c>
       <c r="L33" s="186"/>
-      <c r="M33" s="213"/>
-      <c r="N33" s="213"/>
+      <c r="M33" s="214">
+        <f>M31+M32</f>
+        <v>570</v>
+      </c>
+      <c r="N33" s="214">
+        <f>N29+M33</f>
+        <v>2040</v>
+      </c>
       <c r="Q33" s="150"/>
       <c r="R33" s="150"/>
       <c r="S33" s="150"/>
@@ -9521,14 +9777,14 @@
       <c r="D34" s="149"/>
       <c r="E34" s="185"/>
       <c r="F34" s="186"/>
-      <c r="G34" s="213"/>
-      <c r="H34" s="213"/>
+      <c r="G34" s="214"/>
+      <c r="H34" s="214"/>
       <c r="I34" s="186"/>
-      <c r="J34" s="213"/>
-      <c r="K34" s="213"/>
+      <c r="J34" s="214"/>
+      <c r="K34" s="214"/>
       <c r="L34" s="186"/>
-      <c r="M34" s="213"/>
-      <c r="N34" s="213"/>
+      <c r="M34" s="214"/>
+      <c r="N34" s="214"/>
       <c r="Q34" s="150"/>
       <c r="R34" s="150"/>
       <c r="S34" s="150"/>
@@ -9543,20 +9799,38 @@
       <c r="AB34" s="150"/>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A35" s="149"/>
+      <c r="A35" s="148" t="s">
+        <v>330</v>
+      </c>
       <c r="B35" s="186"/>
-      <c r="C35" s="149"/>
+      <c r="C35" s="148" t="s">
+        <v>329</v>
+      </c>
       <c r="D35" s="149"/>
-      <c r="E35" s="185"/>
+      <c r="E35" s="185">
+        <v>2</v>
+      </c>
       <c r="F35" s="186"/>
-      <c r="G35" s="213"/>
-      <c r="H35" s="213"/>
+      <c r="G35" s="214">
+        <f>J32</f>
+        <v>120090</v>
+      </c>
+      <c r="H35" s="213">
+        <f>G35*E35</f>
+        <v>240180</v>
+      </c>
       <c r="I35" s="186"/>
-      <c r="J35" s="213"/>
-      <c r="K35" s="213"/>
+      <c r="J35" s="214">
+        <f>W8*S15</f>
+        <v>240</v>
+      </c>
+      <c r="K35" s="214"/>
       <c r="L35" s="186"/>
-      <c r="M35" s="213"/>
-      <c r="N35" s="213"/>
+      <c r="M35" s="214">
+        <f>S15+S14*E35</f>
+        <v>660</v>
+      </c>
+      <c r="N35" s="214"/>
       <c r="Q35" s="150"/>
       <c r="R35" s="150"/>
       <c r="S35" s="150"/>
@@ -9577,14 +9851,21 @@
       <c r="D36" s="149"/>
       <c r="E36" s="185"/>
       <c r="F36" s="186"/>
-      <c r="G36" s="213"/>
-      <c r="H36" s="213"/>
+      <c r="G36" s="214"/>
+      <c r="H36" s="219">
+        <v>0</v>
+      </c>
       <c r="I36" s="186"/>
-      <c r="J36" s="213"/>
+      <c r="J36" s="214">
+        <f>J35+H37</f>
+        <v>240420</v>
+      </c>
       <c r="K36" s="213"/>
       <c r="L36" s="186"/>
-      <c r="M36" s="213"/>
-      <c r="N36" s="213"/>
+      <c r="M36" s="219">
+        <v>0</v>
+      </c>
+      <c r="N36" s="219"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="149"/>
@@ -9593,14 +9874,26 @@
       <c r="D37" s="149"/>
       <c r="E37" s="185"/>
       <c r="F37" s="186"/>
-      <c r="G37" s="213"/>
-      <c r="H37" s="213"/>
+      <c r="G37" s="214"/>
+      <c r="H37" s="214">
+        <f>H36+H35</f>
+        <v>240180</v>
+      </c>
       <c r="I37" s="186"/>
-      <c r="J37" s="213"/>
-      <c r="K37" s="213"/>
+      <c r="J37" s="214"/>
+      <c r="K37" s="221">
+        <f>K33+J36</f>
+        <v>478290</v>
+      </c>
       <c r="L37" s="186"/>
-      <c r="M37" s="213"/>
-      <c r="N37" s="213"/>
+      <c r="M37" s="214">
+        <f>M35+M36</f>
+        <v>660</v>
+      </c>
+      <c r="N37" s="214">
+        <f>N33+M37</f>
+        <v>2700</v>
+      </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="149"/>
@@ -9609,30 +9902,48 @@
       <c r="D38" s="149"/>
       <c r="E38" s="185"/>
       <c r="F38" s="186"/>
-      <c r="G38" s="213"/>
-      <c r="H38" s="213"/>
+      <c r="G38" s="214"/>
+      <c r="H38" s="214"/>
       <c r="I38" s="186"/>
-      <c r="J38" s="213"/>
-      <c r="K38" s="213"/>
+      <c r="J38" s="214"/>
+      <c r="K38" s="214"/>
       <c r="L38" s="186"/>
-      <c r="M38" s="213"/>
-      <c r="N38" s="213"/>
+      <c r="M38" s="214"/>
+      <c r="N38" s="214"/>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A39" s="149"/>
+      <c r="A39" s="148" t="s">
+        <v>331</v>
+      </c>
       <c r="B39" s="186"/>
-      <c r="C39" s="149"/>
+      <c r="C39" s="148" t="s">
+        <v>330</v>
+      </c>
       <c r="D39" s="149"/>
-      <c r="E39" s="185"/>
+      <c r="E39" s="185">
+        <v>2</v>
+      </c>
       <c r="F39" s="186"/>
-      <c r="G39" s="213"/>
-      <c r="H39" s="213"/>
+      <c r="G39" s="214">
+        <f>J36</f>
+        <v>240420</v>
+      </c>
+      <c r="H39" s="214">
+        <f>G39*E39</f>
+        <v>480840</v>
+      </c>
       <c r="I39" s="186"/>
-      <c r="J39" s="213"/>
-      <c r="K39" s="213"/>
+      <c r="J39" s="214">
+        <f>W8*S16</f>
+        <v>270</v>
+      </c>
+      <c r="K39" s="214"/>
       <c r="L39" s="186"/>
-      <c r="M39" s="213"/>
-      <c r="N39" s="213"/>
+      <c r="M39" s="214">
+        <f>S16+S15*E39</f>
+        <v>750</v>
+      </c>
+      <c r="N39" s="214"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="149"/>
@@ -9641,14 +9952,21 @@
       <c r="D40" s="149"/>
       <c r="E40" s="185"/>
       <c r="F40" s="186"/>
-      <c r="G40" s="213"/>
-      <c r="H40" s="213"/>
+      <c r="G40" s="214"/>
+      <c r="H40" s="219">
+        <v>0</v>
+      </c>
       <c r="I40" s="186"/>
-      <c r="J40" s="213"/>
-      <c r="K40" s="213"/>
+      <c r="J40" s="214">
+        <f>J39+H41</f>
+        <v>481110</v>
+      </c>
+      <c r="K40" s="214"/>
       <c r="L40" s="186"/>
-      <c r="M40" s="213"/>
-      <c r="N40" s="213"/>
+      <c r="M40" s="219">
+        <v>0</v>
+      </c>
+      <c r="N40" s="219"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="149"/>
@@ -9657,14 +9975,26 @@
       <c r="D41" s="149"/>
       <c r="E41" s="185"/>
       <c r="F41" s="186"/>
-      <c r="G41" s="213"/>
-      <c r="H41" s="213"/>
+      <c r="G41" s="214"/>
+      <c r="H41" s="214">
+        <f>H39+H40</f>
+        <v>480840</v>
+      </c>
       <c r="I41" s="186"/>
-      <c r="J41" s="213"/>
-      <c r="K41" s="213"/>
+      <c r="J41" s="214"/>
+      <c r="K41" s="221">
+        <f>K37+J40</f>
+        <v>959400</v>
+      </c>
       <c r="L41" s="186"/>
-      <c r="M41" s="213"/>
-      <c r="N41" s="213"/>
+      <c r="M41" s="214">
+        <f>M40+M39</f>
+        <v>750</v>
+      </c>
+      <c r="N41" s="214">
+        <f>N37+M41</f>
+        <v>3450</v>
+      </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="149"/>
@@ -9673,30 +10003,45 @@
       <c r="D42" s="149"/>
       <c r="E42" s="185"/>
       <c r="F42" s="186"/>
-      <c r="G42" s="213"/>
-      <c r="H42" s="213"/>
+      <c r="G42" s="214"/>
+      <c r="H42" s="214"/>
       <c r="I42" s="186"/>
-      <c r="J42" s="213"/>
-      <c r="K42" s="213"/>
+      <c r="J42" s="214"/>
+      <c r="K42" s="214"/>
       <c r="L42" s="186"/>
-      <c r="M42" s="213"/>
-      <c r="N42" s="213"/>
+      <c r="M42" s="214"/>
+      <c r="N42" s="214"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A43" s="149"/>
+      <c r="A43" s="148" t="s">
+        <v>332</v>
+      </c>
       <c r="B43" s="186"/>
-      <c r="C43" s="149"/>
+      <c r="C43" s="148" t="s">
+        <v>331</v>
+      </c>
       <c r="D43" s="149"/>
-      <c r="E43" s="185"/>
+      <c r="E43" s="185">
+        <v>2</v>
+      </c>
       <c r="F43" s="186"/>
-      <c r="G43" s="213"/>
-      <c r="H43" s="213"/>
+      <c r="G43" s="214">
+        <f>J40</f>
+        <v>481110</v>
+      </c>
+      <c r="H43" s="214">
+        <f>G43*E43</f>
+        <v>962220</v>
+      </c>
       <c r="I43" s="186"/>
-      <c r="J43" s="213"/>
-      <c r="K43" s="213"/>
+      <c r="J43" s="214">
+        <f>W8*S17</f>
+        <v>300</v>
+      </c>
+      <c r="K43" s="214"/>
       <c r="L43" s="186"/>
-      <c r="M43" s="213"/>
-      <c r="N43" s="213"/>
+      <c r="M43" s="214"/>
+      <c r="N43" s="214"/>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="149"/>
@@ -9705,14 +10050,21 @@
       <c r="D44" s="149"/>
       <c r="E44" s="185"/>
       <c r="F44" s="186"/>
-      <c r="G44" s="213"/>
-      <c r="H44" s="213"/>
+      <c r="G44" s="214"/>
+      <c r="H44" s="219">
+        <v>0</v>
+      </c>
       <c r="I44" s="186"/>
-      <c r="J44" s="213"/>
-      <c r="K44" s="213"/>
+      <c r="J44" s="214">
+        <f>J43+H45</f>
+        <v>962520</v>
+      </c>
+      <c r="K44" s="214"/>
       <c r="L44" s="186"/>
-      <c r="M44" s="213"/>
-      <c r="N44" s="213"/>
+      <c r="M44" s="219">
+        <v>0</v>
+      </c>
+      <c r="N44" s="219"/>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="149"/>
@@ -9721,14 +10073,26 @@
       <c r="D45" s="149"/>
       <c r="E45" s="185"/>
       <c r="F45" s="186"/>
-      <c r="G45" s="213"/>
-      <c r="H45" s="213"/>
+      <c r="G45" s="214"/>
+      <c r="H45" s="214">
+        <f>H44+H43</f>
+        <v>962220</v>
+      </c>
       <c r="I45" s="186"/>
-      <c r="J45" s="213"/>
-      <c r="K45" s="213"/>
+      <c r="J45" s="214"/>
+      <c r="K45" s="221">
+        <f>J44+K41</f>
+        <v>1921920</v>
+      </c>
       <c r="L45" s="186"/>
-      <c r="M45" s="213"/>
-      <c r="N45" s="213"/>
+      <c r="M45" s="214">
+        <f>M44+M43</f>
+        <v>0</v>
+      </c>
+      <c r="N45" s="214">
+        <f>M45+N41</f>
+        <v>3450</v>
+      </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="149"/>
@@ -9737,14 +10101,14 @@
       <c r="D46" s="149"/>
       <c r="E46" s="185"/>
       <c r="F46" s="186"/>
-      <c r="G46" s="213"/>
-      <c r="H46" s="213"/>
+      <c r="G46" s="214"/>
+      <c r="H46" s="214"/>
       <c r="I46" s="186"/>
-      <c r="J46" s="213"/>
-      <c r="K46" s="213"/>
+      <c r="J46" s="214"/>
+      <c r="K46" s="214"/>
       <c r="L46" s="186"/>
-      <c r="M46" s="213"/>
-      <c r="N46" s="213"/>
+      <c r="M46" s="214"/>
+      <c r="N46" s="214"/>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" s="149"/>
@@ -9753,14 +10117,14 @@
       <c r="D47" s="149"/>
       <c r="E47" s="185"/>
       <c r="F47" s="186"/>
-      <c r="G47" s="213"/>
-      <c r="H47" s="213"/>
+      <c r="G47" s="214"/>
+      <c r="H47" s="214"/>
       <c r="I47" s="186"/>
-      <c r="J47" s="213"/>
-      <c r="K47" s="213"/>
+      <c r="J47" s="214"/>
+      <c r="K47" s="214"/>
       <c r="L47" s="186"/>
-      <c r="M47" s="213"/>
-      <c r="N47" s="213"/>
+      <c r="M47" s="214"/>
+      <c r="N47" s="214"/>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" s="149"/>
@@ -9769,270 +10133,293 @@
       <c r="D48" s="149"/>
       <c r="E48" s="185"/>
       <c r="F48" s="186"/>
-      <c r="G48" s="213"/>
-      <c r="H48" s="213"/>
+      <c r="G48" s="214"/>
+      <c r="H48" s="214"/>
       <c r="I48" s="186"/>
-      <c r="J48" s="213"/>
-      <c r="K48" s="213"/>
+      <c r="J48" s="214"/>
+      <c r="K48" s="214"/>
       <c r="L48" s="186"/>
-      <c r="M48" s="213"/>
-      <c r="N48" s="213"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M48" s="214"/>
+      <c r="N48" s="214"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="149"/>
       <c r="B49" s="186"/>
       <c r="C49" s="149"/>
       <c r="D49" s="149"/>
       <c r="E49" s="185"/>
       <c r="F49" s="186"/>
-      <c r="G49" s="213"/>
-      <c r="H49" s="213"/>
+      <c r="G49" s="214"/>
+      <c r="H49" s="214"/>
       <c r="I49" s="186"/>
-      <c r="J49" s="213"/>
-      <c r="K49" s="213"/>
+      <c r="J49" s="214"/>
+      <c r="K49" s="218" t="s">
+        <v>392</v>
+      </c>
       <c r="L49" s="186"/>
-      <c r="M49" s="213"/>
-      <c r="N49" s="213"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M49" s="214"/>
+      <c r="N49" s="218" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="149"/>
       <c r="B50" s="186"/>
       <c r="C50" s="149"/>
       <c r="D50" s="149"/>
       <c r="E50" s="185"/>
       <c r="F50" s="186"/>
-      <c r="G50" s="213"/>
-      <c r="H50" s="213"/>
+      <c r="G50" s="214"/>
+      <c r="H50" s="214"/>
       <c r="I50" s="186"/>
-      <c r="J50" s="213"/>
-      <c r="K50" s="213"/>
-      <c r="L50" s="186"/>
-      <c r="M50" s="213"/>
-      <c r="N50" s="213"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J50" s="214"/>
+      <c r="K50" s="214">
+        <f>K45</f>
+        <v>1921920</v>
+      </c>
+      <c r="L50" s="190" t="s">
+        <v>393</v>
+      </c>
+      <c r="M50" s="214"/>
+      <c r="N50" s="214">
+        <f>N45</f>
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="149"/>
       <c r="B51" s="186"/>
       <c r="C51" s="149"/>
       <c r="D51" s="149"/>
       <c r="E51" s="185"/>
       <c r="F51" s="186"/>
-      <c r="G51" s="213"/>
-      <c r="H51" s="213"/>
+      <c r="G51" s="214"/>
+      <c r="H51" s="214"/>
       <c r="I51" s="186"/>
-      <c r="J51" s="213"/>
-      <c r="K51" s="213"/>
-      <c r="L51" s="186"/>
-      <c r="M51" s="213"/>
-      <c r="N51" s="213"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J51" s="214"/>
+      <c r="K51" s="214">
+        <f>K50/1000</f>
+        <v>1921.92</v>
+      </c>
+      <c r="L51" s="190" t="s">
+        <v>14</v>
+      </c>
+      <c r="M51" s="214"/>
+      <c r="N51" s="214">
+        <f>N50/60</f>
+        <v>57.5</v>
+      </c>
+      <c r="O51" s="119" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="149"/>
       <c r="B52" s="186"/>
       <c r="C52" s="149"/>
       <c r="D52" s="149"/>
       <c r="E52" s="185"/>
       <c r="F52" s="186"/>
-      <c r="G52" s="213"/>
-      <c r="H52" s="213"/>
+      <c r="G52" s="214"/>
+      <c r="H52" s="214"/>
       <c r="I52" s="186"/>
-      <c r="J52" s="213"/>
-      <c r="K52" s="213"/>
+      <c r="J52" s="214"/>
+      <c r="K52" s="214"/>
       <c r="L52" s="186"/>
-      <c r="M52" s="213"/>
-      <c r="N52" s="213"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M52" s="214"/>
+      <c r="N52" s="214"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="149"/>
       <c r="B53" s="186"/>
       <c r="C53" s="149"/>
       <c r="D53" s="149"/>
       <c r="E53" s="185"/>
       <c r="F53" s="186"/>
-      <c r="G53" s="213"/>
-      <c r="H53" s="213"/>
+      <c r="G53" s="214"/>
+      <c r="H53" s="214"/>
       <c r="I53" s="186"/>
-      <c r="J53" s="213"/>
-      <c r="K53" s="213"/>
+      <c r="J53" s="214"/>
+      <c r="K53" s="214"/>
       <c r="L53" s="186"/>
-      <c r="M53" s="213"/>
-      <c r="N53" s="213"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M53" s="214"/>
+      <c r="N53" s="214"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="149"/>
       <c r="B54" s="186"/>
       <c r="C54" s="149"/>
       <c r="D54" s="149"/>
       <c r="E54" s="185"/>
       <c r="F54" s="186"/>
-      <c r="G54" s="213"/>
-      <c r="H54" s="213"/>
+      <c r="G54" s="214"/>
+      <c r="H54" s="214"/>
       <c r="I54" s="186"/>
-      <c r="J54" s="213"/>
-      <c r="K54" s="213"/>
+      <c r="J54" s="214"/>
+      <c r="K54" s="214"/>
       <c r="L54" s="186"/>
-      <c r="M54" s="213"/>
-      <c r="N54" s="213"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M54" s="214"/>
+      <c r="N54" s="214"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="149"/>
       <c r="B55" s="186"/>
       <c r="C55" s="149"/>
       <c r="D55" s="149"/>
       <c r="E55" s="185"/>
       <c r="F55" s="186"/>
-      <c r="G55" s="213"/>
-      <c r="H55" s="213"/>
+      <c r="G55" s="214"/>
+      <c r="H55" s="214"/>
       <c r="I55" s="186"/>
-      <c r="J55" s="213"/>
-      <c r="K55" s="213"/>
+      <c r="J55" s="214"/>
+      <c r="K55" s="214"/>
       <c r="L55" s="186"/>
-      <c r="M55" s="213"/>
-      <c r="N55" s="213"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M55" s="214"/>
+      <c r="N55" s="214"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="149"/>
       <c r="B56" s="186"/>
       <c r="C56" s="149"/>
       <c r="D56" s="149"/>
       <c r="E56" s="185"/>
       <c r="F56" s="186"/>
-      <c r="G56" s="213"/>
-      <c r="H56" s="213"/>
+      <c r="G56" s="214"/>
+      <c r="H56" s="214"/>
       <c r="I56" s="186"/>
-      <c r="J56" s="213"/>
-      <c r="K56" s="213"/>
+      <c r="J56" s="214"/>
+      <c r="K56" s="214"/>
       <c r="L56" s="186"/>
-      <c r="M56" s="213"/>
-      <c r="N56" s="213"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M56" s="214"/>
+      <c r="N56" s="214"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="149"/>
       <c r="B57" s="186"/>
       <c r="C57" s="149"/>
       <c r="D57" s="149"/>
       <c r="E57" s="185"/>
       <c r="F57" s="186"/>
-      <c r="G57" s="213"/>
-      <c r="H57" s="213"/>
+      <c r="G57" s="214"/>
+      <c r="H57" s="214"/>
       <c r="I57" s="186"/>
-      <c r="J57" s="213"/>
-      <c r="K57" s="213"/>
+      <c r="J57" s="214"/>
+      <c r="K57" s="214"/>
       <c r="L57" s="186"/>
-      <c r="M57" s="213"/>
-      <c r="N57" s="213"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M57" s="214"/>
+      <c r="N57" s="214"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="149"/>
       <c r="B58" s="186"/>
       <c r="C58" s="149"/>
       <c r="D58" s="149"/>
       <c r="E58" s="185"/>
       <c r="F58" s="186"/>
-      <c r="G58" s="213"/>
-      <c r="H58" s="213"/>
+      <c r="G58" s="214"/>
+      <c r="H58" s="214"/>
       <c r="I58" s="186"/>
-      <c r="J58" s="213"/>
-      <c r="K58" s="213"/>
+      <c r="J58" s="214"/>
+      <c r="K58" s="214"/>
       <c r="L58" s="186"/>
-      <c r="M58" s="213"/>
-      <c r="N58" s="213"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M58" s="214"/>
+      <c r="N58" s="214"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="149"/>
       <c r="B59" s="186"/>
       <c r="C59" s="149"/>
       <c r="D59" s="149"/>
       <c r="E59" s="185"/>
       <c r="F59" s="186"/>
-      <c r="G59" s="213"/>
-      <c r="H59" s="213"/>
+      <c r="G59" s="214"/>
+      <c r="H59" s="214"/>
       <c r="I59" s="186"/>
-      <c r="J59" s="213"/>
-      <c r="K59" s="213"/>
+      <c r="J59" s="214"/>
+      <c r="K59" s="214"/>
       <c r="L59" s="186"/>
-      <c r="M59" s="213"/>
-      <c r="N59" s="213"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M59" s="214"/>
+      <c r="N59" s="214"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="149"/>
       <c r="B60" s="186"/>
       <c r="C60" s="149"/>
       <c r="D60" s="149"/>
       <c r="E60" s="185"/>
       <c r="F60" s="186"/>
-      <c r="G60" s="213"/>
-      <c r="H60" s="213"/>
+      <c r="G60" s="214"/>
+      <c r="H60" s="214"/>
       <c r="I60" s="186"/>
-      <c r="J60" s="213"/>
-      <c r="K60" s="213"/>
+      <c r="J60" s="214"/>
+      <c r="K60" s="214"/>
       <c r="L60" s="186"/>
-      <c r="M60" s="213"/>
-      <c r="N60" s="213"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M60" s="214"/>
+      <c r="N60" s="214"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="149"/>
       <c r="B61" s="186"/>
       <c r="C61" s="149"/>
       <c r="D61" s="149"/>
       <c r="E61" s="185"/>
       <c r="F61" s="186"/>
-      <c r="G61" s="213"/>
-      <c r="H61" s="213"/>
+      <c r="G61" s="214"/>
+      <c r="H61" s="214"/>
       <c r="I61" s="186"/>
-      <c r="J61" s="213"/>
-      <c r="K61" s="213"/>
+      <c r="J61" s="214"/>
+      <c r="K61" s="214"/>
       <c r="L61" s="186"/>
-      <c r="M61" s="213"/>
-      <c r="N61" s="213"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M61" s="214"/>
+      <c r="N61" s="214"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="149"/>
       <c r="B62" s="186"/>
       <c r="C62" s="149"/>
       <c r="D62" s="149"/>
       <c r="E62" s="185"/>
       <c r="F62" s="186"/>
-      <c r="G62" s="213"/>
-      <c r="H62" s="213"/>
+      <c r="G62" s="214"/>
+      <c r="H62" s="214"/>
       <c r="I62" s="186"/>
-      <c r="J62" s="213"/>
-      <c r="K62" s="213"/>
+      <c r="J62" s="214"/>
+      <c r="K62" s="214"/>
       <c r="L62" s="186"/>
-      <c r="M62" s="213"/>
-      <c r="N62" s="213"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M62" s="214"/>
+      <c r="N62" s="214"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="149"/>
       <c r="B63" s="186"/>
       <c r="C63" s="149"/>
       <c r="D63" s="149"/>
       <c r="E63" s="185"/>
       <c r="F63" s="186"/>
-      <c r="G63" s="213"/>
-      <c r="H63" s="213"/>
+      <c r="G63" s="214"/>
+      <c r="H63" s="214"/>
       <c r="I63" s="186"/>
-      <c r="J63" s="213"/>
-      <c r="K63" s="213"/>
+      <c r="J63" s="214"/>
+      <c r="K63" s="214"/>
       <c r="L63" s="186"/>
-      <c r="M63" s="213"/>
-      <c r="N63" s="213"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M63" s="214"/>
+      <c r="N63" s="214"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="149"/>
       <c r="B64" s="186"/>
       <c r="C64" s="149"/>
       <c r="D64" s="149"/>
       <c r="E64" s="185"/>
       <c r="F64" s="186"/>
-      <c r="G64" s="213"/>
-      <c r="H64" s="213"/>
+      <c r="G64" s="214"/>
+      <c r="H64" s="214"/>
       <c r="I64" s="186"/>
-      <c r="J64" s="213"/>
-      <c r="K64" s="213"/>
+      <c r="J64" s="214"/>
+      <c r="K64" s="214"/>
       <c r="L64" s="186"/>
-      <c r="M64" s="213"/>
-      <c r="N64" s="213"/>
+      <c r="M64" s="214"/>
+      <c r="N64" s="214"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -11759,19 +12146,241 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A26:C42"/>
+  <dimension ref="A4:P42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="143" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="143" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="143"/>
+    <col min="3" max="8" width="9.140625" style="143"/>
+    <col min="9" max="9" width="15.7109375" style="143" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="143" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="143" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="143" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="143" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="143"/>
+    <col min="15" max="15" width="18.5703125" style="143" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="143"/>
   </cols>
   <sheetData>
+    <row r="4" spans="8:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H4" s="225" t="s">
+        <v>365</v>
+      </c>
+      <c r="I4" s="119" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="8:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H5" s="225" t="s">
+        <v>372</v>
+      </c>
+      <c r="I5" s="119" t="s">
+        <v>367</v>
+      </c>
+      <c r="J5" s="119" t="s">
+        <v>368</v>
+      </c>
+      <c r="K5" s="119" t="s">
+        <v>369</v>
+      </c>
+      <c r="L5" s="119" t="s">
+        <v>370</v>
+      </c>
+      <c r="M5" s="119" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="6" spans="8:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H6" s="225" t="s">
+        <v>383</v>
+      </c>
+      <c r="I6" s="119" t="s">
+        <v>373</v>
+      </c>
+      <c r="J6" s="119" t="s">
+        <v>374</v>
+      </c>
+      <c r="K6" s="119" t="s">
+        <v>375</v>
+      </c>
+      <c r="L6" s="119" t="s">
+        <v>376</v>
+      </c>
+      <c r="M6" s="119" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="7" spans="8:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H7" s="225" t="s">
+        <v>384</v>
+      </c>
+      <c r="I7" s="119" t="s">
+        <v>378</v>
+      </c>
+      <c r="J7" s="119" t="s">
+        <v>379</v>
+      </c>
+      <c r="K7" s="119" t="s">
+        <v>380</v>
+      </c>
+      <c r="L7" s="119" t="s">
+        <v>381</v>
+      </c>
+      <c r="M7" s="119" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="8:16" x14ac:dyDescent="0.2">
+      <c r="I10" s="220" t="s">
+        <v>365</v>
+      </c>
+      <c r="K10" s="220" t="s">
+        <v>388</v>
+      </c>
+      <c r="M10" s="220" t="s">
+        <v>383</v>
+      </c>
+      <c r="O10" s="119" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="11" spans="8:16" x14ac:dyDescent="0.2">
+      <c r="I11" s="226" t="s">
+        <v>385</v>
+      </c>
+      <c r="J11" s="226" t="s">
+        <v>386</v>
+      </c>
+      <c r="K11" s="226" t="s">
+        <v>389</v>
+      </c>
+      <c r="L11" s="226" t="s">
+        <v>386</v>
+      </c>
+      <c r="M11" s="226" t="s">
+        <v>389</v>
+      </c>
+      <c r="N11" s="226" t="s">
+        <v>386</v>
+      </c>
+      <c r="O11" s="226" t="s">
+        <v>389</v>
+      </c>
+      <c r="P11" s="226" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="12" spans="8:16" x14ac:dyDescent="0.2">
+      <c r="I12" s="220" t="s">
+        <v>366</v>
+      </c>
+      <c r="J12" s="119" t="s">
+        <v>387</v>
+      </c>
+      <c r="K12" s="220" t="s">
+        <v>367</v>
+      </c>
+      <c r="L12" s="143">
+        <v>20</v>
+      </c>
+      <c r="M12" s="220" t="s">
+        <v>373</v>
+      </c>
+      <c r="N12" s="143">
+        <v>32</v>
+      </c>
+      <c r="O12" s="220" t="s">
+        <v>378</v>
+      </c>
+      <c r="P12" s="143">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="8:16" x14ac:dyDescent="0.2">
+      <c r="K13" s="220" t="s">
+        <v>368</v>
+      </c>
+      <c r="L13" s="143">
+        <v>35</v>
+      </c>
+      <c r="M13" s="220" t="s">
+        <v>374</v>
+      </c>
+      <c r="N13" s="143">
+        <v>56</v>
+      </c>
+      <c r="O13" s="220" t="s">
+        <v>379</v>
+      </c>
+      <c r="P13" s="143">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="8:16" x14ac:dyDescent="0.2">
+      <c r="K14" s="220" t="s">
+        <v>370</v>
+      </c>
+      <c r="L14" s="143">
+        <v>60</v>
+      </c>
+      <c r="M14" s="119" t="s">
+        <v>376</v>
+      </c>
+      <c r="N14" s="143">
+        <v>96</v>
+      </c>
+      <c r="O14" s="220" t="s">
+        <v>381</v>
+      </c>
+      <c r="P14" s="143">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="8:16" x14ac:dyDescent="0.2">
+      <c r="K15" s="220" t="s">
+        <v>369</v>
+      </c>
+      <c r="L15" s="143">
+        <v>100</v>
+      </c>
+      <c r="M15" s="220" t="s">
+        <v>375</v>
+      </c>
+      <c r="N15" s="143">
+        <v>160</v>
+      </c>
+      <c r="O15" s="220" t="s">
+        <v>380</v>
+      </c>
+      <c r="P15" s="143">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="16" spans="8:16" x14ac:dyDescent="0.2">
+      <c r="K16" s="220" t="s">
+        <v>371</v>
+      </c>
+      <c r="L16" s="143">
+        <v>140</v>
+      </c>
+      <c r="M16" s="220" t="s">
+        <v>377</v>
+      </c>
+      <c r="N16" s="143">
+        <v>224</v>
+      </c>
+      <c r="O16" s="220" t="s">
+        <v>382</v>
+      </c>
+      <c r="P16" s="143">
+        <v>403</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="167" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
lots of changes made
</commit_message>
<xml_diff>
--- a/0 DyTech Informations/Dytech Balance.xlsx
+++ b/0 DyTech Informations/Dytech Balance.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
     <sheet name="Steam" sheetId="2" r:id="rId2"/>
     <sheet name="Solar Panels" sheetId="8" r:id="rId3"/>
-    <sheet name="Nuclear Reactor" sheetId="11" r:id="rId4"/>
-    <sheet name="Blad1" sheetId="12" r:id="rId5"/>
+    <sheet name="Nuclear Fuel" sheetId="11" r:id="rId4"/>
+    <sheet name="Membranes" sheetId="16" r:id="rId5"/>
     <sheet name="Laser Turrets" sheetId="3" r:id="rId6"/>
     <sheet name="Empty Sheet" sheetId="9" r:id="rId7"/>
     <sheet name="Gems" sheetId="10" r:id="rId8"/>
@@ -291,6 +291,88 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Jort Geurts</author>
+  </authors>
+  <commentList>
+    <comment ref="G6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MagicLegend:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Energy required to create the specific item per 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">MagicLegend:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sum of energy required to create all the items for the recipe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MagicLegend:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Energy used by the assembling machine to create the item stated in colum A</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author/>
   </authors>
   <commentList>
@@ -321,7 +403,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -644,7 +726,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="416">
   <si>
     <t>README</t>
   </si>
@@ -1678,9 +1760,6 @@
     <t>Total Energy</t>
   </si>
   <si>
-    <t>Clean water is based on the 500 -&gt; 460 recipe</t>
-  </si>
-  <si>
     <t>Mining energy is based on the basic mk 1 miner</t>
   </si>
   <si>
@@ -1837,19 +1916,64 @@
     <t>MW/sec</t>
   </si>
   <si>
-    <t>xx</t>
-  </si>
-  <si>
-    <t>ii</t>
-  </si>
-  <si>
     <t>Statements</t>
   </si>
   <si>
     <t>use S colum</t>
   </si>
   <si>
-    <t>false</t>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Membrane</t>
+  </si>
+  <si>
+    <t>Ruby membrane</t>
+  </si>
+  <si>
+    <t>Membrane frame</t>
+  </si>
+  <si>
+    <t>Iron stick</t>
+  </si>
+  <si>
+    <t>Iron stick recipe is based on the level 2 assembler</t>
+  </si>
+  <si>
+    <t>Mk 2 assembler</t>
+  </si>
+  <si>
+    <t>(0.75 speed)</t>
+  </si>
+  <si>
+    <t>Sapphire membrane</t>
+  </si>
+  <si>
+    <t>Topaz membrane</t>
+  </si>
+  <si>
+    <t>Emerald membrane</t>
+  </si>
+  <si>
+    <t>Diamond membrane</t>
+  </si>
+  <si>
+    <t>Raw-ruby</t>
+  </si>
+  <si>
+    <t>Raw-sapphire</t>
+  </si>
+  <si>
+    <t>Raw-topaz</t>
+  </si>
+  <si>
+    <t>Raw-emerald</t>
+  </si>
+  <si>
+    <t>Raw-diamond</t>
+  </si>
+  <si>
+    <t>(minutes)</t>
   </si>
 </sst>
 </file>
@@ -1988,7 +2112,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="50">
+  <fills count="53">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2280,8 +2404,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2336,61 +2478,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -2406,6 +2495,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2414,7 +2585,7 @@
     <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2656,7 +2827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="40" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="0" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="40" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2713,24 +2884,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="44" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="44" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="44" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="44" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2763,6 +2916,51 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="44" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="44" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="44" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="44" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="50" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="38" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="38" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="38" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="38" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -7238,7 +7436,7 @@
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="226" t="s">
+      <c r="A3" s="220" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="186"/>
@@ -7308,7 +7506,7 @@
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="225" t="s">
+      <c r="K6" s="219" t="s">
         <v>43</v>
       </c>
       <c r="L6" s="186"/>
@@ -7722,7 +7920,7 @@
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="225" t="s">
+      <c r="K16" s="219" t="s">
         <v>120</v>
       </c>
       <c r="L16" s="186"/>
@@ -7739,9 +7937,9 @@
       <c r="W16" s="43"/>
       <c r="X16" s="43"/>
       <c r="Y16" s="43"/>
-      <c r="Z16" s="227"/>
+      <c r="Z16" s="221"/>
       <c r="AA16" s="186"/>
-      <c r="AB16" s="227"/>
+      <c r="AB16" s="221"/>
       <c r="AC16" s="186"/>
       <c r="AD16" s="57"/>
     </row>
@@ -9718,8 +9916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9742,7 +9940,7 @@
       <c r="Y1" s="119"/>
       <c r="Z1" s="119"/>
       <c r="AC1" s="119" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -9759,19 +9957,19 @@
       <c r="AA2" s="150"/>
       <c r="AB2" s="150"/>
     </row>
-    <row r="3" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="144" t="s">
         <v>333</v>
       </c>
-      <c r="D3" s="206" t="s">
+      <c r="D3" s="227" t="s">
         <v>344</v>
       </c>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
-      <c r="H3" s="208"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="229"/>
       <c r="Q3" s="169" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R3" s="166"/>
       <c r="S3" s="166"/>
@@ -9784,14 +9982,7 @@
       <c r="Z3" s="166"/>
       <c r="AA3" s="150"/>
     </row>
-    <row r="4" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="209" t="s">
-        <v>345</v>
-      </c>
-      <c r="E4" s="210"/>
-      <c r="F4" s="210"/>
-      <c r="G4" s="210"/>
-      <c r="H4" s="211"/>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Q4" s="170"/>
       <c r="R4" s="166"/>
       <c r="S4" s="166"/>
@@ -9851,18 +10042,18 @@
         <v>338</v>
       </c>
       <c r="Q6" s="164"/>
-      <c r="R6" s="212" t="s">
-        <v>347</v>
-      </c>
-      <c r="S6" s="212"/>
+      <c r="R6" s="206" t="s">
+        <v>346</v>
+      </c>
+      <c r="S6" s="206"/>
       <c r="T6" s="165"/>
-      <c r="V6" s="213" t="s">
-        <v>359</v>
-      </c>
-      <c r="W6" s="213"/>
-      <c r="X6" s="213"/>
+      <c r="V6" s="207" t="s">
+        <v>358</v>
+      </c>
+      <c r="W6" s="207"/>
+      <c r="X6" s="207"/>
       <c r="Y6" s="205" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="Z6" s="205"/>
       <c r="AA6" s="150"/>
@@ -9903,7 +10094,7 @@
       <c r="V7" s="163"/>
       <c r="W7" s="163"/>
       <c r="X7" s="168" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Y7" s="150"/>
       <c r="Z7" s="150"/>
@@ -9924,16 +10115,16 @@
       <c r="F8" s="153"/>
       <c r="G8" s="172">
         <f>IF(X22="true", X9*Y9*S8, X9*Y9*T8)</f>
-        <v>900</v>
+        <v>1800</v>
       </c>
       <c r="H8" s="176">
         <f>G8</f>
-        <v>900</v>
+        <v>1800</v>
       </c>
       <c r="I8" s="153"/>
       <c r="J8" s="172">
         <f>G8</f>
-        <v>900</v>
+        <v>1800</v>
       </c>
       <c r="K8" s="172"/>
       <c r="L8" s="153"/>
@@ -9953,7 +10144,7 @@
         <v>5</v>
       </c>
       <c r="V8" s="159" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="W8" s="160"/>
       <c r="X8" s="154">
@@ -9975,7 +10166,7 @@
       <c r="G9" s="172"/>
       <c r="H9" s="181">
         <f>H8</f>
-        <v>900</v>
+        <v>1800</v>
       </c>
       <c r="I9" s="153"/>
       <c r="J9" s="172"/>
@@ -10000,7 +10191,7 @@
         <v>120</v>
       </c>
       <c r="V9" s="159" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="W9" s="160"/>
       <c r="X9" s="154">
@@ -10010,7 +10201,7 @@
         <v>2</v>
       </c>
       <c r="Z9" s="119" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AA9" s="150"/>
     </row>
@@ -10027,7 +10218,7 @@
       <c r="J10" s="172"/>
       <c r="K10" s="179">
         <f>H8</f>
-        <v>900</v>
+        <v>1800</v>
       </c>
       <c r="L10" s="153"/>
       <c r="M10" s="172"/>
@@ -10064,11 +10255,11 @@
       <c r="F11" s="153"/>
       <c r="G11" s="172">
         <f>J8</f>
-        <v>900</v>
+        <v>1800</v>
       </c>
       <c r="H11" s="172">
         <f>G11*E11</f>
-        <v>1800</v>
+        <v>3600</v>
       </c>
       <c r="I11" s="153"/>
       <c r="J11" s="172">
@@ -10079,7 +10270,7 @@
       <c r="L11" s="153"/>
       <c r="M11" s="172">
         <f>IF(X22="true", S9+S8*E11, T9+T8*E11)</f>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="N11" s="172"/>
       <c r="Q11" s="164"/>
@@ -10114,7 +10305,7 @@
       <c r="I12" s="153"/>
       <c r="J12" s="172">
         <f>J11+H13</f>
-        <v>16800</v>
+        <v>18600</v>
       </c>
       <c r="K12" s="172"/>
       <c r="L12" s="153"/>
@@ -10149,22 +10340,22 @@
       <c r="G13" s="172"/>
       <c r="H13" s="172">
         <f>H11+H12</f>
-        <v>1800</v>
+        <v>3600</v>
       </c>
       <c r="I13" s="153"/>
       <c r="J13" s="171"/>
       <c r="K13" s="179">
         <f>K10+J12</f>
-        <v>17700</v>
+        <v>20400</v>
       </c>
       <c r="L13" s="153"/>
       <c r="M13" s="171">
         <f>M11+M12</f>
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="N13" s="172">
         <f>N9+M13</f>
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="Q13" s="164"/>
       <c r="R13" s="162" t="s">
@@ -10230,11 +10421,11 @@
       <c r="F15" s="153"/>
       <c r="G15" s="172">
         <f>J12</f>
-        <v>16800</v>
+        <v>18600</v>
       </c>
       <c r="H15" s="172">
         <f>G15*E15</f>
-        <v>33600</v>
+        <v>37200</v>
       </c>
       <c r="I15" s="153"/>
       <c r="J15" s="172">
@@ -10245,7 +10436,7 @@
       <c r="L15" s="153"/>
       <c r="M15" s="172">
         <f>IF(X22="true", S10+S9*E15, T10+T9*E15)</f>
-        <v>420</v>
+        <v>210</v>
       </c>
       <c r="N15" s="172"/>
       <c r="Q15" s="164"/>
@@ -10280,7 +10471,7 @@
       <c r="I16" s="153"/>
       <c r="J16" s="172">
         <f>J15+H17</f>
-        <v>56100</v>
+        <v>59700</v>
       </c>
       <c r="K16" s="172"/>
       <c r="L16" s="153"/>
@@ -10315,22 +10506,22 @@
       <c r="G17" s="172"/>
       <c r="H17" s="181">
         <f>H15+H16</f>
-        <v>33600</v>
+        <v>37200</v>
       </c>
       <c r="I17" s="153"/>
       <c r="J17" s="172"/>
       <c r="K17" s="179">
         <f>K13+J16</f>
-        <v>73800</v>
+        <v>80100</v>
       </c>
       <c r="L17" s="153"/>
       <c r="M17" s="172">
         <f>M15+M16</f>
-        <v>420</v>
+        <v>210</v>
       </c>
       <c r="N17" s="172">
         <f>N13+M17</f>
-        <v>560</v>
+        <v>300</v>
       </c>
       <c r="Q17" s="164"/>
       <c r="R17" s="162" t="s">
@@ -10371,7 +10562,7 @@
         <v>27</v>
       </c>
       <c r="T18" s="158" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="V18" s="160"/>
       <c r="W18" s="160"/>
@@ -10395,11 +10586,11 @@
       <c r="F19" s="153"/>
       <c r="G19" s="172">
         <f>J16</f>
-        <v>56100</v>
+        <v>59700</v>
       </c>
       <c r="H19" s="172">
         <f>G19*E19</f>
-        <v>112200</v>
+        <v>119400</v>
       </c>
       <c r="I19" s="153"/>
       <c r="J19" s="172">
@@ -10410,7 +10601,7 @@
       <c r="L19" s="153"/>
       <c r="M19" s="172">
         <f>IF(X22="true", S11+S10*E19, T11+T10*E19)</f>
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="N19" s="172"/>
       <c r="Q19" s="164"/>
@@ -10439,7 +10630,7 @@
       <c r="I20" s="153"/>
       <c r="J20" s="172">
         <f>J19+H21</f>
-        <v>142200</v>
+        <v>149400</v>
       </c>
       <c r="K20" s="172"/>
       <c r="L20" s="153"/>
@@ -10449,12 +10640,12 @@
       <c r="N20" s="177"/>
       <c r="Q20" s="164"/>
       <c r="R20" s="161" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S20" s="156"/>
       <c r="T20" s="156"/>
-      <c r="V20" s="228" t="s">
-        <v>399</v>
+      <c r="V20" s="222" t="s">
+        <v>396</v>
       </c>
       <c r="W20" s="150"/>
       <c r="X20" s="150"/>
@@ -10472,26 +10663,26 @@
       <c r="G21" s="172"/>
       <c r="H21" s="181">
         <f>H19+H20</f>
-        <v>112200</v>
+        <v>119400</v>
       </c>
       <c r="I21" s="153"/>
       <c r="J21" s="172"/>
       <c r="K21" s="179">
         <f>K17+J20</f>
-        <v>216000</v>
+        <v>229500</v>
       </c>
       <c r="L21" s="153"/>
       <c r="M21" s="171">
         <f>M19+M20</f>
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="N21" s="171">
         <f>M21+N17</f>
-        <v>1160</v>
+        <v>600</v>
       </c>
       <c r="Q21" s="164"/>
       <c r="R21" s="161" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S21" s="156"/>
       <c r="T21" s="156"/>
@@ -10519,16 +10710,16 @@
       <c r="N22" s="172"/>
       <c r="Q22" s="164"/>
       <c r="R22" s="161" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="S22" s="156"/>
       <c r="T22" s="156"/>
       <c r="V22" s="119" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="W22" s="150"/>
       <c r="X22" s="119" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="Y22" s="150"/>
       <c r="Z22" s="150"/>
@@ -10549,11 +10740,11 @@
       <c r="F23" s="153"/>
       <c r="G23" s="172">
         <f>J20</f>
-        <v>142200</v>
+        <v>149400</v>
       </c>
       <c r="H23" s="172">
         <f>G23*E23</f>
-        <v>284400</v>
+        <v>298800</v>
       </c>
       <c r="I23" s="153"/>
       <c r="J23" s="172">
@@ -10564,12 +10755,12 @@
       <c r="L23" s="182"/>
       <c r="M23" s="172">
         <f>IF(X22="true", S12+S11*E23, T12+T11*E23)</f>
-        <v>780</v>
+        <v>390</v>
       </c>
       <c r="N23" s="152"/>
       <c r="Q23" s="164"/>
       <c r="R23" s="161" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="S23" s="156"/>
       <c r="T23" s="156"/>
@@ -10596,7 +10787,7 @@
       <c r="I24" s="153"/>
       <c r="J24" s="172">
         <f>J23+H25</f>
-        <v>321900</v>
+        <v>336300</v>
       </c>
       <c r="K24" s="172"/>
       <c r="L24" s="153"/>
@@ -10606,7 +10797,7 @@
       <c r="N24" s="177"/>
       <c r="Q24" s="164"/>
       <c r="R24" s="161" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="S24" s="156"/>
       <c r="T24" s="156"/>
@@ -10628,26 +10819,26 @@
       <c r="G25" s="172"/>
       <c r="H25" s="172">
         <f>H24+H23</f>
-        <v>284400</v>
+        <v>298800</v>
       </c>
       <c r="I25" s="153"/>
       <c r="J25" s="172"/>
       <c r="K25" s="179">
         <f>K21+J24</f>
-        <v>537900</v>
+        <v>565800</v>
       </c>
       <c r="L25" s="153"/>
       <c r="M25" s="172">
         <f>M24+M23</f>
-        <v>780</v>
+        <v>390</v>
       </c>
       <c r="N25" s="172">
         <f>N21+M25</f>
-        <v>1940</v>
+        <v>990</v>
       </c>
       <c r="Q25" s="164"/>
       <c r="R25" s="161" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S25" s="156"/>
       <c r="T25" s="156"/>
@@ -10676,7 +10867,7 @@
       <c r="N26" s="172"/>
       <c r="Q26" s="164"/>
       <c r="R26" s="161" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S26" s="156"/>
       <c r="T26" s="156"/>
@@ -10703,11 +10894,11 @@
       <c r="F27" s="153"/>
       <c r="G27" s="172">
         <f>H25</f>
-        <v>284400</v>
+        <v>298800</v>
       </c>
       <c r="H27" s="172">
         <f>G27*E27</f>
-        <v>568800</v>
+        <v>597600</v>
       </c>
       <c r="I27" s="153"/>
       <c r="J27" s="172">
@@ -10718,12 +10909,12 @@
       <c r="L27" s="153"/>
       <c r="M27" s="172">
         <f>IF(X22="true", S13+S12*E27, T13+T12*E27)</f>
-        <v>960</v>
+        <v>480</v>
       </c>
       <c r="N27" s="172"/>
       <c r="Q27" s="164"/>
       <c r="R27" s="161" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="S27" s="156"/>
       <c r="T27" s="156"/>
@@ -10750,7 +10941,7 @@
       <c r="I28" s="153"/>
       <c r="J28" s="172">
         <f>J27+H29</f>
-        <v>613800</v>
+        <v>642600</v>
       </c>
       <c r="K28" s="172"/>
       <c r="L28" s="153"/>
@@ -10760,7 +10951,7 @@
       <c r="N28" s="177"/>
       <c r="Q28" s="164"/>
       <c r="R28" s="161" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S28" s="156"/>
       <c r="T28" s="156"/>
@@ -10782,26 +10973,26 @@
       <c r="G29" s="172"/>
       <c r="H29" s="172">
         <f>H28+H27</f>
-        <v>568800</v>
+        <v>597600</v>
       </c>
       <c r="I29" s="153"/>
       <c r="J29" s="172"/>
       <c r="K29" s="179">
         <f>K25+J28</f>
-        <v>1151700</v>
+        <v>1208400</v>
       </c>
       <c r="L29" s="153"/>
       <c r="M29" s="172">
         <f>M27+M28</f>
-        <v>960</v>
+        <v>480</v>
       </c>
       <c r="N29" s="172">
         <f>N25+M29</f>
-        <v>2900</v>
+        <v>1470</v>
       </c>
       <c r="Q29" s="164"/>
       <c r="R29" s="161" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="S29" s="156"/>
       <c r="T29" s="156"/>
@@ -10855,11 +11046,11 @@
       <c r="F31" s="153"/>
       <c r="G31" s="172">
         <f>J28</f>
-        <v>613800</v>
+        <v>642600</v>
       </c>
       <c r="H31" s="172">
         <f>G31*E31</f>
-        <v>1227600</v>
+        <v>1285200</v>
       </c>
       <c r="I31" s="153"/>
       <c r="J31" s="172">
@@ -10870,7 +11061,7 @@
       <c r="L31" s="153"/>
       <c r="M31" s="172">
         <f>IF(X22="true", S14+S13*E31, T14+T13*E31)</f>
-        <v>1140</v>
+        <v>570</v>
       </c>
       <c r="N31" s="172"/>
       <c r="Q31" s="164"/>
@@ -10899,7 +11090,7 @@
       <c r="I32" s="153"/>
       <c r="J32" s="172">
         <f>J31+H33</f>
-        <v>1280100</v>
+        <v>1337700</v>
       </c>
       <c r="K32" s="172"/>
       <c r="L32" s="153"/>
@@ -10929,22 +11120,22 @@
       <c r="G33" s="172"/>
       <c r="H33" s="172">
         <f>H32+H31</f>
-        <v>1227600</v>
+        <v>1285200</v>
       </c>
       <c r="I33" s="153"/>
       <c r="J33" s="172"/>
       <c r="K33" s="179">
         <f>K29+J32</f>
-        <v>2431800</v>
+        <v>2546100</v>
       </c>
       <c r="L33" s="153"/>
       <c r="M33" s="172">
         <f>M31+M32</f>
-        <v>1140</v>
+        <v>570</v>
       </c>
       <c r="N33" s="172">
         <f>N29+M33</f>
-        <v>4040</v>
+        <v>2040</v>
       </c>
       <c r="Q33" s="150"/>
       <c r="R33" s="150"/>
@@ -11002,11 +11193,11 @@
       <c r="F35" s="153"/>
       <c r="G35" s="172">
         <f>J32</f>
-        <v>1280100</v>
+        <v>1337700</v>
       </c>
       <c r="H35" s="171">
         <f>G35*E35</f>
-        <v>2560200</v>
+        <v>2675400</v>
       </c>
       <c r="I35" s="153"/>
       <c r="J35" s="172">
@@ -11017,7 +11208,7 @@
       <c r="L35" s="153"/>
       <c r="M35" s="172">
         <f>IF(X22="true", S15+S14*E35, T15+T14*E35)</f>
-        <v>1320</v>
+        <v>660</v>
       </c>
       <c r="N35" s="172"/>
       <c r="Q35" s="150"/>
@@ -11047,7 +11238,7 @@
       <c r="I36" s="153"/>
       <c r="J36" s="172">
         <f>J35+H37</f>
-        <v>2620200</v>
+        <v>2735400</v>
       </c>
       <c r="K36" s="171"/>
       <c r="L36" s="153"/>
@@ -11066,22 +11257,22 @@
       <c r="G37" s="172"/>
       <c r="H37" s="172">
         <f>H36+H35</f>
-        <v>2560200</v>
+        <v>2675400</v>
       </c>
       <c r="I37" s="153"/>
       <c r="J37" s="172"/>
       <c r="K37" s="179">
         <f>K33+J36</f>
-        <v>5052000</v>
+        <v>5281500</v>
       </c>
       <c r="L37" s="153"/>
       <c r="M37" s="172">
         <f>M35+M36</f>
-        <v>1320</v>
+        <v>660</v>
       </c>
       <c r="N37" s="172">
         <f>N33+M37</f>
-        <v>5360</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.2">
@@ -11115,11 +11306,11 @@
       <c r="F39" s="153"/>
       <c r="G39" s="172">
         <f>J36</f>
-        <v>2620200</v>
+        <v>2735400</v>
       </c>
       <c r="H39" s="172">
         <f>G39*E39</f>
-        <v>5240400</v>
+        <v>5470800</v>
       </c>
       <c r="I39" s="153"/>
       <c r="J39" s="172">
@@ -11130,7 +11321,7 @@
       <c r="L39" s="153"/>
       <c r="M39" s="172">
         <f>IF(X22="true", S16+S15*E39, T16+T15*E39)</f>
-        <v>1500</v>
+        <v>750</v>
       </c>
       <c r="N39" s="172"/>
     </row>
@@ -11148,7 +11339,7 @@
       <c r="I40" s="153"/>
       <c r="J40" s="172">
         <f>J39+H41</f>
-        <v>5307900</v>
+        <v>5538300</v>
       </c>
       <c r="K40" s="172"/>
       <c r="L40" s="153"/>
@@ -11167,22 +11358,22 @@
       <c r="G41" s="172"/>
       <c r="H41" s="172">
         <f>H39+H40</f>
-        <v>5240400</v>
+        <v>5470800</v>
       </c>
       <c r="I41" s="153"/>
       <c r="J41" s="172"/>
       <c r="K41" s="179">
         <f>K37+J40</f>
-        <v>10359900</v>
+        <v>10819800</v>
       </c>
       <c r="L41" s="153"/>
       <c r="M41" s="172">
         <f>M40+M39</f>
-        <v>1500</v>
+        <v>750</v>
       </c>
       <c r="N41" s="172">
         <f>N37+M41</f>
-        <v>6860</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.2">
@@ -11216,11 +11407,11 @@
       <c r="F43" s="153"/>
       <c r="G43" s="172">
         <f>J40</f>
-        <v>5307900</v>
+        <v>5538300</v>
       </c>
       <c r="H43" s="172">
         <f>G43*E43</f>
-        <v>10615800</v>
+        <v>11076600</v>
       </c>
       <c r="I43" s="153"/>
       <c r="J43" s="172">
@@ -11231,7 +11422,7 @@
       <c r="L43" s="153"/>
       <c r="M43" s="172">
         <f>IF(X22="true", S17+S16*E43, T17+T16*E43)</f>
-        <v>1680</v>
+        <v>840</v>
       </c>
       <c r="N43" s="172"/>
     </row>
@@ -11249,7 +11440,7 @@
       <c r="I44" s="153"/>
       <c r="J44" s="172">
         <f>J43+H45</f>
-        <v>10690800</v>
+        <v>11151600</v>
       </c>
       <c r="K44" s="172"/>
       <c r="L44" s="153"/>
@@ -11268,22 +11459,22 @@
       <c r="G45" s="172"/>
       <c r="H45" s="172">
         <f>H44+H43</f>
-        <v>10615800</v>
+        <v>11076600</v>
       </c>
       <c r="I45" s="153"/>
       <c r="J45" s="172"/>
       <c r="K45" s="179">
         <f>J44+K41</f>
-        <v>21050700</v>
+        <v>21971400</v>
       </c>
       <c r="L45" s="153"/>
       <c r="M45" s="172">
         <f>M44+M43</f>
-        <v>1680</v>
+        <v>840</v>
       </c>
       <c r="N45" s="172">
         <f>M45+N41</f>
-        <v>8540</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
@@ -11346,12 +11537,12 @@
       <c r="I49" s="153"/>
       <c r="J49" s="172"/>
       <c r="K49" s="176" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L49" s="153"/>
       <c r="M49" s="172"/>
       <c r="N49" s="176" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
@@ -11367,15 +11558,15 @@
       <c r="J50" s="172"/>
       <c r="K50" s="172">
         <f>K45</f>
-        <v>21050700</v>
+        <v>21971400</v>
       </c>
       <c r="L50" s="157" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M50" s="172"/>
       <c r="N50" s="172">
         <f>N45</f>
-        <v>8540</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
@@ -11391,7 +11582,7 @@
       <c r="J51" s="172"/>
       <c r="K51" s="172">
         <f>K50/1000</f>
-        <v>21050.7</v>
+        <v>21971.4</v>
       </c>
       <c r="L51" s="157" t="s">
         <v>14</v>
@@ -11399,10 +11590,10 @@
       <c r="M51" s="172"/>
       <c r="N51" s="172">
         <f>N50/60</f>
-        <v>142.33333333333334</v>
+        <v>71.5</v>
       </c>
       <c r="O51" s="119" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
@@ -11419,7 +11610,7 @@
       <c r="K52" s="172"/>
       <c r="L52" s="153"/>
       <c r="M52" s="172"/>
-      <c r="N52" s="229"/>
+      <c r="N52" s="223"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="149"/>
@@ -11450,10 +11641,10 @@
       <c r="J54" s="172"/>
       <c r="K54" s="172">
         <f>K51/N51</f>
-        <v>147.89718969555034</v>
+        <v>307.2923076923077</v>
       </c>
       <c r="L54" s="153" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M54" s="172"/>
       <c r="N54" s="172"/>
@@ -11471,10 +11662,10 @@
       <c r="J55" s="172"/>
       <c r="K55" s="172">
         <f>K54/60</f>
-        <v>2.4649531615925055</v>
+        <v>5.1215384615384618</v>
       </c>
       <c r="L55" s="153" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M55" s="172"/>
       <c r="N55" s="172"/>
@@ -11624,10 +11815,9 @@
       <c r="N64" s="172"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="Y6:Z6"/>
     <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:H4"/>
     <mergeCell ref="R6:S6"/>
     <mergeCell ref="V6:X6"/>
   </mergeCells>
@@ -11638,115 +11828,1514 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AA52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="173"/>
+    <col min="9" max="9" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="173"/>
+    <col min="11" max="11" width="10.140625" style="173" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="173"/>
+    <col min="18" max="18" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="151" t="s">
+    <row r="2" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="144" t="s">
+        <v>333</v>
+      </c>
+      <c r="C3" s="240" t="s">
+        <v>403</v>
+      </c>
+      <c r="D3" s="241"/>
+      <c r="E3" s="241"/>
+      <c r="F3" s="241"/>
+      <c r="G3" s="241"/>
+      <c r="H3" s="242"/>
+      <c r="Q3" s="169" t="s">
+        <v>345</v>
+      </c>
+      <c r="R3" s="166"/>
+      <c r="S3" s="166"/>
+      <c r="T3" s="166"/>
+      <c r="U3" s="166"/>
+      <c r="V3" s="166"/>
+      <c r="W3" s="166"/>
+      <c r="X3" s="166"/>
+      <c r="Y3" s="166"/>
+      <c r="Z3" s="166"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" s="119"/>
+      <c r="Q4" s="170"/>
+      <c r="R4" s="166"/>
+      <c r="S4" s="166"/>
+      <c r="T4" s="166"/>
+      <c r="U4" s="166"/>
+      <c r="V4" s="166"/>
+      <c r="W4" s="166"/>
+      <c r="X4" s="166"/>
+      <c r="Y4" s="166"/>
+      <c r="Z4" s="166"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Q5" s="164"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" s="145" t="s">
+        <v>399</v>
+      </c>
+      <c r="B6" s="146"/>
+      <c r="C6" s="147" t="s">
+        <v>334</v>
+      </c>
+      <c r="D6" s="146"/>
+      <c r="E6" s="147" t="s">
+        <v>336</v>
+      </c>
+      <c r="F6" s="146"/>
+      <c r="G6" s="174" t="s">
+        <v>335</v>
+      </c>
+      <c r="H6" s="174" t="s">
+        <v>335</v>
+      </c>
+      <c r="I6" s="146"/>
+      <c r="J6" s="174" t="s">
+        <v>335</v>
+      </c>
+      <c r="K6" s="174" t="s">
+        <v>343</v>
+      </c>
+      <c r="L6" s="146"/>
+      <c r="M6" s="174" t="s">
+        <v>337</v>
+      </c>
+      <c r="N6" s="174" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q6" s="164"/>
+      <c r="R6" s="206" t="s">
+        <v>346</v>
+      </c>
+      <c r="S6" s="206"/>
+      <c r="T6" s="165"/>
+      <c r="U6" s="151"/>
+      <c r="W6" s="224" t="s">
+        <v>358</v>
+      </c>
+      <c r="X6" s="224"/>
+      <c r="Y6" s="224"/>
+      <c r="Z6" s="136" t="s">
+        <v>362</v>
+      </c>
+      <c r="AA6" s="136"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="146"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="174" t="s">
+        <v>342</v>
+      </c>
+      <c r="H7" s="175" t="s">
+        <v>342</v>
+      </c>
+      <c r="I7" s="153"/>
+      <c r="J7" s="174" t="s">
+        <v>342</v>
+      </c>
+      <c r="K7" s="174" t="s">
+        <v>342</v>
+      </c>
+      <c r="L7" s="153"/>
+      <c r="M7" s="175" t="s">
+        <v>339</v>
+      </c>
+      <c r="N7" s="174" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q7" s="164"/>
+      <c r="R7" s="165"/>
+      <c r="S7" s="167" t="s">
+        <v>339</v>
+      </c>
+      <c r="T7" s="165"/>
+      <c r="U7" s="151"/>
+      <c r="W7" s="163"/>
+      <c r="X7" s="163"/>
+      <c r="Y7" s="168" t="s">
+        <v>360</v>
+      </c>
+      <c r="Z7" s="151"/>
+      <c r="AA7" s="151"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" s="148" t="s">
+        <v>401</v>
+      </c>
+      <c r="B8" s="230"/>
+      <c r="C8" s="148" t="s">
+        <v>402</v>
+      </c>
+      <c r="D8" s="149"/>
+      <c r="E8" s="152">
+        <v>10</v>
+      </c>
+      <c r="F8" s="153"/>
+      <c r="G8" s="250">
+        <f>M8*Z10*Y10</f>
+        <v>112.5</v>
+      </c>
+      <c r="H8" s="250">
+        <f>G8*E8</f>
+        <v>1125</v>
+      </c>
+      <c r="I8" s="153"/>
+      <c r="J8" s="250">
+        <f>IF(Y22="true", Y10*Z10*S8, Y10*Z10*T8)</f>
+        <v>1125</v>
+      </c>
+      <c r="K8" s="250"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="252">
+        <v>0.5</v>
+      </c>
+      <c r="N8" s="252"/>
+      <c r="Q8" s="164"/>
+      <c r="R8" s="161" t="s">
+        <v>401</v>
+      </c>
+      <c r="S8" s="156">
+        <v>5</v>
+      </c>
+      <c r="T8" s="156"/>
+      <c r="U8" s="226">
+        <f>IF(Y22 = "true", S8/60, T8/60)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="V8" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="W8" s="159" t="s">
+        <v>359</v>
+      </c>
+      <c r="X8" s="160"/>
+      <c r="Y8" s="154">
+        <v>250</v>
+      </c>
+      <c r="Z8" s="151"/>
+      <c r="AA8" s="151"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" s="149"/>
+      <c r="B9" s="230"/>
+      <c r="C9" s="148"/>
+      <c r="D9" s="149"/>
+      <c r="E9" s="152"/>
+      <c r="F9" s="153"/>
+      <c r="G9" s="250"/>
+      <c r="H9" s="253">
+        <f>H8</f>
+        <v>1125</v>
+      </c>
+      <c r="I9" s="153"/>
+      <c r="J9" s="250"/>
+      <c r="K9" s="255">
+        <f>J8+H9</f>
+        <v>2250</v>
+      </c>
+      <c r="L9" s="153"/>
+      <c r="M9" s="254">
+        <f>S8</f>
+        <v>5</v>
+      </c>
+      <c r="N9" s="254"/>
+      <c r="Q9" s="164"/>
+      <c r="R9" s="161" t="s">
+        <v>400</v>
+      </c>
+      <c r="S9" s="155">
+        <v>120</v>
+      </c>
+      <c r="T9" s="156"/>
+      <c r="U9" s="158">
+        <f>S9/60</f>
+        <v>2</v>
+      </c>
+      <c r="V9" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="W9" s="159" t="s">
+        <v>361</v>
+      </c>
+      <c r="X9" s="160"/>
+      <c r="Y9" s="154">
+        <v>90</v>
+      </c>
+      <c r="Z9" s="151">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="119" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="236"/>
+      <c r="B10" s="237"/>
+      <c r="C10" s="236"/>
+      <c r="D10" s="236"/>
+      <c r="E10" s="238"/>
+      <c r="F10" s="239"/>
+      <c r="G10" s="251"/>
+      <c r="H10" s="251"/>
+      <c r="I10" s="239"/>
+      <c r="J10" s="251"/>
+      <c r="K10" s="251"/>
+      <c r="L10" s="239"/>
+      <c r="M10" s="251">
+        <f>IF(Y22="true", M8*Z10*(E8/2)+M9, M8*Z10*(E8/2)+T8)</f>
+        <v>8.75</v>
+      </c>
+      <c r="N10" s="251">
+        <f>M10/60</f>
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="O10" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q10" s="164"/>
+      <c r="R10" s="161" t="s">
+        <v>406</v>
+      </c>
+      <c r="S10" s="155">
+        <v>180</v>
+      </c>
+      <c r="T10" s="156"/>
+      <c r="U10" s="226">
+        <f>S10/60</f>
+        <v>3</v>
+      </c>
+      <c r="V10" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="W10" s="159" t="s">
+        <v>404</v>
+      </c>
+      <c r="X10" s="160"/>
+      <c r="Y10" s="154">
+        <v>150</v>
+      </c>
+      <c r="Z10" s="151">
+        <v>1.5</v>
+      </c>
+      <c r="AA10" s="119" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="149"/>
+      <c r="B11" s="230"/>
+      <c r="C11" s="149"/>
+      <c r="D11" s="149"/>
+      <c r="E11" s="152"/>
+      <c r="F11" s="153"/>
+      <c r="G11" s="250"/>
+      <c r="H11" s="250"/>
+      <c r="I11" s="153"/>
+      <c r="J11" s="250"/>
+      <c r="K11" s="250"/>
+      <c r="L11" s="153"/>
+      <c r="M11" s="250"/>
+      <c r="N11" s="250"/>
+      <c r="Q11" s="164"/>
+      <c r="R11" s="161" t="s">
+        <v>407</v>
+      </c>
+      <c r="S11" s="155">
+        <v>240</v>
+      </c>
+      <c r="T11" s="156"/>
+      <c r="U11" s="226">
+        <f>S11/60</f>
+        <v>4</v>
+      </c>
+      <c r="V11" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="W11" s="160"/>
+      <c r="X11" s="160"/>
+      <c r="Y11" s="154"/>
+      <c r="Z11" s="151"/>
+      <c r="AA11" s="151"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="247" t="s">
+        <v>400</v>
+      </c>
+      <c r="B12" s="244"/>
+      <c r="C12" s="247" t="s">
+        <v>401</v>
+      </c>
+      <c r="D12" s="243"/>
+      <c r="E12" s="245">
+        <v>1</v>
+      </c>
+      <c r="F12" s="246"/>
+      <c r="G12" s="252">
+        <f>K9</f>
+        <v>2250</v>
+      </c>
+      <c r="H12" s="252">
+        <f>G12*E12</f>
+        <v>2250</v>
+      </c>
+      <c r="I12" s="246"/>
+      <c r="J12" s="252">
+        <f>Y10*Z10*S9</f>
+        <v>27000</v>
+      </c>
+      <c r="K12" s="252"/>
+      <c r="L12" s="246"/>
+      <c r="M12" s="252">
+        <f>M10</f>
+        <v>8.75</v>
+      </c>
+      <c r="N12" s="252"/>
+      <c r="Q12" s="164"/>
+      <c r="R12" s="161" t="s">
+        <v>408</v>
+      </c>
+      <c r="S12" s="155">
+        <v>300</v>
+      </c>
+      <c r="T12" s="156"/>
+      <c r="U12" s="226">
+        <f>S12/60</f>
+        <v>5</v>
+      </c>
+      <c r="V12" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="W12" s="160"/>
+      <c r="X12" s="160"/>
+      <c r="Y12" s="154"/>
+      <c r="Z12" s="151"/>
+      <c r="AA12" s="151"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" s="149"/>
+      <c r="B13" s="230"/>
+      <c r="C13" s="148" t="s">
+        <v>410</v>
+      </c>
+      <c r="D13" s="149"/>
+      <c r="E13" s="152">
+        <v>1</v>
+      </c>
+      <c r="F13" s="153"/>
+      <c r="G13" s="250">
+        <f>Y10*Z10*S17</f>
+        <v>4500</v>
+      </c>
+      <c r="H13" s="254">
+        <f>G13*E13</f>
+        <v>4500</v>
+      </c>
+      <c r="I13" s="153"/>
+      <c r="J13" s="250"/>
+      <c r="K13" s="250"/>
+      <c r="L13" s="153"/>
+      <c r="M13" s="252">
+        <f>S17</f>
+        <v>20</v>
+      </c>
+      <c r="N13" s="252"/>
+      <c r="Q13" s="164"/>
+      <c r="R13" s="161" t="s">
+        <v>409</v>
+      </c>
+      <c r="S13" s="156">
+        <v>360</v>
+      </c>
+      <c r="T13" s="156"/>
+      <c r="U13" s="226">
+        <f>S13/60</f>
+        <v>6</v>
+      </c>
+      <c r="V13" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="W13" s="160"/>
+      <c r="X13" s="160"/>
+      <c r="Y13" s="154"/>
+      <c r="Z13" s="151"/>
+      <c r="AA13" s="151"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" s="149"/>
+      <c r="B14" s="230"/>
+      <c r="C14" s="149"/>
+      <c r="D14" s="149"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="153"/>
+      <c r="G14" s="250"/>
+      <c r="H14" s="250">
+        <f>H13+H12</f>
+        <v>6750</v>
+      </c>
+      <c r="I14" s="153"/>
+      <c r="J14" s="250"/>
+      <c r="K14" s="250"/>
+      <c r="L14" s="153"/>
+      <c r="M14" s="254">
+        <f>IF(Y22="true", S9, T9)</f>
+        <v>120</v>
+      </c>
+      <c r="N14" s="254"/>
+      <c r="Q14" s="164"/>
+      <c r="R14" s="162"/>
+      <c r="S14" s="158">
+        <f>(S8+ S9+S10+S11+S12+S13)/60</f>
+        <v>20.083333333333332</v>
+      </c>
+      <c r="T14" s="158" t="s">
+        <v>393</v>
+      </c>
+      <c r="U14" s="151"/>
+      <c r="W14" s="160"/>
+      <c r="X14" s="160"/>
+      <c r="Y14" s="154"/>
+      <c r="Z14" s="151"/>
+      <c r="AA14" s="151"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A15" s="149"/>
+      <c r="B15" s="230"/>
+      <c r="C15" s="149"/>
+      <c r="D15" s="149"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="153"/>
+      <c r="G15" s="250"/>
+      <c r="H15" s="250"/>
+      <c r="I15" s="153"/>
+      <c r="J15" s="250"/>
+      <c r="K15" s="255">
+        <f>H14+J12</f>
+        <v>33750</v>
+      </c>
+      <c r="L15" s="153"/>
+      <c r="M15" s="250">
+        <f>M13+M12+M14</f>
+        <v>148.75</v>
+      </c>
+      <c r="N15" s="250">
+        <f>M15/60</f>
+        <v>2.4791666666666665</v>
+      </c>
+      <c r="O15" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q15" s="164"/>
+      <c r="R15" s="162"/>
+      <c r="S15" s="234"/>
+      <c r="T15" s="235"/>
+      <c r="U15" s="151"/>
+      <c r="W15" s="159"/>
+      <c r="X15" s="160"/>
+      <c r="Y15" s="154">
+        <v>60</v>
+      </c>
+      <c r="Z15" s="151"/>
+      <c r="AA15" s="151"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A16" s="149"/>
+      <c r="B16" s="230"/>
+      <c r="C16" s="149"/>
+      <c r="D16" s="149"/>
+      <c r="E16" s="152"/>
+      <c r="F16" s="153"/>
+      <c r="G16" s="250"/>
+      <c r="H16" s="250"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="250"/>
+      <c r="K16" s="250"/>
+      <c r="L16" s="153"/>
+      <c r="M16" s="250"/>
+      <c r="N16" s="250"/>
+      <c r="Q16" s="164"/>
+      <c r="R16" s="162"/>
+      <c r="S16" s="234"/>
+      <c r="T16" s="235"/>
+      <c r="U16" s="151"/>
+      <c r="W16" s="160"/>
+      <c r="X16" s="160"/>
+      <c r="Y16" s="154"/>
+      <c r="Z16" s="151"/>
+      <c r="AA16" s="151"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A17" s="148" t="s">
+        <v>406</v>
+      </c>
+      <c r="B17" s="230"/>
+      <c r="C17" s="148" t="s">
+        <v>401</v>
+      </c>
+      <c r="D17" s="149"/>
+      <c r="E17" s="152">
+        <v>1</v>
+      </c>
+      <c r="F17" s="153"/>
+      <c r="G17" s="250">
+        <f>K9</f>
+        <v>2250</v>
+      </c>
+      <c r="H17" s="250">
+        <f>G17*E17</f>
+        <v>2250</v>
+      </c>
+      <c r="I17" s="153"/>
+      <c r="J17" s="250">
+        <f>Y10*Z10*S10</f>
+        <v>40500</v>
+      </c>
+      <c r="K17" s="250"/>
+      <c r="L17" s="153"/>
+      <c r="M17" s="250">
+        <f>M10</f>
+        <v>8.75</v>
+      </c>
+      <c r="N17" s="250"/>
+      <c r="Q17" s="164"/>
+      <c r="R17" s="161" t="s">
+        <v>410</v>
+      </c>
+      <c r="S17" s="156">
+        <v>20</v>
+      </c>
+      <c r="T17" s="156"/>
+      <c r="U17" s="151"/>
+      <c r="W17" s="160"/>
+      <c r="X17" s="160"/>
+      <c r="Y17" s="154"/>
+      <c r="Z17" s="151"/>
+      <c r="AA17" s="151"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A18" s="149"/>
+      <c r="B18" s="230"/>
+      <c r="C18" s="148" t="s">
+        <v>411</v>
+      </c>
+      <c r="D18" s="149"/>
+      <c r="E18" s="152">
+        <v>1</v>
+      </c>
+      <c r="F18" s="153"/>
+      <c r="G18" s="250">
+        <f>Y10*Z10*S18</f>
+        <v>7875</v>
+      </c>
+      <c r="H18" s="254">
+        <f>G18*E18</f>
+        <v>7875</v>
+      </c>
+      <c r="I18" s="153"/>
+      <c r="J18" s="250"/>
+      <c r="K18" s="250"/>
+      <c r="L18" s="153"/>
+      <c r="M18" s="250">
+        <f>S18</f>
+        <v>35</v>
+      </c>
+      <c r="N18" s="250"/>
+      <c r="Q18" s="164"/>
+      <c r="R18" s="161" t="s">
+        <v>411</v>
+      </c>
+      <c r="S18" s="156">
+        <v>35</v>
+      </c>
+      <c r="T18" s="156"/>
+      <c r="U18" s="151"/>
+      <c r="W18" s="160"/>
+      <c r="X18" s="160"/>
+      <c r="Y18" s="154"/>
+      <c r="Z18" s="151"/>
+      <c r="AA18" s="151"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A19" s="149"/>
+      <c r="B19" s="230"/>
+      <c r="C19" s="149"/>
+      <c r="D19" s="149"/>
+      <c r="E19" s="152"/>
+      <c r="F19" s="153"/>
+      <c r="G19" s="250"/>
+      <c r="H19" s="250">
+        <f>H18+H17</f>
+        <v>10125</v>
+      </c>
+      <c r="I19" s="153"/>
+      <c r="J19" s="250"/>
+      <c r="K19" s="250"/>
+      <c r="L19" s="153"/>
+      <c r="M19" s="254">
+        <f>IF(Y22="true", S10, T10)</f>
+        <v>180</v>
+      </c>
+      <c r="N19" s="254"/>
+      <c r="Q19" s="164"/>
+      <c r="R19" s="161" t="s">
+        <v>412</v>
+      </c>
+      <c r="S19" s="156">
+        <v>60</v>
+      </c>
+      <c r="T19" s="156"/>
+      <c r="U19" s="151"/>
+      <c r="W19" s="151"/>
+      <c r="X19" s="151"/>
+      <c r="Y19" s="151"/>
+      <c r="Z19" s="151"/>
+      <c r="AA19" s="151"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20" s="149"/>
+      <c r="B20" s="230"/>
+      <c r="C20" s="149"/>
+      <c r="D20" s="149"/>
+      <c r="E20" s="152"/>
+      <c r="F20" s="153"/>
+      <c r="G20" s="250"/>
+      <c r="H20" s="250"/>
+      <c r="I20" s="153"/>
+      <c r="J20" s="250"/>
+      <c r="K20" s="255">
+        <f>J17+H19</f>
+        <v>50625</v>
+      </c>
+      <c r="L20" s="153"/>
+      <c r="M20" s="250">
+        <f>M19+M18+M17</f>
+        <v>223.75</v>
+      </c>
+      <c r="N20" s="250">
+        <f>M20/60</f>
+        <v>3.7291666666666665</v>
+      </c>
+      <c r="O20" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q20" s="164"/>
+      <c r="R20" s="161" t="s">
+        <v>413</v>
+      </c>
+      <c r="S20" s="156">
+        <v>100</v>
+      </c>
+      <c r="T20" s="156"/>
+      <c r="U20" s="151"/>
+      <c r="W20" s="248" t="s">
+        <v>396</v>
+      </c>
+      <c r="X20" s="230"/>
+      <c r="Y20" s="230"/>
+      <c r="Z20" s="151"/>
+      <c r="AA20" s="151"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A21" s="149"/>
+      <c r="B21" s="230"/>
+      <c r="C21" s="149"/>
+      <c r="D21" s="149"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="153"/>
+      <c r="G21" s="250"/>
+      <c r="H21" s="250"/>
+      <c r="I21" s="153"/>
+      <c r="J21" s="250"/>
+      <c r="K21" s="250"/>
+      <c r="L21" s="153"/>
+      <c r="M21" s="250"/>
+      <c r="N21" s="250"/>
+      <c r="Q21" s="164"/>
+      <c r="R21" s="161" t="s">
+        <v>414</v>
+      </c>
+      <c r="S21" s="156">
+        <v>140</v>
+      </c>
+      <c r="T21" s="156"/>
+      <c r="U21" s="151"/>
+      <c r="W21" s="233"/>
+      <c r="X21" s="233"/>
+      <c r="Y21" s="225"/>
+      <c r="Z21" s="151"/>
+      <c r="AA21" s="151"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A22" s="148" t="s">
+        <v>407</v>
+      </c>
+      <c r="B22" s="230"/>
+      <c r="C22" s="148" t="s">
+        <v>401</v>
+      </c>
+      <c r="D22" s="149"/>
+      <c r="E22" s="152">
+        <v>1</v>
+      </c>
+      <c r="F22" s="153"/>
+      <c r="G22" s="250">
+        <f>K9</f>
+        <v>2250</v>
+      </c>
+      <c r="H22" s="250">
+        <f>G22*E22</f>
+        <v>2250</v>
+      </c>
+      <c r="I22" s="153"/>
+      <c r="J22" s="250">
+        <f>Y10*Z10*S11</f>
+        <v>54000</v>
+      </c>
+      <c r="K22" s="250"/>
+      <c r="L22" s="153"/>
+      <c r="M22" s="250">
+        <f>M10</f>
+        <v>8.75</v>
+      </c>
+      <c r="N22" s="250"/>
+      <c r="Q22" s="164"/>
+      <c r="R22" s="234"/>
+      <c r="S22" s="235"/>
+      <c r="T22" s="235"/>
+      <c r="U22" s="151"/>
+      <c r="W22" s="232" t="s">
         <v>397</v>
       </c>
-      <c r="B1" s="151" t="s">
+      <c r="X22" s="233"/>
+      <c r="Y22" s="249" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <f>A2+B2</f>
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>16</v>
-      </c>
-      <c r="C3" s="151">
-        <f t="shared" ref="C3:E6" si="0">A3+B3</f>
-        <v>22</v>
-      </c>
-      <c r="E3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>17</v>
-      </c>
-      <c r="C4" s="151">
-        <f>A4+B4</f>
-        <v>24</v>
-      </c>
-      <c r="E4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>18</v>
-      </c>
-      <c r="C5" s="151">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E5">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>19</v>
-      </c>
-      <c r="C6" s="151">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="E6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9">
-        <f>SUM(C2:C8)</f>
-        <v>120</v>
-      </c>
+      <c r="Z22" s="151"/>
+      <c r="AA22" s="151"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A23" s="149"/>
+      <c r="B23" s="230"/>
+      <c r="C23" s="148" t="s">
+        <v>412</v>
+      </c>
+      <c r="D23" s="149"/>
+      <c r="E23" s="152">
+        <v>1</v>
+      </c>
+      <c r="F23" s="153"/>
+      <c r="G23" s="250">
+        <f>Y10*Z10*S19</f>
+        <v>13500</v>
+      </c>
+      <c r="H23" s="254">
+        <f>G23*E23</f>
+        <v>13500</v>
+      </c>
+      <c r="I23" s="153"/>
+      <c r="J23" s="250"/>
+      <c r="K23" s="250"/>
+      <c r="L23" s="153"/>
+      <c r="M23" s="250">
+        <f>S19</f>
+        <v>60</v>
+      </c>
+      <c r="N23" s="250"/>
+      <c r="Q23" s="164"/>
+      <c r="R23" s="234"/>
+      <c r="S23" s="235"/>
+      <c r="T23" s="235"/>
+      <c r="U23" s="151"/>
+      <c r="W23" s="233"/>
+      <c r="X23" s="233"/>
+      <c r="Y23" s="231"/>
+      <c r="Z23" s="151"/>
+      <c r="AA23" s="151"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24" s="149"/>
+      <c r="B24" s="230"/>
+      <c r="C24" s="149"/>
+      <c r="D24" s="149"/>
+      <c r="E24" s="152"/>
+      <c r="F24" s="153"/>
+      <c r="G24" s="250"/>
+      <c r="H24" s="250">
+        <f>H23+H22</f>
+        <v>15750</v>
+      </c>
+      <c r="I24" s="153"/>
+      <c r="J24" s="250"/>
+      <c r="K24" s="250"/>
+      <c r="L24" s="153"/>
+      <c r="M24" s="254">
+        <f>IF(Y22="true", S11, T11)</f>
+        <v>240</v>
+      </c>
+      <c r="N24" s="254"/>
+      <c r="Q24" s="164"/>
+      <c r="R24" s="234"/>
+      <c r="S24" s="235"/>
+      <c r="T24" s="235"/>
+      <c r="U24" s="151"/>
+      <c r="W24" s="233"/>
+      <c r="X24" s="233"/>
+      <c r="Y24" s="225"/>
+      <c r="Z24" s="151"/>
+      <c r="AA24" s="151"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25" s="149"/>
+      <c r="B25" s="230"/>
+      <c r="C25" s="149"/>
+      <c r="D25" s="149"/>
+      <c r="E25" s="152"/>
+      <c r="F25" s="153"/>
+      <c r="G25" s="250"/>
+      <c r="H25" s="250"/>
+      <c r="I25" s="153"/>
+      <c r="J25" s="250"/>
+      <c r="K25" s="255">
+        <f>J22+H24</f>
+        <v>69750</v>
+      </c>
+      <c r="L25" s="153"/>
+      <c r="M25" s="250">
+        <f>M24+M23+M22</f>
+        <v>308.75</v>
+      </c>
+      <c r="N25" s="250">
+        <f>M25/60</f>
+        <v>5.145833333333333</v>
+      </c>
+      <c r="O25" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q25" s="164"/>
+      <c r="R25" s="234"/>
+      <c r="S25" s="235"/>
+      <c r="T25" s="235"/>
+      <c r="U25" s="151"/>
+      <c r="W25" s="233"/>
+      <c r="X25" s="233"/>
+      <c r="Y25" s="225"/>
+      <c r="Z25" s="151"/>
+      <c r="AA25" s="151"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26" s="149"/>
+      <c r="B26" s="230"/>
+      <c r="C26" s="149"/>
+      <c r="D26" s="149"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="153"/>
+      <c r="G26" s="250"/>
+      <c r="H26" s="250"/>
+      <c r="I26" s="153"/>
+      <c r="J26" s="250"/>
+      <c r="K26" s="250"/>
+      <c r="L26" s="153"/>
+      <c r="M26" s="250"/>
+      <c r="N26" s="250"/>
+      <c r="R26" s="234"/>
+      <c r="S26" s="235"/>
+      <c r="T26" s="235"/>
+      <c r="U26" s="151"/>
+      <c r="W26" s="233"/>
+      <c r="X26" s="233"/>
+      <c r="Y26" s="225"/>
+      <c r="Z26" s="151"/>
+      <c r="AA26" s="151"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27" s="148" t="s">
+        <v>408</v>
+      </c>
+      <c r="B27" s="230"/>
+      <c r="C27" s="148" t="s">
+        <v>401</v>
+      </c>
+      <c r="D27" s="149"/>
+      <c r="E27" s="152">
+        <v>1</v>
+      </c>
+      <c r="F27" s="153"/>
+      <c r="G27" s="250">
+        <f>K9</f>
+        <v>2250</v>
+      </c>
+      <c r="H27" s="250">
+        <f>G27*E27</f>
+        <v>2250</v>
+      </c>
+      <c r="I27" s="153"/>
+      <c r="J27" s="250">
+        <f>Y10*Z10*S12</f>
+        <v>67500</v>
+      </c>
+      <c r="K27" s="250"/>
+      <c r="L27" s="153"/>
+      <c r="M27" s="250">
+        <f>M10</f>
+        <v>8.75</v>
+      </c>
+      <c r="N27" s="250"/>
+      <c r="R27" s="234"/>
+      <c r="S27" s="235"/>
+      <c r="T27" s="235"/>
+      <c r="U27" s="151"/>
+      <c r="V27" s="151"/>
+      <c r="W27" s="151"/>
+      <c r="X27" s="151"/>
+      <c r="Y27" s="151"/>
+      <c r="Z27" s="151"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" s="149"/>
+      <c r="B28" s="230"/>
+      <c r="C28" s="148" t="s">
+        <v>413</v>
+      </c>
+      <c r="D28" s="149"/>
+      <c r="E28" s="152">
+        <v>1</v>
+      </c>
+      <c r="F28" s="153"/>
+      <c r="G28" s="250">
+        <f>Y10*Z10*S20</f>
+        <v>22500</v>
+      </c>
+      <c r="H28" s="254">
+        <f>G28*E28</f>
+        <v>22500</v>
+      </c>
+      <c r="I28" s="153"/>
+      <c r="J28" s="250"/>
+      <c r="K28" s="250"/>
+      <c r="L28" s="153"/>
+      <c r="M28" s="250">
+        <f>S20</f>
+        <v>100</v>
+      </c>
+      <c r="N28" s="250"/>
+      <c r="R28" s="234"/>
+      <c r="S28" s="235"/>
+      <c r="T28" s="235"/>
+      <c r="U28" s="151"/>
+      <c r="V28" s="151"/>
+      <c r="W28" s="151"/>
+      <c r="X28" s="151"/>
+      <c r="Y28" s="151"/>
+      <c r="Z28" s="151"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A29" s="149"/>
+      <c r="B29" s="230"/>
+      <c r="C29" s="149"/>
+      <c r="D29" s="149"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="153"/>
+      <c r="G29" s="250"/>
+      <c r="H29" s="250">
+        <f>H28+H27</f>
+        <v>24750</v>
+      </c>
+      <c r="I29" s="153"/>
+      <c r="J29" s="250"/>
+      <c r="K29" s="250"/>
+      <c r="L29" s="153"/>
+      <c r="M29" s="254">
+        <f>S12</f>
+        <v>300</v>
+      </c>
+      <c r="N29" s="254"/>
+      <c r="R29" s="234"/>
+      <c r="S29" s="235"/>
+      <c r="T29" s="235"/>
+      <c r="U29" s="151"/>
+      <c r="V29" s="151"/>
+      <c r="W29" s="151"/>
+      <c r="X29" s="151"/>
+      <c r="Y29" s="151"/>
+      <c r="Z29" s="151"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A30" s="149"/>
+      <c r="B30" s="230"/>
+      <c r="C30" s="149"/>
+      <c r="D30" s="149"/>
+      <c r="E30" s="152"/>
+      <c r="F30" s="153"/>
+      <c r="G30" s="250"/>
+      <c r="H30" s="250"/>
+      <c r="I30" s="153"/>
+      <c r="J30" s="250"/>
+      <c r="K30" s="255">
+        <f>H29+J27</f>
+        <v>92250</v>
+      </c>
+      <c r="L30" s="153"/>
+      <c r="M30" s="250">
+        <f>M29+M28+M27</f>
+        <v>408.75</v>
+      </c>
+      <c r="N30" s="250">
+        <f>M30/60</f>
+        <v>6.8125</v>
+      </c>
+      <c r="O30" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="R30" s="235"/>
+      <c r="S30" s="235"/>
+      <c r="T30" s="235"/>
+      <c r="U30" s="151"/>
+      <c r="V30" s="151"/>
+      <c r="W30" s="151"/>
+      <c r="X30" s="151"/>
+      <c r="Y30" s="151"/>
+      <c r="Z30" s="151"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A31" s="149"/>
+      <c r="B31" s="230"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="149"/>
+      <c r="E31" s="152"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="250"/>
+      <c r="H31" s="250"/>
+      <c r="I31" s="153"/>
+      <c r="J31" s="250"/>
+      <c r="K31" s="250"/>
+      <c r="L31" s="153"/>
+      <c r="M31" s="250"/>
+      <c r="N31" s="250"/>
+      <c r="R31" s="234"/>
+      <c r="S31" s="234"/>
+      <c r="T31" s="235"/>
+      <c r="U31" s="151"/>
+      <c r="V31" s="151"/>
+      <c r="W31" s="151"/>
+      <c r="X31" s="151"/>
+      <c r="Y31" s="151"/>
+      <c r="Z31" s="151"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A32" s="148" t="s">
+        <v>409</v>
+      </c>
+      <c r="B32" s="230"/>
+      <c r="C32" s="148" t="s">
+        <v>401</v>
+      </c>
+      <c r="D32" s="149"/>
+      <c r="E32" s="152">
+        <v>1</v>
+      </c>
+      <c r="F32" s="153"/>
+      <c r="G32" s="250">
+        <f>K9</f>
+        <v>2250</v>
+      </c>
+      <c r="H32" s="250">
+        <f>G32*E32</f>
+        <v>2250</v>
+      </c>
+      <c r="I32" s="153"/>
+      <c r="J32" s="250">
+        <f>Y10*Z10*S13</f>
+        <v>81000</v>
+      </c>
+      <c r="K32" s="250"/>
+      <c r="L32" s="153"/>
+      <c r="M32" s="250">
+        <f>M10</f>
+        <v>8.75</v>
+      </c>
+      <c r="N32" s="250"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="149"/>
+      <c r="B33" s="230"/>
+      <c r="C33" s="148" t="s">
+        <v>414</v>
+      </c>
+      <c r="D33" s="149"/>
+      <c r="E33" s="152">
+        <v>1</v>
+      </c>
+      <c r="F33" s="153"/>
+      <c r="G33" s="250">
+        <f>Y10*Z10*S21</f>
+        <v>31500</v>
+      </c>
+      <c r="H33" s="254">
+        <f>G33*E33</f>
+        <v>31500</v>
+      </c>
+      <c r="I33" s="153"/>
+      <c r="J33" s="250"/>
+      <c r="K33" s="250"/>
+      <c r="L33" s="153"/>
+      <c r="M33" s="250">
+        <f>S21</f>
+        <v>140</v>
+      </c>
+      <c r="N33" s="250"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="149"/>
+      <c r="B34" s="230"/>
+      <c r="C34" s="149"/>
+      <c r="D34" s="149"/>
+      <c r="E34" s="152"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="250"/>
+      <c r="H34" s="250">
+        <f>H33+H32</f>
+        <v>33750</v>
+      </c>
+      <c r="I34" s="153"/>
+      <c r="J34" s="250"/>
+      <c r="K34" s="250"/>
+      <c r="L34" s="153"/>
+      <c r="M34" s="254">
+        <f>S13</f>
+        <v>360</v>
+      </c>
+      <c r="N34" s="254"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="149"/>
+      <c r="B35" s="230"/>
+      <c r="C35" s="149"/>
+      <c r="D35" s="149"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="153"/>
+      <c r="G35" s="250"/>
+      <c r="H35" s="250"/>
+      <c r="I35" s="153"/>
+      <c r="J35" s="250"/>
+      <c r="K35" s="255">
+        <f>J32+H34</f>
+        <v>114750</v>
+      </c>
+      <c r="L35" s="153"/>
+      <c r="M35" s="250">
+        <f>M34+M33+M32</f>
+        <v>508.75</v>
+      </c>
+      <c r="N35" s="250">
+        <f>M35/60</f>
+        <v>8.4791666666666661</v>
+      </c>
+      <c r="O35" s="119" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="149"/>
+      <c r="B36" s="230"/>
+      <c r="C36" s="149"/>
+      <c r="D36" s="149"/>
+      <c r="E36" s="152"/>
+      <c r="F36" s="153"/>
+      <c r="G36" s="250"/>
+      <c r="H36" s="250"/>
+      <c r="I36" s="153"/>
+      <c r="J36" s="250"/>
+      <c r="K36" s="250"/>
+      <c r="L36" s="153"/>
+      <c r="M36" s="250"/>
+      <c r="N36" s="250"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="149"/>
+      <c r="B37" s="230"/>
+      <c r="C37" s="149"/>
+      <c r="D37" s="149"/>
+      <c r="E37" s="152"/>
+      <c r="F37" s="153"/>
+      <c r="G37" s="250"/>
+      <c r="H37" s="250"/>
+      <c r="I37" s="153"/>
+      <c r="J37" s="250"/>
+      <c r="K37" s="250"/>
+      <c r="L37" s="153"/>
+      <c r="M37" s="250"/>
+      <c r="N37" s="250"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="149"/>
+      <c r="B38" s="230"/>
+      <c r="C38" s="149"/>
+      <c r="D38" s="149"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="153"/>
+      <c r="G38" s="250"/>
+      <c r="H38" s="250"/>
+      <c r="I38" s="153"/>
+      <c r="J38" s="250"/>
+      <c r="K38" s="250"/>
+      <c r="L38" s="153"/>
+      <c r="M38" s="250"/>
+      <c r="N38" s="250"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="235"/>
+      <c r="B39" s="235"/>
+      <c r="C39" s="235"/>
+      <c r="D39" s="235"/>
+      <c r="E39" s="235"/>
+      <c r="F39" s="235"/>
+      <c r="G39" s="256"/>
+      <c r="H39" s="256"/>
+      <c r="I39" s="235"/>
+      <c r="J39" s="256"/>
+      <c r="K39" s="256"/>
+      <c r="L39" s="235"/>
+      <c r="M39" s="256"/>
+      <c r="N39" s="256"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="235"/>
+      <c r="B40" s="235"/>
+      <c r="C40" s="235"/>
+      <c r="D40" s="235"/>
+      <c r="E40" s="235"/>
+      <c r="F40" s="235"/>
+      <c r="G40" s="256"/>
+      <c r="H40" s="256"/>
+      <c r="I40" s="235"/>
+      <c r="J40" s="256"/>
+      <c r="K40" s="256"/>
+      <c r="L40" s="235"/>
+      <c r="M40" s="256"/>
+      <c r="N40" s="256"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="235"/>
+      <c r="B41" s="235"/>
+      <c r="C41" s="235"/>
+      <c r="D41" s="235"/>
+      <c r="E41" s="235"/>
+      <c r="F41" s="235"/>
+      <c r="G41" s="256"/>
+      <c r="H41" s="256"/>
+      <c r="I41" s="235"/>
+      <c r="J41" s="256"/>
+      <c r="K41" s="256"/>
+      <c r="L41" s="235"/>
+      <c r="M41" s="256"/>
+      <c r="N41" s="256"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="235"/>
+      <c r="B42" s="235"/>
+      <c r="C42" s="235"/>
+      <c r="D42" s="235"/>
+      <c r="E42" s="235"/>
+      <c r="F42" s="235"/>
+      <c r="G42" s="256"/>
+      <c r="H42" s="256"/>
+      <c r="I42" s="235"/>
+      <c r="J42" s="256"/>
+      <c r="K42" s="256"/>
+      <c r="L42" s="235"/>
+      <c r="M42" s="256"/>
+      <c r="N42" s="256"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="235"/>
+      <c r="B43" s="235"/>
+      <c r="C43" s="235"/>
+      <c r="D43" s="235"/>
+      <c r="E43" s="235"/>
+      <c r="F43" s="235"/>
+      <c r="G43" s="256"/>
+      <c r="H43" s="256"/>
+      <c r="I43" s="235"/>
+      <c r="J43" s="256"/>
+      <c r="K43" s="256"/>
+      <c r="L43" s="235"/>
+      <c r="M43" s="256"/>
+      <c r="N43" s="256"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="235"/>
+      <c r="B44" s="235"/>
+      <c r="C44" s="235"/>
+      <c r="D44" s="235"/>
+      <c r="E44" s="235"/>
+      <c r="F44" s="235"/>
+      <c r="G44" s="256"/>
+      <c r="H44" s="256"/>
+      <c r="I44" s="235"/>
+      <c r="J44" s="256"/>
+      <c r="K44" s="256"/>
+      <c r="L44" s="235"/>
+      <c r="M44" s="256"/>
+      <c r="N44" s="256"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="235"/>
+      <c r="B45" s="235"/>
+      <c r="C45" s="235"/>
+      <c r="D45" s="235"/>
+      <c r="E45" s="235"/>
+      <c r="F45" s="235"/>
+      <c r="G45" s="256"/>
+      <c r="H45" s="256"/>
+      <c r="I45" s="235"/>
+      <c r="J45" s="256"/>
+      <c r="K45" s="256"/>
+      <c r="L45" s="235"/>
+      <c r="M45" s="256"/>
+      <c r="N45" s="256"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="235"/>
+      <c r="B46" s="235"/>
+      <c r="C46" s="235"/>
+      <c r="D46" s="235"/>
+      <c r="E46" s="235"/>
+      <c r="F46" s="235"/>
+      <c r="G46" s="256"/>
+      <c r="H46" s="256"/>
+      <c r="I46" s="235"/>
+      <c r="J46" s="256"/>
+      <c r="K46" s="256"/>
+      <c r="L46" s="235"/>
+      <c r="M46" s="256"/>
+      <c r="N46" s="256"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="235"/>
+      <c r="B47" s="235"/>
+      <c r="C47" s="235"/>
+      <c r="D47" s="235"/>
+      <c r="E47" s="235"/>
+      <c r="F47" s="235"/>
+      <c r="G47" s="256"/>
+      <c r="H47" s="256"/>
+      <c r="I47" s="235"/>
+      <c r="J47" s="256"/>
+      <c r="K47" s="256"/>
+      <c r="L47" s="235"/>
+      <c r="M47" s="256"/>
+      <c r="N47" s="256"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="235"/>
+      <c r="B48" s="235"/>
+      <c r="C48" s="235"/>
+      <c r="D48" s="235"/>
+      <c r="E48" s="235"/>
+      <c r="F48" s="235"/>
+      <c r="G48" s="256"/>
+      <c r="H48" s="256"/>
+      <c r="I48" s="235"/>
+      <c r="J48" s="256"/>
+      <c r="K48" s="256"/>
+      <c r="L48" s="235"/>
+      <c r="M48" s="256"/>
+      <c r="N48" s="256"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="235"/>
+      <c r="B49" s="235"/>
+      <c r="C49" s="235"/>
+      <c r="D49" s="235"/>
+      <c r="E49" s="235"/>
+      <c r="F49" s="235"/>
+      <c r="G49" s="256"/>
+      <c r="H49" s="256"/>
+      <c r="I49" s="235"/>
+      <c r="J49" s="256"/>
+      <c r="K49" s="256"/>
+      <c r="L49" s="235"/>
+      <c r="M49" s="256"/>
+      <c r="N49" s="256"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="235"/>
+      <c r="B50" s="235"/>
+      <c r="C50" s="235"/>
+      <c r="D50" s="235"/>
+      <c r="E50" s="235"/>
+      <c r="F50" s="235"/>
+      <c r="G50" s="256"/>
+      <c r="H50" s="256"/>
+      <c r="I50" s="235"/>
+      <c r="J50" s="256"/>
+      <c r="K50" s="256"/>
+      <c r="L50" s="235"/>
+      <c r="M50" s="256"/>
+      <c r="N50" s="256"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="235"/>
+      <c r="B51" s="235"/>
+      <c r="C51" s="235"/>
+      <c r="D51" s="235"/>
+      <c r="E51" s="235"/>
+      <c r="F51" s="235"/>
+      <c r="G51" s="256"/>
+      <c r="H51" s="256"/>
+      <c r="I51" s="235"/>
+      <c r="J51" s="256"/>
+      <c r="K51" s="256"/>
+      <c r="L51" s="235"/>
+      <c r="M51" s="256"/>
+      <c r="N51" s="256"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="235"/>
+      <c r="B52" s="235"/>
+      <c r="C52" s="235"/>
+      <c r="D52" s="235"/>
+      <c r="E52" s="235"/>
+      <c r="F52" s="235"/>
+      <c r="G52" s="256"/>
+      <c r="H52" s="256"/>
+      <c r="I52" s="235"/>
+      <c r="J52" s="256"/>
+      <c r="K52" s="256"/>
+      <c r="L52" s="235"/>
+      <c r="M52" s="256"/>
+      <c r="N52" s="256"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C9">
-    <cfRule type="iconSet" priority="1">
-      <iconSet iconSet="3Arrows">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
+  <mergeCells count="2">
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="R6:S6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11755,7 +13344,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11779,11 +13368,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="215"/>
-      <c r="B1" s="215"/>
+      <c r="A1" s="209"/>
+      <c r="B1" s="209"/>
       <c r="C1" s="186"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
       <c r="F1" s="186"/>
       <c r="G1" s="186"/>
       <c r="H1" s="186"/>
@@ -11795,20 +13384,20 @@
       <c r="N1" s="186"/>
       <c r="O1" s="186"/>
       <c r="P1" s="186"/>
-      <c r="Q1" s="215"/>
+      <c r="Q1" s="209"/>
     </row>
     <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="186"/>
-      <c r="B2" s="214" t="s">
+      <c r="B2" s="208" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="186"/>
       <c r="D2" s="186"/>
-      <c r="E2" s="223" t="s">
+      <c r="E2" s="217" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="186"/>
-      <c r="G2" s="224" t="s">
+      <c r="G2" s="218" t="s">
         <v>45</v>
       </c>
       <c r="H2" s="186"/>
@@ -11824,10 +13413,10 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="186"/>
-      <c r="B3" s="215"/>
+      <c r="B3" s="209"/>
       <c r="C3" s="186"/>
       <c r="D3" s="186"/>
-      <c r="E3" s="215"/>
+      <c r="E3" s="209"/>
       <c r="F3" s="186"/>
       <c r="G3" s="186"/>
       <c r="H3" s="186"/>
@@ -11843,10 +13432,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="186"/>
-      <c r="B4" s="216"/>
+      <c r="B4" s="210"/>
       <c r="C4" s="186"/>
       <c r="D4" s="186"/>
-      <c r="E4" s="222" t="s">
+      <c r="E4" s="216" t="s">
         <v>103</v>
       </c>
       <c r="F4" s="186"/>
@@ -11952,10 +13541,10 @@
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="186"/>
-      <c r="B7" s="217"/>
+      <c r="B7" s="211"/>
       <c r="C7" s="186"/>
       <c r="D7" s="186"/>
-      <c r="E7" s="215"/>
+      <c r="E7" s="209"/>
       <c r="F7" s="186"/>
       <c r="G7" s="186"/>
       <c r="H7" s="186"/>
@@ -11971,12 +13560,12 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="186"/>
-      <c r="B8" s="216" t="s">
+      <c r="B8" s="210" t="s">
         <v>122</v>
       </c>
       <c r="C8" s="186"/>
       <c r="D8" s="186"/>
-      <c r="E8" s="218" t="s">
+      <c r="E8" s="212" t="s">
         <v>123</v>
       </c>
       <c r="F8" s="186"/>
@@ -12328,10 +13917,10 @@
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="186"/>
-      <c r="B16" s="217"/>
+      <c r="B16" s="211"/>
       <c r="C16" s="186"/>
       <c r="D16" s="186"/>
-      <c r="E16" s="215"/>
+      <c r="E16" s="209"/>
       <c r="F16" s="186"/>
       <c r="G16" s="186"/>
       <c r="H16" s="186"/>
@@ -12347,12 +13936,12 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="186"/>
-      <c r="B17" s="216" t="s">
+      <c r="B17" s="210" t="s">
         <v>182</v>
       </c>
       <c r="C17" s="186"/>
       <c r="D17" s="186"/>
-      <c r="E17" s="220" t="s">
+      <c r="E17" s="214" t="s">
         <v>183</v>
       </c>
       <c r="F17" s="186"/>
@@ -12669,10 +14258,10 @@
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="186"/>
-      <c r="B25" s="217"/>
+      <c r="B25" s="211"/>
       <c r="C25" s="186"/>
       <c r="D25" s="186"/>
-      <c r="E25" s="215"/>
+      <c r="E25" s="209"/>
       <c r="F25" s="186"/>
       <c r="G25" s="186"/>
       <c r="H25" s="186"/>
@@ -12688,12 +14277,12 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="186"/>
-      <c r="B26" s="216" t="s">
+      <c r="B26" s="210" t="s">
         <v>216</v>
       </c>
       <c r="C26" s="186"/>
       <c r="D26" s="186"/>
-      <c r="E26" s="221" t="s">
+      <c r="E26" s="215" t="s">
         <v>217</v>
       </c>
       <c r="F26" s="186"/>
@@ -12992,10 +14581,10 @@
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="186"/>
-      <c r="B34" s="217"/>
+      <c r="B34" s="211"/>
       <c r="C34" s="186"/>
       <c r="D34" s="186"/>
-      <c r="E34" s="215"/>
+      <c r="E34" s="209"/>
       <c r="F34" s="186"/>
       <c r="G34" s="186"/>
       <c r="H34" s="186"/>
@@ -13011,12 +14600,12 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="186"/>
-      <c r="B35" s="216" t="s">
+      <c r="B35" s="210" t="s">
         <v>246</v>
       </c>
       <c r="C35" s="186"/>
       <c r="D35" s="186"/>
-      <c r="E35" s="219" t="s">
+      <c r="E35" s="213" t="s">
         <v>247</v>
       </c>
       <c r="F35" s="186"/>
@@ -13464,7 +15053,7 @@
   <dimension ref="A4:P42"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="L12" sqref="L12:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13484,133 +15073,133 @@
   <sheetData>
     <row r="4" spans="8:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="H4" s="183" t="s">
+        <v>364</v>
+      </c>
+      <c r="I4" s="119" t="s">
         <v>365</v>
-      </c>
-      <c r="I4" s="119" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="5" spans="8:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="H5" s="183" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I5" s="119" t="s">
+        <v>366</v>
+      </c>
+      <c r="J5" s="119" t="s">
         <v>367</v>
       </c>
-      <c r="J5" s="119" t="s">
+      <c r="K5" s="119" t="s">
         <v>368</v>
       </c>
-      <c r="K5" s="119" t="s">
+      <c r="L5" s="119" t="s">
         <v>369</v>
       </c>
-      <c r="L5" s="119" t="s">
+      <c r="M5" s="119" t="s">
         <v>370</v>
-      </c>
-      <c r="M5" s="119" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="6" spans="8:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="H6" s="183" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I6" s="119" t="s">
+        <v>372</v>
+      </c>
+      <c r="J6" s="119" t="s">
         <v>373</v>
       </c>
-      <c r="J6" s="119" t="s">
+      <c r="K6" s="119" t="s">
         <v>374</v>
       </c>
-      <c r="K6" s="119" t="s">
+      <c r="L6" s="119" t="s">
         <v>375</v>
       </c>
-      <c r="L6" s="119" t="s">
+      <c r="M6" s="119" t="s">
         <v>376</v>
-      </c>
-      <c r="M6" s="119" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="7" spans="8:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="H7" s="183" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I7" s="119" t="s">
+        <v>377</v>
+      </c>
+      <c r="J7" s="119" t="s">
         <v>378</v>
       </c>
-      <c r="J7" s="119" t="s">
+      <c r="K7" s="119" t="s">
         <v>379</v>
       </c>
-      <c r="K7" s="119" t="s">
+      <c r="L7" s="119" t="s">
         <v>380</v>
       </c>
-      <c r="L7" s="119" t="s">
+      <c r="M7" s="119" t="s">
         <v>381</v>
-      </c>
-      <c r="M7" s="119" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="10" spans="8:16" x14ac:dyDescent="0.2">
       <c r="I10" s="178" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K10" s="178" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M10" s="178" t="s">
+        <v>382</v>
+      </c>
+      <c r="O10" s="119" t="s">
         <v>383</v>
-      </c>
-      <c r="O10" s="119" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="11" spans="8:16" x14ac:dyDescent="0.2">
       <c r="I11" s="184" t="s">
+        <v>384</v>
+      </c>
+      <c r="J11" s="184" t="s">
         <v>385</v>
       </c>
-      <c r="J11" s="184" t="s">
-        <v>386</v>
-      </c>
       <c r="K11" s="184" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L11" s="184" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="M11" s="184" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="N11" s="184" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="O11" s="184" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P11" s="184" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="8:16" x14ac:dyDescent="0.2">
       <c r="I12" s="178" t="s">
+        <v>365</v>
+      </c>
+      <c r="J12" s="119" t="s">
+        <v>386</v>
+      </c>
+      <c r="K12" s="178" t="s">
         <v>366</v>
-      </c>
-      <c r="J12" s="119" t="s">
-        <v>387</v>
-      </c>
-      <c r="K12" s="178" t="s">
-        <v>367</v>
       </c>
       <c r="L12" s="143">
         <v>20</v>
       </c>
       <c r="M12" s="178" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N12" s="143">
         <v>32</v>
       </c>
       <c r="O12" s="178" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="P12" s="143">
         <v>58</v>
@@ -13618,19 +15207,19 @@
     </row>
     <row r="13" spans="8:16" x14ac:dyDescent="0.2">
       <c r="K13" s="178" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L13" s="143">
         <v>35</v>
       </c>
       <c r="M13" s="178" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N13" s="143">
         <v>56</v>
       </c>
       <c r="O13" s="178" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="P13" s="143">
         <v>101</v>
@@ -13638,19 +15227,19 @@
     </row>
     <row r="14" spans="8:16" x14ac:dyDescent="0.2">
       <c r="K14" s="178" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L14" s="143">
         <v>60</v>
       </c>
       <c r="M14" s="119" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N14" s="143">
         <v>96</v>
       </c>
       <c r="O14" s="178" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="P14" s="143">
         <v>173</v>
@@ -13658,19 +15247,19 @@
     </row>
     <row r="15" spans="8:16" x14ac:dyDescent="0.2">
       <c r="K15" s="178" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L15" s="143">
         <v>100</v>
       </c>
       <c r="M15" s="178" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N15" s="143">
         <v>160</v>
       </c>
       <c r="O15" s="178" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="P15" s="143">
         <v>288</v>
@@ -13678,19 +15267,19 @@
     </row>
     <row r="16" spans="8:16" x14ac:dyDescent="0.2">
       <c r="K16" s="178" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L16" s="143">
         <v>140</v>
       </c>
       <c r="M16" s="178" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N16" s="143">
         <v>224</v>
       </c>
       <c r="O16" s="178" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="P16" s="143">
         <v>403</v>
@@ -13811,7 +15400,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
balance sheet work done
</commit_message>
<xml_diff>
--- a/0 DyTech Informations/Dytech Balance.xlsx
+++ b/0 DyTech Informations/Dytech Balance.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\.FactorioModding\DyTech-master\0 DyTech Informations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\.Dytech\DyTech\0 DyTech Informations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135" tabRatio="781" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135" tabRatio="781" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Energy used by the chemical processor to create the fuel stated in colum A</t>
+Energy used by the chemical processor to create the item stated in colum A</t>
         </r>
       </text>
     </comment>
@@ -1026,7 +1026,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="466">
   <si>
     <t>README</t>
   </si>
@@ -2405,9 +2405,6 @@
     <t>Copper Cable</t>
   </si>
   <si>
-    <t>Furnace used is electronic Furnace.</t>
-  </si>
-  <si>
     <t>leeg</t>
   </si>
   <si>
@@ -2418,6 +2415,15 @@
   </si>
   <si>
     <t>Copper ore</t>
+  </si>
+  <si>
+    <t>Furnace used is an electronic Furnace.</t>
+  </si>
+  <si>
+    <t>Electric Furnace</t>
+  </si>
+  <si>
+    <t>(2 speed)</t>
   </si>
 </sst>
 </file>
@@ -2915,7 +2921,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -3115,6 +3121,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3125,7 +3140,7 @@
     <xf numFmtId="0" fontId="14" fillId="53" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="54" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="279">
+  <cellXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3407,7 +3422,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="55" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1"/>
@@ -3464,9 +3478,6 @@
     <xf numFmtId="0" fontId="14" fillId="36" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="49" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3474,9 +3485,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="49" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="49" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3489,6 +3497,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3545,6 +3559,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="47" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="47" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -5884,68 +5907,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="238"/>
-      <c r="B1" s="235" t="s">
+      <c r="A1" s="237"/>
+      <c r="B1" s="234" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="227"/>
-      <c r="D1" s="235" t="s">
+      <c r="C1" s="226"/>
+      <c r="D1" s="234" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="227"/>
-      <c r="F1" s="227"/>
-      <c r="G1" s="227"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="235" t="s">
+      <c r="M1" s="234" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="227"/>
-      <c r="O1" s="227"/>
-      <c r="P1" s="227"/>
-      <c r="Q1" s="238"/>
+      <c r="N1" s="226"/>
+      <c r="O1" s="226"/>
+      <c r="P1" s="226"/>
+      <c r="Q1" s="237"/>
       <c r="U1" s="9"/>
-      <c r="V1" s="233"/>
-      <c r="W1" s="227"/>
-      <c r="X1" s="227"/>
+      <c r="V1" s="232"/>
+      <c r="W1" s="226"/>
+      <c r="X1" s="226"/>
     </row>
     <row r="2" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="227"/>
-      <c r="B2" s="229" t="s">
+      <c r="A2" s="226"/>
+      <c r="B2" s="228" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="227"/>
-      <c r="D2" s="234" t="s">
+      <c r="C2" s="226"/>
+      <c r="D2" s="233" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="227"/>
-      <c r="F2" s="227"/>
-      <c r="G2" s="227"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
-      <c r="L2" s="236"/>
-      <c r="M2" s="234" t="s">
+      <c r="L2" s="235"/>
+      <c r="M2" s="233" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="227"/>
-      <c r="O2" s="227"/>
-      <c r="P2" s="227"/>
-      <c r="Q2" s="227"/>
+      <c r="N2" s="226"/>
+      <c r="O2" s="226"/>
+      <c r="P2" s="226"/>
+      <c r="Q2" s="226"/>
       <c r="R2" s="13"/>
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="226"/>
-      <c r="W2" s="227"/>
-      <c r="X2" s="227"/>
+      <c r="V2" s="225"/>
+      <c r="W2" s="226"/>
+      <c r="X2" s="226"/>
     </row>
     <row r="3" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="227"/>
+      <c r="A3" s="226"/>
       <c r="B3" s="18" t="s">
         <v>23</v>
       </c>
@@ -5968,7 +5991,7 @@
       <c r="I3" s="26"/>
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
-      <c r="L3" s="227"/>
+      <c r="L3" s="226"/>
       <c r="M3" s="24" t="s">
         <v>82</v>
       </c>
@@ -5979,7 +6002,7 @@
         <v>84</v>
       </c>
       <c r="P3" s="24"/>
-      <c r="Q3" s="227"/>
+      <c r="Q3" s="226"/>
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
@@ -5989,7 +6012,7 @@
       <c r="X3" s="27"/>
     </row>
     <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="227"/>
+      <c r="A4" s="226"/>
       <c r="B4" s="18" t="s">
         <v>101</v>
       </c>
@@ -6011,7 +6034,7 @@
       <c r="I4" s="36"/>
       <c r="J4" s="36"/>
       <c r="K4" s="36"/>
-      <c r="L4" s="227"/>
+      <c r="L4" s="226"/>
       <c r="M4" s="29">
         <v>1</v>
       </c>
@@ -6022,7 +6045,7 @@
         <v>0.1</v>
       </c>
       <c r="P4" s="42"/>
-      <c r="Q4" s="227"/>
+      <c r="Q4" s="226"/>
       <c r="R4" s="43"/>
       <c r="S4" s="39"/>
       <c r="U4" s="43"/>
@@ -6031,7 +6054,7 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="227"/>
+      <c r="A5" s="226"/>
       <c r="B5" s="18" t="s">
         <v>108</v>
       </c>
@@ -6057,7 +6080,7 @@
       <c r="I5" s="36"/>
       <c r="J5" s="36"/>
       <c r="K5" s="36"/>
-      <c r="L5" s="227"/>
+      <c r="L5" s="226"/>
       <c r="M5" s="29">
         <v>2</v>
       </c>
@@ -6068,7 +6091,7 @@
         <v>0.2</v>
       </c>
       <c r="P5" s="42"/>
-      <c r="Q5" s="227"/>
+      <c r="Q5" s="226"/>
       <c r="R5" s="43"/>
       <c r="S5" s="39"/>
       <c r="T5" s="10"/>
@@ -6078,7 +6101,7 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="227"/>
+      <c r="A6" s="226"/>
       <c r="B6" s="14"/>
       <c r="C6" s="45"/>
       <c r="D6" s="29">
@@ -6102,7 +6125,7 @@
       <c r="I6" s="36"/>
       <c r="J6" s="36"/>
       <c r="K6" s="36"/>
-      <c r="L6" s="227"/>
+      <c r="L6" s="226"/>
       <c r="M6" s="29">
         <v>3</v>
       </c>
@@ -6113,7 +6136,7 @@
         <v>0.3</v>
       </c>
       <c r="P6" s="42"/>
-      <c r="Q6" s="227"/>
+      <c r="Q6" s="226"/>
       <c r="R6" s="43"/>
       <c r="S6" s="39"/>
       <c r="U6" s="43"/>
@@ -6122,7 +6145,7 @@
       <c r="X6" s="10"/>
     </row>
     <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="227"/>
+      <c r="A7" s="226"/>
       <c r="B7" s="14"/>
       <c r="C7" s="45"/>
       <c r="D7" s="29">
@@ -6144,7 +6167,7 @@
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
       <c r="K7" s="36"/>
-      <c r="L7" s="227"/>
+      <c r="L7" s="226"/>
       <c r="M7" s="29">
         <v>4</v>
       </c>
@@ -6155,14 +6178,14 @@
         <v>0.4</v>
       </c>
       <c r="P7" s="42"/>
-      <c r="Q7" s="227"/>
+      <c r="Q7" s="226"/>
       <c r="R7" s="43"/>
       <c r="S7" s="39"/>
       <c r="U7" s="43"/>
       <c r="V7" s="43"/>
     </row>
     <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="227"/>
+      <c r="A8" s="226"/>
       <c r="B8" s="14"/>
       <c r="C8" s="45"/>
       <c r="D8" s="29">
@@ -6186,7 +6209,7 @@
       <c r="I8" s="36"/>
       <c r="J8" s="36"/>
       <c r="K8" s="36"/>
-      <c r="L8" s="227"/>
+      <c r="L8" s="226"/>
       <c r="M8" s="29">
         <v>5</v>
       </c>
@@ -6197,14 +6220,14 @@
         <v>0.5</v>
       </c>
       <c r="P8" s="42"/>
-      <c r="Q8" s="227"/>
+      <c r="Q8" s="226"/>
       <c r="R8" s="43"/>
       <c r="S8" s="39"/>
       <c r="U8" s="43"/>
       <c r="V8" s="43"/>
     </row>
     <row r="9" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="227"/>
+      <c r="A9" s="226"/>
       <c r="B9" s="14"/>
       <c r="C9" s="45"/>
       <c r="D9" s="29">
@@ -6226,7 +6249,7 @@
       <c r="I9" s="36"/>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
-      <c r="L9" s="227"/>
+      <c r="L9" s="226"/>
       <c r="M9" s="29">
         <v>6</v>
       </c>
@@ -6237,14 +6260,14 @@
         <v>0.6</v>
       </c>
       <c r="P9" s="42"/>
-      <c r="Q9" s="227"/>
+      <c r="Q9" s="226"/>
       <c r="R9" s="43"/>
       <c r="S9" s="39"/>
       <c r="U9" s="43"/>
       <c r="V9" s="43"/>
     </row>
     <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="227"/>
+      <c r="A10" s="226"/>
       <c r="B10" s="14"/>
       <c r="C10" s="45"/>
       <c r="D10" s="29">
@@ -6268,7 +6291,7 @@
       <c r="I10" s="36"/>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
-      <c r="L10" s="227"/>
+      <c r="L10" s="226"/>
       <c r="M10" s="29">
         <v>7</v>
       </c>
@@ -6279,14 +6302,14 @@
         <v>0.7</v>
       </c>
       <c r="P10" s="42"/>
-      <c r="Q10" s="227"/>
+      <c r="Q10" s="226"/>
       <c r="R10" s="43"/>
       <c r="S10" s="39"/>
       <c r="U10" s="43"/>
       <c r="V10" s="43"/>
     </row>
     <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="227"/>
+      <c r="A11" s="226"/>
       <c r="B11" s="14"/>
       <c r="C11" s="45"/>
       <c r="D11" s="29">
@@ -6310,7 +6333,7 @@
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
-      <c r="L11" s="227"/>
+      <c r="L11" s="226"/>
       <c r="M11" s="29">
         <v>8</v>
       </c>
@@ -6321,30 +6344,30 @@
         <v>0.8</v>
       </c>
       <c r="P11" s="42"/>
-      <c r="Q11" s="227"/>
+      <c r="Q11" s="226"/>
       <c r="R11" s="43"/>
       <c r="S11" s="39"/>
       <c r="U11" s="43"/>
       <c r="V11" s="43"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="227"/>
-      <c r="B12" s="230"/>
-      <c r="C12" s="227"/>
-      <c r="D12" s="231"/>
-      <c r="E12" s="227"/>
-      <c r="F12" s="227"/>
-      <c r="G12" s="227"/>
+      <c r="A12" s="226"/>
+      <c r="B12" s="229"/>
+      <c r="C12" s="226"/>
+      <c r="D12" s="230"/>
+      <c r="E12" s="226"/>
+      <c r="F12" s="226"/>
+      <c r="G12" s="226"/>
       <c r="H12" s="56"/>
       <c r="I12" s="56"/>
       <c r="J12" s="56"/>
       <c r="K12" s="56"/>
-      <c r="L12" s="227"/>
-      <c r="M12" s="231"/>
-      <c r="N12" s="227"/>
-      <c r="O12" s="227"/>
-      <c r="P12" s="227"/>
-      <c r="Q12" s="227"/>
+      <c r="L12" s="226"/>
+      <c r="M12" s="230"/>
+      <c r="N12" s="226"/>
+      <c r="O12" s="226"/>
+      <c r="P12" s="226"/>
+      <c r="Q12" s="226"/>
       <c r="R12" s="17"/>
       <c r="S12" s="17"/>
       <c r="T12" s="17"/>
@@ -6354,37 +6377,37 @@
       <c r="X12" s="17"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="227"/>
-      <c r="B13" s="229"/>
-      <c r="C13" s="227"/>
-      <c r="D13" s="232" t="s">
+      <c r="A13" s="226"/>
+      <c r="B13" s="228"/>
+      <c r="C13" s="226"/>
+      <c r="D13" s="231" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="227"/>
-      <c r="F13" s="227"/>
-      <c r="G13" s="227"/>
+      <c r="E13" s="226"/>
+      <c r="F13" s="226"/>
+      <c r="G13" s="226"/>
       <c r="H13" s="58"/>
       <c r="I13" s="58"/>
       <c r="J13" s="58"/>
       <c r="K13" s="58"/>
-      <c r="L13" s="227"/>
-      <c r="M13" s="232" t="s">
+      <c r="L13" s="226"/>
+      <c r="M13" s="231" t="s">
         <v>144</v>
       </c>
-      <c r="N13" s="227"/>
-      <c r="O13" s="227"/>
-      <c r="P13" s="227"/>
-      <c r="Q13" s="227"/>
+      <c r="N13" s="226"/>
+      <c r="O13" s="226"/>
+      <c r="P13" s="226"/>
+      <c r="Q13" s="226"/>
       <c r="R13" s="17"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
       <c r="U13" s="17"/>
-      <c r="V13" s="226"/>
-      <c r="W13" s="227"/>
-      <c r="X13" s="227"/>
+      <c r="V13" s="225"/>
+      <c r="W13" s="226"/>
+      <c r="X13" s="226"/>
     </row>
     <row r="14" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="227"/>
+      <c r="A14" s="226"/>
       <c r="B14" s="14"/>
       <c r="C14" s="45"/>
       <c r="D14" s="60" t="s">
@@ -6405,7 +6428,7 @@
       <c r="I14" s="60"/>
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
-      <c r="L14" s="227"/>
+      <c r="L14" s="226"/>
       <c r="M14" s="60" t="s">
         <v>151</v>
       </c>
@@ -6414,7 +6437,7 @@
       </c>
       <c r="O14" s="60"/>
       <c r="P14" s="60"/>
-      <c r="Q14" s="227"/>
+      <c r="Q14" s="226"/>
       <c r="R14" s="27"/>
       <c r="S14" s="27"/>
       <c r="T14" s="27"/>
@@ -6424,7 +6447,7 @@
       <c r="X14" s="27"/>
     </row>
     <row r="15" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="227"/>
+      <c r="A15" s="226"/>
       <c r="B15" s="14"/>
       <c r="C15" s="45"/>
       <c r="D15" s="62">
@@ -6444,7 +6467,7 @@
       <c r="I15" s="68"/>
       <c r="J15" s="68"/>
       <c r="K15" s="68"/>
-      <c r="L15" s="227"/>
+      <c r="L15" s="226"/>
       <c r="M15" s="62">
         <v>1</v>
       </c>
@@ -6453,7 +6476,7 @@
       </c>
       <c r="O15" s="65"/>
       <c r="P15" s="65"/>
-      <c r="Q15" s="227"/>
+      <c r="Q15" s="226"/>
       <c r="R15" s="43"/>
       <c r="S15" s="39"/>
       <c r="U15" s="43"/>
@@ -6461,7 +6484,7 @@
       <c r="W15" s="10"/>
     </row>
     <row r="16" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="227"/>
+      <c r="A16" s="226"/>
       <c r="B16" s="14"/>
       <c r="C16" s="45"/>
       <c r="D16" s="62">
@@ -6483,7 +6506,7 @@
       <c r="I16" s="68"/>
       <c r="J16" s="68"/>
       <c r="K16" s="68"/>
-      <c r="L16" s="227"/>
+      <c r="L16" s="226"/>
       <c r="M16" s="62">
         <v>2</v>
       </c>
@@ -6492,7 +6515,7 @@
       </c>
       <c r="O16" s="65"/>
       <c r="P16" s="65"/>
-      <c r="Q16" s="227"/>
+      <c r="Q16" s="226"/>
       <c r="R16" s="43"/>
       <c r="S16" s="39"/>
       <c r="U16" s="43"/>
@@ -6500,7 +6523,7 @@
       <c r="W16" s="10"/>
     </row>
     <row r="17" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="227"/>
+      <c r="A17" s="226"/>
       <c r="B17" s="14"/>
       <c r="C17" s="45"/>
       <c r="D17" s="62">
@@ -6524,7 +6547,7 @@
       <c r="I17" s="68"/>
       <c r="J17" s="68"/>
       <c r="K17" s="68"/>
-      <c r="L17" s="227"/>
+      <c r="L17" s="226"/>
       <c r="M17" s="62">
         <v>3</v>
       </c>
@@ -6533,7 +6556,7 @@
       </c>
       <c r="O17" s="65"/>
       <c r="P17" s="65"/>
-      <c r="Q17" s="227"/>
+      <c r="Q17" s="226"/>
       <c r="R17" s="43"/>
       <c r="S17" s="39"/>
       <c r="U17" s="43"/>
@@ -6541,7 +6564,7 @@
       <c r="W17" s="10"/>
     </row>
     <row r="18" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="227"/>
+      <c r="A18" s="226"/>
       <c r="B18" s="14"/>
       <c r="C18" s="45"/>
       <c r="D18" s="62">
@@ -6563,7 +6586,7 @@
       <c r="I18" s="68"/>
       <c r="J18" s="68"/>
       <c r="K18" s="68"/>
-      <c r="L18" s="227"/>
+      <c r="L18" s="226"/>
       <c r="M18" s="62">
         <v>4</v>
       </c>
@@ -6572,13 +6595,13 @@
       </c>
       <c r="O18" s="65"/>
       <c r="P18" s="65"/>
-      <c r="Q18" s="227"/>
+      <c r="Q18" s="226"/>
       <c r="R18" s="43"/>
       <c r="U18" s="43"/>
       <c r="V18" s="43"/>
     </row>
     <row r="19" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="227"/>
+      <c r="A19" s="226"/>
       <c r="B19" s="14"/>
       <c r="C19" s="45"/>
       <c r="D19" s="62">
@@ -6602,7 +6625,7 @@
       <c r="I19" s="68"/>
       <c r="J19" s="68"/>
       <c r="K19" s="68"/>
-      <c r="L19" s="227"/>
+      <c r="L19" s="226"/>
       <c r="M19" s="62">
         <v>5</v>
       </c>
@@ -6611,13 +6634,13 @@
       </c>
       <c r="O19" s="65"/>
       <c r="P19" s="65"/>
-      <c r="Q19" s="227"/>
+      <c r="Q19" s="226"/>
       <c r="R19" s="43"/>
       <c r="U19" s="43"/>
       <c r="V19" s="43"/>
     </row>
     <row r="20" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="227"/>
+      <c r="A20" s="226"/>
       <c r="B20" s="14"/>
       <c r="C20" s="45"/>
       <c r="D20" s="62">
@@ -6639,7 +6662,7 @@
       <c r="I20" s="68"/>
       <c r="J20" s="68"/>
       <c r="K20" s="68"/>
-      <c r="L20" s="227"/>
+      <c r="L20" s="226"/>
       <c r="M20" s="62">
         <v>6</v>
       </c>
@@ -6648,14 +6671,14 @@
       </c>
       <c r="O20" s="65"/>
       <c r="P20" s="65"/>
-      <c r="Q20" s="227"/>
+      <c r="Q20" s="226"/>
       <c r="R20" s="43"/>
       <c r="S20" s="39"/>
       <c r="U20" s="43"/>
       <c r="V20" s="43"/>
     </row>
     <row r="21" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="227"/>
+      <c r="A21" s="226"/>
       <c r="B21" s="14"/>
       <c r="C21" s="45"/>
       <c r="D21" s="62">
@@ -6679,7 +6702,7 @@
       <c r="I21" s="68"/>
       <c r="J21" s="68"/>
       <c r="K21" s="68"/>
-      <c r="L21" s="227"/>
+      <c r="L21" s="226"/>
       <c r="M21" s="62">
         <v>7</v>
       </c>
@@ -6688,14 +6711,14 @@
       </c>
       <c r="O21" s="65"/>
       <c r="P21" s="65"/>
-      <c r="Q21" s="227"/>
+      <c r="Q21" s="226"/>
       <c r="R21" s="43"/>
       <c r="S21" s="39"/>
       <c r="U21" s="43"/>
       <c r="V21" s="43"/>
     </row>
     <row r="22" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="227"/>
+      <c r="A22" s="226"/>
       <c r="B22" s="14"/>
       <c r="C22" s="45"/>
       <c r="D22" s="62">
@@ -6719,7 +6742,7 @@
       <c r="I22" s="68"/>
       <c r="J22" s="68"/>
       <c r="K22" s="68"/>
-      <c r="L22" s="227"/>
+      <c r="L22" s="226"/>
       <c r="M22" s="62">
         <v>8</v>
       </c>
@@ -6728,30 +6751,30 @@
       </c>
       <c r="O22" s="65"/>
       <c r="P22" s="65"/>
-      <c r="Q22" s="227"/>
+      <c r="Q22" s="226"/>
       <c r="R22" s="43"/>
       <c r="S22" s="39"/>
       <c r="U22" s="43"/>
       <c r="V22" s="43"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="227"/>
-      <c r="B23" s="230"/>
-      <c r="C23" s="227"/>
-      <c r="D23" s="231"/>
-      <c r="E23" s="227"/>
-      <c r="F23" s="227"/>
-      <c r="G23" s="227"/>
+      <c r="A23" s="226"/>
+      <c r="B23" s="229"/>
+      <c r="C23" s="226"/>
+      <c r="D23" s="230"/>
+      <c r="E23" s="226"/>
+      <c r="F23" s="226"/>
+      <c r="G23" s="226"/>
       <c r="H23" s="56"/>
       <c r="I23" s="56"/>
       <c r="J23" s="56"/>
       <c r="K23" s="56"/>
-      <c r="L23" s="227"/>
-      <c r="M23" s="231"/>
-      <c r="N23" s="227"/>
-      <c r="O23" s="227"/>
-      <c r="P23" s="227"/>
-      <c r="Q23" s="227"/>
+      <c r="L23" s="226"/>
+      <c r="M23" s="230"/>
+      <c r="N23" s="226"/>
+      <c r="O23" s="226"/>
+      <c r="P23" s="226"/>
+      <c r="Q23" s="226"/>
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
       <c r="T23" s="17"/>
@@ -6761,39 +6784,39 @@
       <c r="X23" s="17"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="227"/>
-      <c r="B24" s="229" t="s">
+      <c r="A24" s="226"/>
+      <c r="B24" s="228" t="s">
         <v>177</v>
       </c>
-      <c r="C24" s="227"/>
-      <c r="D24" s="228" t="s">
+      <c r="C24" s="226"/>
+      <c r="D24" s="227" t="s">
         <v>178</v>
       </c>
-      <c r="E24" s="227"/>
-      <c r="F24" s="227"/>
-      <c r="G24" s="227"/>
+      <c r="E24" s="226"/>
+      <c r="F24" s="226"/>
+      <c r="G24" s="226"/>
       <c r="H24" s="74"/>
       <c r="I24" s="74"/>
       <c r="J24" s="74"/>
       <c r="K24" s="74"/>
-      <c r="L24" s="227"/>
-      <c r="M24" s="228" t="s">
+      <c r="L24" s="226"/>
+      <c r="M24" s="227" t="s">
         <v>179</v>
       </c>
-      <c r="N24" s="227"/>
-      <c r="O24" s="227"/>
-      <c r="P24" s="227"/>
-      <c r="Q24" s="227"/>
+      <c r="N24" s="226"/>
+      <c r="O24" s="226"/>
+      <c r="P24" s="226"/>
+      <c r="Q24" s="226"/>
       <c r="R24" s="17"/>
       <c r="S24" s="17"/>
       <c r="T24" s="17"/>
       <c r="U24" s="17"/>
-      <c r="V24" s="226"/>
-      <c r="W24" s="227"/>
-      <c r="X24" s="227"/>
+      <c r="V24" s="225"/>
+      <c r="W24" s="226"/>
+      <c r="X24" s="226"/>
     </row>
     <row r="25" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="227"/>
+      <c r="A25" s="226"/>
       <c r="B25" s="14" t="s">
         <v>180</v>
       </c>
@@ -6824,7 +6847,7 @@
       <c r="K25" s="76" t="s">
         <v>190</v>
       </c>
-      <c r="L25" s="227"/>
+      <c r="L25" s="226"/>
       <c r="M25" s="76" t="s">
         <v>191</v>
       </c>
@@ -6837,7 +6860,7 @@
       <c r="P25" s="76" t="s">
         <v>194</v>
       </c>
-      <c r="Q25" s="227"/>
+      <c r="Q25" s="226"/>
       <c r="R25" s="27"/>
       <c r="S25" s="27"/>
       <c r="T25" s="27"/>
@@ -6847,7 +6870,7 @@
       <c r="X25" s="27"/>
     </row>
     <row r="26" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="227"/>
+      <c r="A26" s="226"/>
       <c r="B26" s="14" t="s">
         <v>195</v>
       </c>
@@ -6881,7 +6904,7 @@
         <f>E26/E26</f>
         <v>1</v>
       </c>
-      <c r="L26" s="227"/>
+      <c r="L26" s="226"/>
       <c r="M26" s="77">
         <v>1</v>
       </c>
@@ -6894,7 +6917,7 @@
       <c r="P26" s="81">
         <v>0.2</v>
       </c>
-      <c r="Q26" s="227"/>
+      <c r="Q26" s="226"/>
       <c r="R26" s="43"/>
       <c r="U26" s="43"/>
       <c r="V26" s="43"/>
@@ -6902,7 +6925,7 @@
       <c r="X26" s="10"/>
     </row>
     <row r="27" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="227"/>
+      <c r="A27" s="226"/>
       <c r="B27" s="14"/>
       <c r="C27" s="45"/>
       <c r="D27" s="77">
@@ -6933,7 +6956,7 @@
         <f t="shared" ref="K27:K33" si="11">E27/E$26</f>
         <v>2</v>
       </c>
-      <c r="L27" s="227"/>
+      <c r="L27" s="226"/>
       <c r="M27" s="77">
         <v>2</v>
       </c>
@@ -6946,7 +6969,7 @@
       <c r="P27" s="81">
         <v>0.4</v>
       </c>
-      <c r="Q27" s="227"/>
+      <c r="Q27" s="226"/>
       <c r="R27" s="43"/>
       <c r="U27" s="43"/>
       <c r="V27" s="43"/>
@@ -6954,7 +6977,7 @@
       <c r="X27" s="10"/>
     </row>
     <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="227"/>
+      <c r="A28" s="226"/>
       <c r="B28" s="14"/>
       <c r="C28" s="45"/>
       <c r="D28" s="77">
@@ -6987,7 +7010,7 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="L28" s="227"/>
+      <c r="L28" s="226"/>
       <c r="M28" s="77">
         <v>3</v>
       </c>
@@ -7000,7 +7023,7 @@
       <c r="P28" s="81">
         <v>0.6</v>
       </c>
-      <c r="Q28" s="227"/>
+      <c r="Q28" s="226"/>
       <c r="R28" s="43"/>
       <c r="U28" s="43"/>
       <c r="V28" s="43"/>
@@ -7008,7 +7031,7 @@
       <c r="X28" s="10"/>
     </row>
     <row r="29" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="227"/>
+      <c r="A29" s="226"/>
       <c r="B29" s="14"/>
       <c r="C29" s="45"/>
       <c r="D29" s="77">
@@ -7039,7 +7062,7 @@
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="L29" s="227"/>
+      <c r="L29" s="226"/>
       <c r="M29" s="77">
         <v>4</v>
       </c>
@@ -7052,13 +7075,13 @@
       <c r="P29" s="81">
         <v>0.8</v>
       </c>
-      <c r="Q29" s="227"/>
+      <c r="Q29" s="226"/>
       <c r="R29" s="43"/>
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
     </row>
     <row r="30" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="227"/>
+      <c r="A30" s="226"/>
       <c r="B30" s="14"/>
       <c r="C30" s="45"/>
       <c r="D30" s="77">
@@ -7091,7 +7114,7 @@
         <f t="shared" si="11"/>
         <v>8</v>
       </c>
-      <c r="L30" s="227"/>
+      <c r="L30" s="226"/>
       <c r="M30" s="77">
         <v>5</v>
       </c>
@@ -7104,13 +7127,13 @@
       <c r="P30" s="81">
         <v>1</v>
       </c>
-      <c r="Q30" s="227"/>
+      <c r="Q30" s="226"/>
       <c r="R30" s="43"/>
       <c r="U30" s="43"/>
       <c r="V30" s="43"/>
     </row>
     <row r="31" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="227"/>
+      <c r="A31" s="226"/>
       <c r="B31" s="14"/>
       <c r="C31" s="45"/>
       <c r="D31" s="77">
@@ -7141,7 +7164,7 @@
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
-      <c r="L31" s="227"/>
+      <c r="L31" s="226"/>
       <c r="M31" s="77">
         <v>6</v>
       </c>
@@ -7154,13 +7177,13 @@
       <c r="P31" s="81">
         <v>1.2</v>
       </c>
-      <c r="Q31" s="227"/>
+      <c r="Q31" s="226"/>
       <c r="R31" s="43"/>
       <c r="U31" s="43"/>
       <c r="V31" s="43"/>
     </row>
     <row r="32" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="227"/>
+      <c r="A32" s="226"/>
       <c r="B32" s="14"/>
       <c r="C32" s="45"/>
       <c r="D32" s="77">
@@ -7193,7 +7216,7 @@
         <f t="shared" si="11"/>
         <v>13.999999999999998</v>
       </c>
-      <c r="L32" s="227"/>
+      <c r="L32" s="226"/>
       <c r="M32" s="77">
         <v>7</v>
       </c>
@@ -7206,13 +7229,13 @@
       <c r="P32" s="81">
         <v>1.6</v>
       </c>
-      <c r="Q32" s="227"/>
+      <c r="Q32" s="226"/>
       <c r="R32" s="43"/>
       <c r="U32" s="43"/>
       <c r="V32" s="43"/>
     </row>
     <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="227"/>
+      <c r="A33" s="226"/>
       <c r="B33" s="14"/>
       <c r="C33" s="45"/>
       <c r="D33" s="77">
@@ -7245,7 +7268,7 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-      <c r="L33" s="227"/>
+      <c r="L33" s="226"/>
       <c r="M33" s="77">
         <v>8</v>
       </c>
@@ -7258,55 +7281,55 @@
       <c r="P33" s="81">
         <v>2</v>
       </c>
-      <c r="Q33" s="227"/>
+      <c r="Q33" s="226"/>
       <c r="R33" s="43"/>
       <c r="U33" s="43"/>
       <c r="V33" s="43"/>
     </row>
     <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="227"/>
-      <c r="B34" s="230"/>
-      <c r="C34" s="227"/>
-      <c r="D34" s="231"/>
-      <c r="E34" s="227"/>
-      <c r="F34" s="227"/>
-      <c r="G34" s="227"/>
+      <c r="A34" s="226"/>
+      <c r="B34" s="229"/>
+      <c r="C34" s="226"/>
+      <c r="D34" s="230"/>
+      <c r="E34" s="226"/>
+      <c r="F34" s="226"/>
+      <c r="G34" s="226"/>
       <c r="H34" s="56"/>
       <c r="I34" s="56"/>
       <c r="J34" s="56"/>
       <c r="K34" s="56"/>
-      <c r="L34" s="227"/>
-      <c r="M34" s="231"/>
-      <c r="N34" s="227"/>
-      <c r="O34" s="227"/>
-      <c r="P34" s="227"/>
-      <c r="Q34" s="227"/>
+      <c r="L34" s="226"/>
+      <c r="M34" s="230"/>
+      <c r="N34" s="226"/>
+      <c r="O34" s="226"/>
+      <c r="P34" s="226"/>
+      <c r="Q34" s="226"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="227"/>
-      <c r="B35" s="229"/>
-      <c r="C35" s="227"/>
-      <c r="D35" s="237" t="s">
+      <c r="A35" s="226"/>
+      <c r="B35" s="228"/>
+      <c r="C35" s="226"/>
+      <c r="D35" s="236" t="s">
         <v>238</v>
       </c>
-      <c r="E35" s="227"/>
-      <c r="F35" s="227"/>
-      <c r="G35" s="227"/>
+      <c r="E35" s="226"/>
+      <c r="F35" s="226"/>
+      <c r="G35" s="226"/>
       <c r="H35" s="96"/>
       <c r="I35" s="96"/>
       <c r="J35" s="96"/>
       <c r="K35" s="96"/>
-      <c r="L35" s="227"/>
-      <c r="M35" s="237" t="s">
+      <c r="L35" s="226"/>
+      <c r="M35" s="236" t="s">
         <v>239</v>
       </c>
-      <c r="N35" s="227"/>
-      <c r="O35" s="227"/>
-      <c r="P35" s="227"/>
-      <c r="Q35" s="227"/>
+      <c r="N35" s="226"/>
+      <c r="O35" s="226"/>
+      <c r="P35" s="226"/>
+      <c r="Q35" s="226"/>
     </row>
     <row r="36" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="227"/>
+      <c r="A36" s="226"/>
       <c r="B36" s="14"/>
       <c r="C36" s="45"/>
       <c r="D36" s="97" t="s">
@@ -7325,7 +7348,7 @@
       <c r="I36" s="97"/>
       <c r="J36" s="97"/>
       <c r="K36" s="97"/>
-      <c r="L36" s="227"/>
+      <c r="L36" s="226"/>
       <c r="M36" s="97" t="s">
         <v>244</v>
       </c>
@@ -7334,10 +7357,10 @@
       </c>
       <c r="O36" s="97"/>
       <c r="P36" s="97"/>
-      <c r="Q36" s="227"/>
+      <c r="Q36" s="226"/>
     </row>
     <row r="37" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="227"/>
+      <c r="A37" s="226"/>
       <c r="B37" s="14"/>
       <c r="C37" s="45"/>
       <c r="D37" s="99">
@@ -7355,7 +7378,7 @@
       <c r="I37" s="53"/>
       <c r="J37" s="53"/>
       <c r="K37" s="53"/>
-      <c r="L37" s="227"/>
+      <c r="L37" s="226"/>
       <c r="M37" s="99">
         <v>1</v>
       </c>
@@ -7364,10 +7387,10 @@
       </c>
       <c r="O37" s="53"/>
       <c r="P37" s="53"/>
-      <c r="Q37" s="227"/>
+      <c r="Q37" s="226"/>
     </row>
     <row r="38" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="227"/>
+      <c r="A38" s="226"/>
       <c r="B38" s="14"/>
       <c r="C38" s="45"/>
       <c r="D38" s="99">
@@ -7386,7 +7409,7 @@
       <c r="I38" s="53"/>
       <c r="J38" s="53"/>
       <c r="K38" s="53"/>
-      <c r="L38" s="227"/>
+      <c r="L38" s="226"/>
       <c r="M38" s="99">
         <v>2</v>
       </c>
@@ -7395,10 +7418,10 @@
       </c>
       <c r="O38" s="53"/>
       <c r="P38" s="53"/>
-      <c r="Q38" s="227"/>
+      <c r="Q38" s="226"/>
     </row>
     <row r="39" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="227"/>
+      <c r="A39" s="226"/>
       <c r="B39" s="14"/>
       <c r="C39" s="45"/>
       <c r="D39" s="99">
@@ -7419,7 +7442,7 @@
       <c r="I39" s="53"/>
       <c r="J39" s="53"/>
       <c r="K39" s="53"/>
-      <c r="L39" s="227"/>
+      <c r="L39" s="226"/>
       <c r="M39" s="99">
         <v>3</v>
       </c>
@@ -7428,10 +7451,10 @@
       </c>
       <c r="O39" s="53"/>
       <c r="P39" s="53"/>
-      <c r="Q39" s="227"/>
+      <c r="Q39" s="226"/>
     </row>
     <row r="40" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="227"/>
+      <c r="A40" s="226"/>
       <c r="B40" s="14"/>
       <c r="C40" s="45"/>
       <c r="D40" s="99">
@@ -7450,7 +7473,7 @@
       <c r="I40" s="53"/>
       <c r="J40" s="53"/>
       <c r="K40" s="53"/>
-      <c r="L40" s="227"/>
+      <c r="L40" s="226"/>
       <c r="M40" s="99">
         <v>4</v>
       </c>
@@ -7459,10 +7482,10 @@
       </c>
       <c r="O40" s="53"/>
       <c r="P40" s="53"/>
-      <c r="Q40" s="227"/>
+      <c r="Q40" s="226"/>
     </row>
     <row r="41" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="227"/>
+      <c r="A41" s="226"/>
       <c r="B41" s="14"/>
       <c r="C41" s="45"/>
       <c r="D41" s="99">
@@ -7483,7 +7506,7 @@
       <c r="I41" s="53"/>
       <c r="J41" s="53"/>
       <c r="K41" s="53"/>
-      <c r="L41" s="227"/>
+      <c r="L41" s="226"/>
       <c r="M41" s="99">
         <v>5</v>
       </c>
@@ -7492,10 +7515,10 @@
       </c>
       <c r="O41" s="53"/>
       <c r="P41" s="53"/>
-      <c r="Q41" s="227"/>
+      <c r="Q41" s="226"/>
     </row>
     <row r="42" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="227"/>
+      <c r="A42" s="226"/>
       <c r="B42" s="14"/>
       <c r="C42" s="45"/>
       <c r="D42" s="99">
@@ -7514,7 +7537,7 @@
       <c r="I42" s="53"/>
       <c r="J42" s="53"/>
       <c r="K42" s="53"/>
-      <c r="L42" s="227"/>
+      <c r="L42" s="226"/>
       <c r="M42" s="99">
         <v>6</v>
       </c>
@@ -7523,10 +7546,10 @@
       </c>
       <c r="O42" s="53"/>
       <c r="P42" s="53"/>
-      <c r="Q42" s="227"/>
+      <c r="Q42" s="226"/>
     </row>
     <row r="43" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="227"/>
+      <c r="A43" s="226"/>
       <c r="B43" s="14"/>
       <c r="C43" s="45"/>
       <c r="D43" s="99">
@@ -7547,7 +7570,7 @@
       <c r="I43" s="53"/>
       <c r="J43" s="53"/>
       <c r="K43" s="53"/>
-      <c r="L43" s="227"/>
+      <c r="L43" s="226"/>
       <c r="M43" s="99">
         <v>7</v>
       </c>
@@ -7556,10 +7579,10 @@
       </c>
       <c r="O43" s="53"/>
       <c r="P43" s="53"/>
-      <c r="Q43" s="227"/>
+      <c r="Q43" s="226"/>
     </row>
     <row r="44" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="227"/>
+      <c r="A44" s="226"/>
       <c r="B44" s="14"/>
       <c r="C44" s="45"/>
       <c r="D44" s="99">
@@ -7580,7 +7603,7 @@
       <c r="I44" s="53"/>
       <c r="J44" s="53"/>
       <c r="K44" s="53"/>
-      <c r="L44" s="227"/>
+      <c r="L44" s="226"/>
       <c r="M44" s="99">
         <v>8</v>
       </c>
@@ -7589,52 +7612,52 @@
       </c>
       <c r="O44" s="53"/>
       <c r="P44" s="53"/>
-      <c r="Q44" s="227"/>
+      <c r="Q44" s="226"/>
     </row>
     <row r="45" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="227"/>
-      <c r="B45" s="230"/>
-      <c r="C45" s="227"/>
-      <c r="D45" s="231"/>
-      <c r="E45" s="227"/>
-      <c r="F45" s="227"/>
-      <c r="G45" s="227"/>
+      <c r="A45" s="226"/>
+      <c r="B45" s="229"/>
+      <c r="C45" s="226"/>
+      <c r="D45" s="230"/>
+      <c r="E45" s="226"/>
+      <c r="F45" s="226"/>
+      <c r="G45" s="226"/>
       <c r="H45" s="56"/>
       <c r="I45" s="56"/>
       <c r="J45" s="56"/>
       <c r="K45" s="56"/>
-      <c r="L45" s="227"/>
-      <c r="M45" s="231"/>
-      <c r="N45" s="227"/>
-      <c r="O45" s="227"/>
-      <c r="P45" s="227"/>
-      <c r="Q45" s="227"/>
+      <c r="L45" s="226"/>
+      <c r="M45" s="230"/>
+      <c r="N45" s="226"/>
+      <c r="O45" s="226"/>
+      <c r="P45" s="226"/>
+      <c r="Q45" s="226"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="227"/>
-      <c r="B46" s="229"/>
-      <c r="C46" s="227"/>
-      <c r="D46" s="239" t="s">
+      <c r="A46" s="226"/>
+      <c r="B46" s="228"/>
+      <c r="C46" s="226"/>
+      <c r="D46" s="238" t="s">
         <v>258</v>
       </c>
-      <c r="E46" s="227"/>
-      <c r="F46" s="227"/>
-      <c r="G46" s="227"/>
+      <c r="E46" s="226"/>
+      <c r="F46" s="226"/>
+      <c r="G46" s="226"/>
       <c r="H46" s="106"/>
       <c r="I46" s="106"/>
       <c r="J46" s="106"/>
       <c r="K46" s="106"/>
-      <c r="L46" s="227"/>
-      <c r="M46" s="239" t="s">
+      <c r="L46" s="226"/>
+      <c r="M46" s="238" t="s">
         <v>262</v>
       </c>
-      <c r="N46" s="227"/>
-      <c r="O46" s="227"/>
-      <c r="P46" s="227"/>
-      <c r="Q46" s="227"/>
+      <c r="N46" s="226"/>
+      <c r="O46" s="226"/>
+      <c r="P46" s="226"/>
+      <c r="Q46" s="226"/>
     </row>
     <row r="47" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="227"/>
+      <c r="A47" s="226"/>
       <c r="B47" s="14"/>
       <c r="C47" s="45"/>
       <c r="D47" s="108" t="s">
@@ -7651,7 +7674,7 @@
       <c r="I47" s="108"/>
       <c r="J47" s="108"/>
       <c r="K47" s="108"/>
-      <c r="L47" s="227"/>
+      <c r="L47" s="226"/>
       <c r="M47" s="108" t="s">
         <v>273</v>
       </c>
@@ -7660,10 +7683,10 @@
       </c>
       <c r="O47" s="108"/>
       <c r="P47" s="108"/>
-      <c r="Q47" s="227"/>
+      <c r="Q47" s="226"/>
     </row>
     <row r="48" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="227"/>
+      <c r="A48" s="226"/>
       <c r="B48" s="14"/>
       <c r="C48" s="45"/>
       <c r="D48" s="110">
@@ -7678,7 +7701,7 @@
       <c r="I48" s="113"/>
       <c r="J48" s="113"/>
       <c r="K48" s="113"/>
-      <c r="L48" s="227"/>
+      <c r="L48" s="226"/>
       <c r="M48" s="110">
         <v>1</v>
       </c>
@@ -7687,10 +7710,10 @@
       </c>
       <c r="O48" s="113"/>
       <c r="P48" s="113"/>
-      <c r="Q48" s="227"/>
+      <c r="Q48" s="226"/>
     </row>
     <row r="49" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="227"/>
+      <c r="A49" s="226"/>
       <c r="B49" s="14"/>
       <c r="C49" s="45"/>
       <c r="D49" s="110">
@@ -7706,7 +7729,7 @@
       <c r="I49" s="113"/>
       <c r="J49" s="113"/>
       <c r="K49" s="113"/>
-      <c r="L49" s="227"/>
+      <c r="L49" s="226"/>
       <c r="M49" s="110">
         <v>2</v>
       </c>
@@ -7715,10 +7738,10 @@
       </c>
       <c r="O49" s="113"/>
       <c r="P49" s="113"/>
-      <c r="Q49" s="227"/>
+      <c r="Q49" s="226"/>
     </row>
     <row r="50" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="227"/>
+      <c r="A50" s="226"/>
       <c r="B50" s="14"/>
       <c r="C50" s="45"/>
       <c r="D50" s="110">
@@ -7736,7 +7759,7 @@
       <c r="I50" s="113"/>
       <c r="J50" s="113"/>
       <c r="K50" s="113"/>
-      <c r="L50" s="227"/>
+      <c r="L50" s="226"/>
       <c r="M50" s="110">
         <v>3</v>
       </c>
@@ -7745,10 +7768,10 @@
       </c>
       <c r="O50" s="113"/>
       <c r="P50" s="113"/>
-      <c r="Q50" s="227"/>
+      <c r="Q50" s="226"/>
     </row>
     <row r="51" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="227"/>
+      <c r="A51" s="226"/>
       <c r="B51" s="14"/>
       <c r="C51" s="45"/>
       <c r="D51" s="110">
@@ -7764,7 +7787,7 @@
       <c r="I51" s="113"/>
       <c r="J51" s="113"/>
       <c r="K51" s="113"/>
-      <c r="L51" s="227"/>
+      <c r="L51" s="226"/>
       <c r="M51" s="110">
         <v>4</v>
       </c>
@@ -7773,10 +7796,10 @@
       </c>
       <c r="O51" s="113"/>
       <c r="P51" s="113"/>
-      <c r="Q51" s="227"/>
+      <c r="Q51" s="226"/>
     </row>
     <row r="52" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="227"/>
+      <c r="A52" s="226"/>
       <c r="B52" s="14"/>
       <c r="C52" s="45"/>
       <c r="D52" s="110">
@@ -7794,7 +7817,7 @@
       <c r="I52" s="113"/>
       <c r="J52" s="113"/>
       <c r="K52" s="113"/>
-      <c r="L52" s="227"/>
+      <c r="L52" s="226"/>
       <c r="M52" s="110">
         <v>5</v>
       </c>
@@ -7803,10 +7826,10 @@
       </c>
       <c r="O52" s="113"/>
       <c r="P52" s="113"/>
-      <c r="Q52" s="227"/>
+      <c r="Q52" s="226"/>
     </row>
     <row r="53" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="227"/>
+      <c r="A53" s="226"/>
       <c r="B53" s="14"/>
       <c r="C53" s="45"/>
       <c r="D53" s="110">
@@ -7822,7 +7845,7 @@
       <c r="I53" s="113"/>
       <c r="J53" s="113"/>
       <c r="K53" s="113"/>
-      <c r="L53" s="227"/>
+      <c r="L53" s="226"/>
       <c r="M53" s="110">
         <v>6</v>
       </c>
@@ -7831,10 +7854,10 @@
       </c>
       <c r="O53" s="113"/>
       <c r="P53" s="113"/>
-      <c r="Q53" s="227"/>
+      <c r="Q53" s="226"/>
     </row>
     <row r="54" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="227"/>
+      <c r="A54" s="226"/>
       <c r="B54" s="14"/>
       <c r="C54" s="45"/>
       <c r="D54" s="110">
@@ -7852,7 +7875,7 @@
       <c r="I54" s="113"/>
       <c r="J54" s="113"/>
       <c r="K54" s="113"/>
-      <c r="L54" s="227"/>
+      <c r="L54" s="226"/>
       <c r="M54" s="110">
         <v>7</v>
       </c>
@@ -7861,10 +7884,10 @@
       </c>
       <c r="O54" s="113"/>
       <c r="P54" s="113"/>
-      <c r="Q54" s="227"/>
+      <c r="Q54" s="226"/>
     </row>
     <row r="55" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="227"/>
+      <c r="A55" s="226"/>
       <c r="B55" s="14"/>
       <c r="C55" s="45"/>
       <c r="D55" s="110">
@@ -7882,7 +7905,7 @@
       <c r="I55" s="113"/>
       <c r="J55" s="113"/>
       <c r="K55" s="113"/>
-      <c r="L55" s="227"/>
+      <c r="L55" s="226"/>
       <c r="M55" s="110">
         <v>8</v>
       </c>
@@ -7891,26 +7914,26 @@
       </c>
       <c r="O55" s="113"/>
       <c r="P55" s="113"/>
-      <c r="Q55" s="227"/>
+      <c r="Q55" s="226"/>
     </row>
     <row r="56" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="227"/>
+      <c r="A56" s="226"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="238"/>
-      <c r="E56" s="227"/>
-      <c r="F56" s="227"/>
-      <c r="G56" s="227"/>
-      <c r="H56" s="227"/>
-      <c r="I56" s="227"/>
-      <c r="J56" s="227"/>
-      <c r="K56" s="227"/>
-      <c r="L56" s="227"/>
-      <c r="M56" s="227"/>
-      <c r="N56" s="227"/>
-      <c r="O56" s="227"/>
-      <c r="P56" s="227"/>
-      <c r="Q56" s="227"/>
+      <c r="D56" s="237"/>
+      <c r="E56" s="226"/>
+      <c r="F56" s="226"/>
+      <c r="G56" s="226"/>
+      <c r="H56" s="226"/>
+      <c r="I56" s="226"/>
+      <c r="J56" s="226"/>
+      <c r="K56" s="226"/>
+      <c r="L56" s="226"/>
+      <c r="M56" s="226"/>
+      <c r="N56" s="226"/>
+      <c r="O56" s="226"/>
+      <c r="P56" s="226"/>
+      <c r="Q56" s="226"/>
     </row>
   </sheetData>
   <mergeCells count="38">
@@ -8197,90 +8220,90 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="244" t="s">
+      <c r="A26" s="243" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="227"/>
-      <c r="C26" s="227"/>
+      <c r="B26" s="226"/>
+      <c r="C26" s="226"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="243"/>
-      <c r="B27" s="227"/>
+      <c r="A27" s="242"/>
+      <c r="B27" s="226"/>
       <c r="C27" s="50"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="243"/>
-      <c r="B28" s="227"/>
+      <c r="A28" s="242"/>
+      <c r="B28" s="226"/>
       <c r="C28" s="51"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="243"/>
-      <c r="B29" s="227"/>
+      <c r="A29" s="242"/>
+      <c r="B29" s="226"/>
       <c r="C29" s="121"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="243"/>
-      <c r="B30" s="227"/>
+      <c r="A30" s="242"/>
+      <c r="B30" s="226"/>
       <c r="C30" s="53"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="243"/>
-      <c r="B31" s="227"/>
+      <c r="A31" s="242"/>
+      <c r="B31" s="226"/>
       <c r="C31" s="53"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="241"/>
-      <c r="B32" s="227"/>
+      <c r="A32" s="240"/>
+      <c r="B32" s="226"/>
       <c r="C32" s="121"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="240"/>
-      <c r="B33" s="227"/>
+      <c r="A33" s="239"/>
+      <c r="B33" s="226"/>
       <c r="C33" s="53"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="240"/>
-      <c r="B34" s="227"/>
+      <c r="A34" s="239"/>
+      <c r="B34" s="226"/>
       <c r="C34" s="53"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="240"/>
-      <c r="B35" s="227"/>
+      <c r="A35" s="239"/>
+      <c r="B35" s="226"/>
       <c r="C35" s="53"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="240"/>
-      <c r="B36" s="227"/>
+      <c r="A36" s="239"/>
+      <c r="B36" s="226"/>
       <c r="C36" s="53"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="240"/>
-      <c r="B37" s="227"/>
+      <c r="A37" s="239"/>
+      <c r="B37" s="226"/>
       <c r="C37" s="53"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="240"/>
-      <c r="B38" s="227"/>
+      <c r="A38" s="239"/>
+      <c r="B38" s="226"/>
       <c r="C38" s="53"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="240"/>
-      <c r="B39" s="227"/>
+      <c r="A39" s="239"/>
+      <c r="B39" s="226"/>
       <c r="C39" s="53"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="240"/>
-      <c r="B40" s="227"/>
+      <c r="A40" s="239"/>
+      <c r="B40" s="226"/>
       <c r="C40" s="53"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="240"/>
-      <c r="B41" s="227"/>
+      <c r="A41" s="239"/>
+      <c r="B41" s="226"/>
       <c r="C41" s="53"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="240"/>
-      <c r="B42" s="227"/>
+      <c r="A42" s="239"/>
+      <c r="B42" s="226"/>
       <c r="C42" s="53"/>
     </row>
   </sheetData>
@@ -8487,17 +8510,17 @@
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="277" t="s">
+      <c r="A3" s="276" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="227"/>
-      <c r="C3" s="227"/>
-      <c r="D3" s="227"/>
-      <c r="E3" s="227"/>
-      <c r="F3" s="227"/>
-      <c r="G3" s="227"/>
-      <c r="H3" s="227"/>
-      <c r="I3" s="227"/>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -8525,20 +8548,20 @@
       <c r="P4" s="19"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="234" t="s">
+      <c r="A5" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="227"/>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="227"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="227"/>
-      <c r="H5" s="227"/>
-      <c r="I5" s="227"/>
-      <c r="J5" s="227"/>
-      <c r="K5" s="227"/>
-      <c r="L5" s="227"/>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
+      <c r="J5" s="226"/>
+      <c r="K5" s="226"/>
+      <c r="L5" s="226"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
@@ -8557,10 +8580,10 @@
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="276" t="s">
+      <c r="K6" s="275" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="227"/>
+      <c r="L6" s="226"/>
       <c r="M6" s="23"/>
       <c r="N6" s="23"/>
       <c r="O6" s="23"/>
@@ -8927,20 +8950,20 @@
       <c r="P13" s="10"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="234" t="s">
+      <c r="A15" s="233" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="227"/>
-      <c r="C15" s="227"/>
-      <c r="D15" s="227"/>
-      <c r="E15" s="227"/>
-      <c r="F15" s="227"/>
-      <c r="G15" s="227"/>
-      <c r="H15" s="227"/>
-      <c r="I15" s="227"/>
-      <c r="J15" s="227"/>
-      <c r="K15" s="227"/>
-      <c r="L15" s="227"/>
+      <c r="B15" s="226"/>
+      <c r="C15" s="226"/>
+      <c r="D15" s="226"/>
+      <c r="E15" s="226"/>
+      <c r="F15" s="226"/>
+      <c r="G15" s="226"/>
+      <c r="H15" s="226"/>
+      <c r="I15" s="226"/>
+      <c r="J15" s="226"/>
+      <c r="K15" s="226"/>
+      <c r="L15" s="226"/>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
@@ -8971,10 +8994,10 @@
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="276" t="s">
+      <c r="K16" s="275" t="s">
         <v>120</v>
       </c>
-      <c r="L16" s="227"/>
+      <c r="L16" s="226"/>
       <c r="M16" s="23"/>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -8988,10 +9011,10 @@
       <c r="W16" s="43"/>
       <c r="X16" s="43"/>
       <c r="Y16" s="43"/>
-      <c r="Z16" s="278"/>
-      <c r="AA16" s="227"/>
-      <c r="AB16" s="278"/>
-      <c r="AC16" s="227"/>
+      <c r="Z16" s="277"/>
+      <c r="AA16" s="226"/>
+      <c r="AB16" s="277"/>
+      <c r="AC16" s="226"/>
       <c r="AD16" s="57"/>
     </row>
     <row r="17" spans="1:28" ht="15" x14ac:dyDescent="0.25">
@@ -9819,18 +9842,18 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="234" t="s">
+      <c r="B1" s="233" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="227"/>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="227"/>
-      <c r="G1" s="227"/>
-      <c r="H1" s="227"/>
-      <c r="I1" s="227"/>
-      <c r="J1" s="227"/>
-      <c r="K1" s="227"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="226"/>
+      <c r="K1" s="226"/>
       <c r="L1" s="12"/>
       <c r="M1" s="117"/>
       <c r="N1" s="117"/>
@@ -10229,11 +10252,11 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="244" t="s">
+      <c r="A9" s="243" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="227"/>
-      <c r="C9" s="227"/>
+      <c r="B9" s="226"/>
+      <c r="C9" s="226"/>
       <c r="M9" s="140" t="s">
         <v>293</v>
       </c>
@@ -10243,10 +10266,10 @@
       <c r="O9" s="140"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="243" t="s">
+      <c r="A10" s="242" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="227"/>
+      <c r="B10" s="226"/>
       <c r="C10" s="50">
         <f>C4*14/5100</f>
         <v>1.6016000000000001</v>
@@ -10258,20 +10281,20 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="243" t="s">
+      <c r="A11" s="242" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="227"/>
+      <c r="B11" s="226"/>
       <c r="C11" s="51">
         <v>1</v>
       </c>
       <c r="D11" s="51"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="243" t="s">
+      <c r="A12" s="242" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="227"/>
+      <c r="B12" s="226"/>
       <c r="C12" s="121">
         <v>1.55</v>
       </c>
@@ -10283,10 +10306,10 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="243" t="s">
+      <c r="A13" s="242" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="227"/>
+      <c r="B13" s="226"/>
       <c r="C13" s="53">
         <v>0.8</v>
       </c>
@@ -10302,10 +10325,10 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="243" t="s">
+      <c r="A14" s="242" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="227"/>
+      <c r="B14" s="226"/>
       <c r="C14" s="53">
         <v>10</v>
       </c>
@@ -10320,10 +10343,10 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="241" t="s">
+      <c r="A15" s="240" t="s">
         <v>311</v>
       </c>
-      <c r="B15" s="227"/>
+      <c r="B15" s="226"/>
       <c r="C15" s="121">
         <v>1.3</v>
       </c>
@@ -10342,10 +10365,10 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="242" t="s">
+      <c r="A16" s="241" t="s">
         <v>312</v>
       </c>
-      <c r="B16" s="227"/>
+      <c r="B16" s="226"/>
       <c r="C16" s="138">
         <v>1.1000000000000001</v>
       </c>
@@ -10361,10 +10384,10 @@
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="242" t="s">
+      <c r="A17" s="241" t="s">
         <v>310</v>
       </c>
-      <c r="B17" s="227"/>
+      <c r="B17" s="226"/>
       <c r="C17" s="138">
         <v>1</v>
       </c>
@@ -10380,8 +10403,8 @@
       <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="240"/>
-      <c r="B18" s="227"/>
+      <c r="A18" s="239"/>
+      <c r="B18" s="226"/>
       <c r="C18" s="53"/>
       <c r="D18" s="53"/>
       <c r="E18" s="10">
@@ -10395,8 +10418,8 @@
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="240"/>
-      <c r="B19" s="227"/>
+      <c r="A19" s="239"/>
+      <c r="B19" s="226"/>
       <c r="C19" s="53"/>
       <c r="D19" s="53"/>
     </row>
@@ -10526,13 +10549,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="D1" s="245" t="s">
+      <c r="D1" s="244" t="s">
         <v>281</v>
       </c>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
+      <c r="G1" s="244"/>
+      <c r="H1" s="244"/>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D2" s="130" t="s">
@@ -10856,92 +10879,92 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="244" t="s">
+      <c r="A26" s="243" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="227"/>
-      <c r="C26" s="227"/>
+      <c r="B26" s="226"/>
+      <c r="C26" s="226"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="241" t="s">
+      <c r="A27" s="240" t="s">
         <v>302</v>
       </c>
-      <c r="B27" s="227"/>
+      <c r="B27" s="226"/>
       <c r="C27" s="129">
         <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="241"/>
-      <c r="B28" s="227"/>
+      <c r="A28" s="240"/>
+      <c r="B28" s="226"/>
       <c r="C28" s="139"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="241" t="s">
+      <c r="A29" s="240" t="s">
         <v>303</v>
       </c>
-      <c r="B29" s="227"/>
+      <c r="B29" s="226"/>
       <c r="C29" s="121">
         <v>0.79</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="241" t="s">
+      <c r="A30" s="240" t="s">
         <v>299</v>
       </c>
-      <c r="B30" s="241"/>
+      <c r="B30" s="240"/>
       <c r="C30" s="138">
         <f>C29*C$34</f>
         <v>1.1850000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="241" t="s">
+      <c r="A31" s="240" t="s">
         <v>298</v>
       </c>
-      <c r="B31" s="241"/>
+      <c r="B31" s="240"/>
       <c r="C31" s="138">
         <f t="shared" ref="C31:C33" si="5">C30*C$34</f>
         <v>1.7775000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="241" t="s">
+      <c r="A32" s="240" t="s">
         <v>300</v>
       </c>
-      <c r="B32" s="241"/>
+      <c r="B32" s="240"/>
       <c r="C32" s="138">
         <f t="shared" si="5"/>
         <v>2.6662500000000002</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="242" t="s">
+      <c r="A33" s="241" t="s">
         <v>301</v>
       </c>
-      <c r="B33" s="240"/>
+      <c r="B33" s="239"/>
       <c r="C33" s="138">
         <f t="shared" si="5"/>
         <v>3.9993750000000006</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="242" t="s">
+      <c r="A34" s="241" t="s">
         <v>304</v>
       </c>
-      <c r="B34" s="227"/>
+      <c r="B34" s="226"/>
       <c r="C34" s="53">
         <v>1.5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="240"/>
-      <c r="B35" s="227"/>
+      <c r="A35" s="239"/>
+      <c r="B35" s="226"/>
       <c r="C35" s="53"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="240"/>
-      <c r="B36" s="227"/>
+      <c r="A36" s="239"/>
+      <c r="B36" s="226"/>
       <c r="C36" s="53"/>
     </row>
   </sheetData>
@@ -10967,8 +10990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY49"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BO43" sqref="BO43"/>
+    <sheetView tabSelected="1" topLeftCell="AZ4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BE29" sqref="BE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11001,22 +11024,22 @@
       <c r="A3" s="144" t="s">
         <v>333</v>
       </c>
-      <c r="D3" s="247" t="s">
+      <c r="D3" s="245" t="s">
         <v>419</v>
       </c>
-      <c r="E3" s="248"/>
-      <c r="F3" s="249"/>
-      <c r="G3" s="220"/>
-      <c r="U3" s="247" t="s">
+      <c r="E3" s="246"/>
+      <c r="F3" s="247"/>
+      <c r="G3" s="219"/>
+      <c r="U3" s="245" t="s">
         <v>443</v>
       </c>
-      <c r="V3" s="251"/>
-      <c r="W3" s="252"/>
-      <c r="AL3" s="247" t="s">
+      <c r="V3" s="248"/>
+      <c r="W3" s="249"/>
+      <c r="AL3" s="245" t="s">
         <v>420</v>
       </c>
-      <c r="AM3" s="251"/>
-      <c r="AN3" s="252"/>
+      <c r="AM3" s="248"/>
+      <c r="AN3" s="249"/>
     </row>
     <row r="6" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A6" s="147" t="s">
@@ -11115,10 +11138,10 @@
       <c r="AV6" s="174" t="s">
         <v>338</v>
       </c>
-      <c r="AY6" s="250" t="s">
+      <c r="AY6" s="253" t="s">
         <v>345</v>
       </c>
-      <c r="AZ6" s="250"/>
+      <c r="AZ6" s="253"/>
       <c r="BA6" s="166"/>
       <c r="BB6" s="166"/>
       <c r="BC6" s="166"/>
@@ -11224,8 +11247,8 @@
       <c r="AV7" s="175" t="s">
         <v>339</v>
       </c>
-      <c r="AY7" s="250"/>
-      <c r="AZ7" s="250"/>
+      <c r="AY7" s="253"/>
+      <c r="AZ7" s="253"/>
       <c r="BA7" s="166"/>
       <c r="BB7" s="166"/>
       <c r="BC7" s="166"/>
@@ -11303,7 +11326,7 @@
       <c r="AV8" s="152"/>
       <c r="AY8" s="164"/>
       <c r="BO8" s="119" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:77" x14ac:dyDescent="0.2">
@@ -11357,15 +11380,16 @@
       <c r="BP9" s="165"/>
       <c r="BQ9" s="165"/>
       <c r="BR9" s="165"/>
-      <c r="BT9" s="253" t="s">
+      <c r="BT9" s="250" t="s">
         <v>358</v>
       </c>
-      <c r="BU9" s="253"/>
-      <c r="BV9" s="253"/>
-      <c r="BW9" s="254" t="s">
+      <c r="BU9" s="250"/>
+      <c r="BV9" s="250"/>
+      <c r="BW9" s="281" t="s">
         <v>362</v>
       </c>
-      <c r="BX9" s="254"/>
+      <c r="BX9" s="279"/>
+      <c r="BY9" s="163"/>
     </row>
     <row r="10" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A10" s="149"/>
@@ -11455,8 +11479,9 @@
       <c r="BV10" s="168" t="s">
         <v>360</v>
       </c>
-      <c r="BW10" s="214"/>
-      <c r="BX10" s="214"/>
+      <c r="BW10" s="282"/>
+      <c r="BX10" s="280"/>
+      <c r="BY10" s="163"/>
     </row>
     <row r="11" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A11" s="149"/>
@@ -11542,8 +11567,9 @@
       <c r="BV11" s="154">
         <v>250</v>
       </c>
-      <c r="BW11" s="214"/>
-      <c r="BX11" s="214"/>
+      <c r="BW11" s="154"/>
+      <c r="BX11" s="154"/>
+      <c r="BY11" s="154"/>
     </row>
     <row r="12" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A12" s="149"/>
@@ -11594,20 +11620,31 @@
       </c>
       <c r="BB12" s="153"/>
       <c r="BC12" s="148" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="BD12" s="149"/>
       <c r="BE12" s="152">
         <v>1</v>
       </c>
       <c r="BF12" s="153"/>
-      <c r="BG12" s="152"/>
-      <c r="BH12" s="152"/>
+      <c r="BG12" s="152">
+        <f>BV12*BW12*BM12</f>
+        <v>90</v>
+      </c>
+      <c r="BH12" s="152">
+        <f>BG12*BE12</f>
+        <v>90</v>
+      </c>
       <c r="BI12" s="153"/>
       <c r="BJ12" s="152"/>
-      <c r="BK12" s="152"/>
+      <c r="BK12" s="152">
+        <f>BH12</f>
+        <v>90</v>
+      </c>
       <c r="BL12" s="153"/>
-      <c r="BM12" s="152"/>
+      <c r="BM12" s="152">
+        <v>0.5</v>
+      </c>
       <c r="BN12" s="152"/>
       <c r="BP12" s="162"/>
       <c r="BQ12" s="156"/>
@@ -11619,12 +11656,13 @@
       <c r="BV12" s="154">
         <v>90</v>
       </c>
-      <c r="BW12" s="214">
+      <c r="BW12" s="154">
         <v>2</v>
       </c>
-      <c r="BX12" s="119" t="s">
+      <c r="BX12" s="278" t="s">
         <v>363</v>
       </c>
+      <c r="BY12" s="154"/>
     </row>
     <row r="13" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A13" s="149"/>
@@ -11694,12 +11732,13 @@
       <c r="BV13" s="154">
         <v>150</v>
       </c>
-      <c r="BW13" s="219">
+      <c r="BW13" s="154">
         <v>1.5</v>
       </c>
-      <c r="BX13" s="119" t="s">
+      <c r="BX13" s="278" t="s">
         <v>405</v>
       </c>
+      <c r="BY13" s="154"/>
     </row>
     <row r="14" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A14" s="148" t="s">
@@ -11764,11 +11803,20 @@
       <c r="BP14" s="162"/>
       <c r="BQ14" s="156"/>
       <c r="BR14" s="156"/>
-      <c r="BT14" s="160"/>
+      <c r="BT14" s="160" t="s">
+        <v>464</v>
+      </c>
       <c r="BU14" s="160"/>
-      <c r="BV14" s="154"/>
-      <c r="BW14" s="214"/>
-      <c r="BX14" s="214"/>
+      <c r="BV14" s="154">
+        <v>180</v>
+      </c>
+      <c r="BW14" s="154">
+        <v>0.5</v>
+      </c>
+      <c r="BX14" s="154" t="s">
+        <v>465</v>
+      </c>
+      <c r="BY14" s="154"/>
     </row>
     <row r="15" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A15" s="149"/>
@@ -11819,20 +11867,31 @@
       </c>
       <c r="BB15" s="153"/>
       <c r="BC15" s="148" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="BD15" s="149"/>
       <c r="BE15" s="152">
         <v>1</v>
       </c>
       <c r="BF15" s="153"/>
-      <c r="BG15" s="152"/>
-      <c r="BH15" s="152"/>
+      <c r="BG15" s="152">
+        <f>BV12*BW12*BM15</f>
+        <v>90</v>
+      </c>
+      <c r="BH15" s="152">
+        <f>BG15*BE15</f>
+        <v>90</v>
+      </c>
       <c r="BI15" s="153"/>
       <c r="BJ15" s="152"/>
-      <c r="BK15" s="152"/>
+      <c r="BK15" s="152">
+        <f>BH15</f>
+        <v>90</v>
+      </c>
       <c r="BL15" s="153"/>
-      <c r="BM15" s="152"/>
+      <c r="BM15" s="152">
+        <v>0.5</v>
+      </c>
       <c r="BN15" s="152"/>
       <c r="BP15" s="162"/>
       <c r="BQ15" s="156"/>
@@ -11840,8 +11899,9 @@
       <c r="BT15" s="160"/>
       <c r="BU15" s="160"/>
       <c r="BV15" s="154"/>
-      <c r="BW15" s="214"/>
-      <c r="BX15" s="214"/>
+      <c r="BW15" s="154"/>
+      <c r="BX15" s="154"/>
+      <c r="BY15" s="154"/>
     </row>
     <row r="16" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A16" s="149"/>
@@ -11907,10 +11967,11 @@
       <c r="BT16" s="160"/>
       <c r="BU16" s="160"/>
       <c r="BV16" s="154"/>
-      <c r="BW16" s="214"/>
-      <c r="BX16" s="214"/>
-    </row>
-    <row r="17" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BW16" s="154"/>
+      <c r="BX16" s="154"/>
+      <c r="BY16" s="154"/>
+    </row>
+    <row r="17" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A17" s="149"/>
       <c r="B17" s="153"/>
       <c r="C17" s="149"/>
@@ -11974,10 +12035,11 @@
       <c r="BT17" s="160"/>
       <c r="BU17" s="160"/>
       <c r="BV17" s="154"/>
-      <c r="BW17" s="214"/>
-      <c r="BX17" s="214"/>
-    </row>
-    <row r="18" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BW17" s="154"/>
+      <c r="BX17" s="154"/>
+      <c r="BY17" s="154"/>
+    </row>
+    <row r="18" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A18" s="149"/>
       <c r="B18" s="153"/>
       <c r="C18" s="149"/>
@@ -12026,31 +12088,46 @@
       </c>
       <c r="BB18" s="153"/>
       <c r="BC18" s="148" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="BD18" s="149"/>
       <c r="BE18" s="152">
         <v>1</v>
       </c>
       <c r="BF18" s="153"/>
-      <c r="BG18" s="152"/>
-      <c r="BH18" s="152"/>
+      <c r="BG18" s="152">
+        <f>BV14*BW14*BM18</f>
+        <v>315</v>
+      </c>
+      <c r="BH18" s="152">
+        <f>BG18*BE18</f>
+        <v>315</v>
+      </c>
       <c r="BI18" s="153"/>
       <c r="BJ18" s="152"/>
-      <c r="BK18" s="152"/>
+      <c r="BK18" s="152">
+        <f>BH18+BK12</f>
+        <v>405</v>
+      </c>
       <c r="BL18" s="153"/>
-      <c r="BM18" s="152"/>
-      <c r="BN18" s="152"/>
+      <c r="BM18" s="152">
+        <v>3.5</v>
+      </c>
+      <c r="BN18" s="152">
+        <f>BM18*BW14</f>
+        <v>1.75</v>
+      </c>
       <c r="BP18" s="162"/>
       <c r="BQ18" s="156"/>
       <c r="BR18" s="156"/>
       <c r="BT18" s="159"/>
       <c r="BU18" s="160"/>
       <c r="BV18" s="154"/>
-      <c r="BW18" s="214"/>
-      <c r="BX18" s="214"/>
-    </row>
-    <row r="19" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BW18" s="154"/>
+      <c r="BX18" s="154"/>
+      <c r="BY18" s="154"/>
+    </row>
+    <row r="19" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A19" s="149"/>
       <c r="B19" s="153"/>
       <c r="C19" s="149"/>
@@ -12114,10 +12191,11 @@
       <c r="BT19" s="160"/>
       <c r="BU19" s="160"/>
       <c r="BV19" s="154"/>
-      <c r="BW19" s="214"/>
-      <c r="BX19" s="214"/>
-    </row>
-    <row r="20" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BW19" s="154"/>
+      <c r="BX19" s="154"/>
+      <c r="BY19" s="154"/>
+    </row>
+    <row r="20" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A20" s="149"/>
       <c r="B20" s="153"/>
       <c r="C20" s="149"/>
@@ -12178,10 +12256,11 @@
       <c r="BT20" s="160"/>
       <c r="BU20" s="160"/>
       <c r="BV20" s="154"/>
-      <c r="BW20" s="214"/>
-      <c r="BX20" s="214"/>
-    </row>
-    <row r="21" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BW20" s="154"/>
+      <c r="BX20" s="154"/>
+      <c r="BY20" s="154"/>
+    </row>
+    <row r="21" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A21" s="149"/>
       <c r="B21" s="153"/>
       <c r="C21" s="149"/>
@@ -12230,28 +12309,43 @@
       </c>
       <c r="BB21" s="153"/>
       <c r="BC21" s="148" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="BD21" s="149"/>
       <c r="BE21" s="152">
         <v>1</v>
       </c>
       <c r="BF21" s="153"/>
-      <c r="BG21" s="152"/>
-      <c r="BH21" s="152"/>
+      <c r="BG21" s="152">
+        <f>BV14*BW14*BM21</f>
+        <v>315</v>
+      </c>
+      <c r="BH21" s="152">
+        <f>BG21*BE21</f>
+        <v>315</v>
+      </c>
       <c r="BI21" s="153"/>
       <c r="BJ21" s="152"/>
-      <c r="BK21" s="152"/>
+      <c r="BK21" s="152">
+        <f>BH21+BK15</f>
+        <v>405</v>
+      </c>
       <c r="BL21" s="153"/>
-      <c r="BM21" s="152"/>
-      <c r="BN21" s="152"/>
+      <c r="BM21" s="152">
+        <v>3.5</v>
+      </c>
+      <c r="BN21" s="152">
+        <f>BM21*BW14</f>
+        <v>1.75</v>
+      </c>
       <c r="BT21" s="160"/>
       <c r="BU21" s="160"/>
       <c r="BV21" s="154"/>
-      <c r="BW21" s="214"/>
-      <c r="BX21" s="214"/>
-    </row>
-    <row r="22" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BW21" s="154"/>
+      <c r="BX21" s="154"/>
+      <c r="BY21" s="154"/>
+    </row>
+    <row r="22" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A22" s="149"/>
       <c r="B22" s="153"/>
       <c r="C22" s="149"/>
@@ -12315,7 +12409,7 @@
       <c r="BW22" s="214"/>
       <c r="BX22" s="214"/>
     </row>
-    <row r="23" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A23" s="149"/>
       <c r="B23" s="153"/>
       <c r="C23" s="149"/>
@@ -12373,15 +12467,13 @@
       <c r="BL23" s="153"/>
       <c r="BM23" s="152"/>
       <c r="BN23" s="152"/>
-      <c r="BT23" s="185" t="s">
-        <v>396</v>
-      </c>
+      <c r="BT23" s="185"/>
       <c r="BU23" s="214"/>
       <c r="BV23" s="214"/>
       <c r="BW23" s="214"/>
       <c r="BX23" s="214"/>
     </row>
-    <row r="24" spans="1:76" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:77" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="149"/>
       <c r="B24" s="153"/>
       <c r="C24" s="149"/>
@@ -12425,27 +12517,47 @@
       <c r="AU24" s="152"/>
       <c r="AV24" s="152"/>
       <c r="AY24" s="164"/>
-      <c r="BA24" s="149"/>
+      <c r="BA24" s="149" t="s">
+        <v>458</v>
+      </c>
       <c r="BB24" s="153"/>
-      <c r="BC24" s="149"/>
+      <c r="BC24" s="149" t="s">
+        <v>447</v>
+      </c>
       <c r="BD24" s="149"/>
-      <c r="BE24" s="152"/>
+      <c r="BE24" s="152">
+        <v>0.5</v>
+      </c>
       <c r="BF24" s="153"/>
-      <c r="BG24" s="152"/>
-      <c r="BH24" s="152"/>
+      <c r="BG24" s="152">
+        <f>BV13*BW13*BM24</f>
+        <v>112.5</v>
+      </c>
+      <c r="BH24" s="152">
+        <f>BG24*BE24</f>
+        <v>56.25</v>
+      </c>
       <c r="BI24" s="153"/>
       <c r="BJ24" s="152"/>
-      <c r="BK24" s="152"/>
+      <c r="BK24" s="152">
+        <f>BH24+BK21</f>
+        <v>461.25</v>
+      </c>
       <c r="BL24" s="153"/>
-      <c r="BM24" s="152"/>
-      <c r="BN24" s="152"/>
+      <c r="BM24" s="152">
+        <v>0.5</v>
+      </c>
+      <c r="BN24" s="152">
+        <f>BN21*BE24+BM24</f>
+        <v>1.375</v>
+      </c>
       <c r="BT24" s="214"/>
       <c r="BU24" s="214"/>
       <c r="BV24" s="214"/>
       <c r="BW24" s="214"/>
       <c r="BX24" s="214"/>
     </row>
-    <row r="25" spans="1:76" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:77" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="149"/>
       <c r="B25" s="153"/>
       <c r="C25" s="149"/>
@@ -12503,23 +12615,19 @@
       <c r="BL25" s="153"/>
       <c r="BM25" s="152"/>
       <c r="BN25" s="152"/>
-      <c r="BP25" s="247" t="s">
-        <v>459</v>
-      </c>
-      <c r="BQ25" s="248"/>
-      <c r="BR25" s="248"/>
-      <c r="BS25" s="249"/>
-      <c r="BT25" s="119" t="s">
-        <v>397</v>
-      </c>
+      <c r="BP25" s="245" t="s">
+        <v>463</v>
+      </c>
+      <c r="BQ25" s="246"/>
+      <c r="BR25" s="246"/>
+      <c r="BS25" s="247"/>
+      <c r="BT25" s="119"/>
       <c r="BU25" s="214"/>
-      <c r="BV25" s="119" t="s">
-        <v>398</v>
-      </c>
+      <c r="BV25" s="119"/>
       <c r="BW25" s="214"/>
       <c r="BX25" s="214"/>
     </row>
-    <row r="26" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A26" s="149"/>
       <c r="B26" s="153"/>
       <c r="C26" s="149"/>
@@ -12578,7 +12686,7 @@
       <c r="BM26" s="152"/>
       <c r="BN26" s="152"/>
     </row>
-    <row r="27" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A27" s="149"/>
       <c r="B27" s="153"/>
       <c r="C27" s="149"/>
@@ -12622,11 +12730,17 @@
       <c r="AU27" s="152"/>
       <c r="AV27" s="152"/>
       <c r="AY27" s="164"/>
-      <c r="BA27" s="149"/>
+      <c r="BA27" s="149" t="s">
+        <v>454</v>
+      </c>
       <c r="BB27" s="153"/>
-      <c r="BC27" s="149"/>
+      <c r="BC27" s="149" t="s">
+        <v>455</v>
+      </c>
       <c r="BD27" s="149"/>
-      <c r="BE27" s="152"/>
+      <c r="BE27" s="152">
+        <v>1</v>
+      </c>
       <c r="BF27" s="153"/>
       <c r="BG27" s="152"/>
       <c r="BH27" s="152"/>
@@ -12637,7 +12751,7 @@
       <c r="BM27" s="152"/>
       <c r="BN27" s="152"/>
     </row>
-    <row r="28" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A28" s="149"/>
       <c r="B28" s="153"/>
       <c r="C28" s="149"/>
@@ -12683,9 +12797,13 @@
       <c r="AY28" s="164"/>
       <c r="BA28" s="149"/>
       <c r="BB28" s="153"/>
-      <c r="BC28" s="149"/>
+      <c r="BC28" s="149" t="s">
+        <v>458</v>
+      </c>
       <c r="BD28" s="149"/>
-      <c r="BE28" s="152"/>
+      <c r="BE28" s="152">
+        <v>3</v>
+      </c>
       <c r="BF28" s="153"/>
       <c r="BG28" s="152"/>
       <c r="BH28" s="152"/>
@@ -12695,14 +12813,14 @@
       <c r="BL28" s="153"/>
       <c r="BM28" s="152"/>
       <c r="BN28" s="152"/>
-      <c r="BP28" s="246" t="s">
+      <c r="BP28" s="252" t="s">
         <v>453</v>
       </c>
-      <c r="BQ28" s="246"/>
-      <c r="BR28" s="246"/>
-      <c r="BS28" s="246"/>
-    </row>
-    <row r="29" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BQ28" s="252"/>
+      <c r="BR28" s="252"/>
+      <c r="BS28" s="252"/>
+    </row>
+    <row r="29" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A29" s="149"/>
       <c r="B29" s="153"/>
       <c r="C29" s="149"/>
@@ -12760,16 +12878,16 @@
       <c r="BL29" s="153"/>
       <c r="BM29" s="152"/>
       <c r="BN29" s="152"/>
-      <c r="BP29" s="221"/>
-      <c r="BQ29" s="221"/>
-      <c r="BR29" s="224" t="s">
+      <c r="BP29" s="220"/>
+      <c r="BQ29" s="220"/>
+      <c r="BR29" s="223" t="s">
         <v>337</v>
       </c>
-      <c r="BS29" s="224" t="s">
+      <c r="BS29" s="223" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="30" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A30" s="149"/>
       <c r="B30" s="153"/>
       <c r="C30" s="149"/>
@@ -12827,14 +12945,14 @@
       <c r="BL30" s="153"/>
       <c r="BM30" s="152"/>
       <c r="BN30" s="152"/>
-      <c r="BP30" s="225" t="s">
+      <c r="BP30" s="224" t="s">
         <v>455</v>
       </c>
-      <c r="BQ30" s="223"/>
-      <c r="BR30" s="222"/>
-      <c r="BS30" s="222"/>
-    </row>
-    <row r="31" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BQ30" s="222"/>
+      <c r="BR30" s="221"/>
+      <c r="BS30" s="221"/>
+    </row>
+    <row r="31" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A31" s="149"/>
       <c r="B31" s="153"/>
       <c r="C31" s="149"/>
@@ -12892,14 +13010,14 @@
       <c r="BL31" s="153"/>
       <c r="BM31" s="152"/>
       <c r="BN31" s="152"/>
-      <c r="BP31" s="225" t="s">
+      <c r="BP31" s="224" t="s">
         <v>456</v>
       </c>
-      <c r="BQ31" s="223"/>
-      <c r="BR31" s="222"/>
-      <c r="BS31" s="222"/>
-    </row>
-    <row r="32" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BQ31" s="222"/>
+      <c r="BR31" s="221"/>
+      <c r="BS31" s="221"/>
+    </row>
+    <row r="32" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A32" s="149"/>
       <c r="B32" s="153"/>
       <c r="C32" s="149"/>
@@ -12957,12 +13075,12 @@
       <c r="BL32" s="153"/>
       <c r="BM32" s="152"/>
       <c r="BN32" s="152"/>
-      <c r="BP32" s="225" t="s">
+      <c r="BP32" s="224" t="s">
         <v>457</v>
       </c>
-      <c r="BQ32" s="223"/>
-      <c r="BR32" s="222"/>
-      <c r="BS32" s="222"/>
+      <c r="BQ32" s="222"/>
+      <c r="BR32" s="221"/>
+      <c r="BS32" s="221"/>
     </row>
     <row r="33" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A33" s="149"/>
@@ -13022,14 +13140,14 @@
       <c r="BL33" s="153"/>
       <c r="BM33" s="152"/>
       <c r="BN33" s="152"/>
-      <c r="BP33" s="225" t="s">
+      <c r="BP33" s="224" t="s">
         <v>458</v>
       </c>
-      <c r="BQ33" s="223"/>
-      <c r="BR33" s="222">
+      <c r="BQ33" s="222"/>
+      <c r="BR33" s="221">
         <v>0.5</v>
       </c>
-      <c r="BS33" s="222">
+      <c r="BS33" s="221">
         <f>BV13*BW13*BR33</f>
         <v>112.5</v>
       </c>
@@ -13092,12 +13210,12 @@
       <c r="BL34" s="153"/>
       <c r="BM34" s="152"/>
       <c r="BN34" s="152"/>
-      <c r="BP34" s="225" t="s">
+      <c r="BP34" s="224" t="s">
         <v>454</v>
       </c>
-      <c r="BQ34" s="223"/>
-      <c r="BR34" s="222"/>
-      <c r="BS34" s="222"/>
+      <c r="BQ34" s="222"/>
+      <c r="BR34" s="221"/>
+      <c r="BS34" s="221"/>
     </row>
     <row r="35" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A35" s="149"/>
@@ -13157,10 +13275,10 @@
       <c r="BL35" s="153"/>
       <c r="BM35" s="152"/>
       <c r="BN35" s="152"/>
-      <c r="BP35" s="223"/>
-      <c r="BQ35" s="223"/>
-      <c r="BR35" s="222"/>
-      <c r="BS35" s="222"/>
+      <c r="BP35" s="222"/>
+      <c r="BQ35" s="222"/>
+      <c r="BR35" s="221"/>
+      <c r="BS35" s="221"/>
     </row>
     <row r="36" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A36" s="149"/>
@@ -13220,10 +13338,10 @@
       <c r="BL36" s="153"/>
       <c r="BM36" s="152"/>
       <c r="BN36" s="152"/>
-      <c r="BP36" s="223"/>
-      <c r="BQ36" s="223"/>
-      <c r="BR36" s="222"/>
-      <c r="BS36" s="222"/>
+      <c r="BP36" s="222"/>
+      <c r="BQ36" s="222"/>
+      <c r="BR36" s="221"/>
+      <c r="BS36" s="221"/>
     </row>
     <row r="37" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A37" s="149"/>
@@ -13854,14 +13972,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="BT9:BV9"/>
-    <mergeCell ref="BW9:BX9"/>
     <mergeCell ref="BP28:BS28"/>
     <mergeCell ref="BP25:BS25"/>
     <mergeCell ref="AY6:AZ7"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="BT9:BV9"/>
+    <mergeCell ref="BW9:BX9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13874,7 +13992,7 @@
   <dimension ref="A1:AC64"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6:Z22"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13918,13 +14036,13 @@
       <c r="A3" s="144" t="s">
         <v>333</v>
       </c>
-      <c r="D3" s="255" t="s">
+      <c r="D3" s="254" t="s">
         <v>344</v>
       </c>
-      <c r="E3" s="256"/>
-      <c r="F3" s="256"/>
-      <c r="G3" s="256"/>
-      <c r="H3" s="257"/>
+      <c r="E3" s="255"/>
+      <c r="F3" s="255"/>
+      <c r="G3" s="255"/>
+      <c r="H3" s="256"/>
       <c r="Q3" s="169" t="s">
         <v>345</v>
       </c>
@@ -13999,20 +14117,20 @@
         <v>338</v>
       </c>
       <c r="Q6" s="164"/>
-      <c r="R6" s="258" t="s">
+      <c r="R6" s="257" t="s">
         <v>346</v>
       </c>
-      <c r="S6" s="258"/>
+      <c r="S6" s="257"/>
       <c r="T6" s="165"/>
-      <c r="V6" s="253" t="s">
+      <c r="V6" s="250" t="s">
         <v>358</v>
       </c>
-      <c r="W6" s="253"/>
-      <c r="X6" s="253"/>
-      <c r="Y6" s="254" t="s">
+      <c r="W6" s="250"/>
+      <c r="X6" s="250"/>
+      <c r="Y6" s="251" t="s">
         <v>362</v>
       </c>
-      <c r="Z6" s="254"/>
+      <c r="Z6" s="251"/>
       <c r="AA6" s="150"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -15789,7 +15907,7 @@
   <dimension ref="A2:AA52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W10" sqref="W10:AA10"/>
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15810,14 +15928,14 @@
       <c r="A3" s="144" t="s">
         <v>333</v>
       </c>
-      <c r="C3" s="259" t="s">
+      <c r="C3" s="258" t="s">
         <v>403</v>
       </c>
-      <c r="D3" s="260"/>
-      <c r="E3" s="260"/>
-      <c r="F3" s="260"/>
-      <c r="G3" s="260"/>
-      <c r="H3" s="261"/>
+      <c r="D3" s="259"/>
+      <c r="E3" s="259"/>
+      <c r="F3" s="259"/>
+      <c r="G3" s="259"/>
+      <c r="H3" s="260"/>
       <c r="Q3" s="169" t="s">
         <v>345</v>
       </c>
@@ -15881,10 +15999,10 @@
         <v>338</v>
       </c>
       <c r="Q6" s="164"/>
-      <c r="R6" s="258" t="s">
+      <c r="R6" s="257" t="s">
         <v>346</v>
       </c>
-      <c r="S6" s="258"/>
+      <c r="S6" s="257"/>
       <c r="T6" s="165"/>
       <c r="U6" s="151"/>
       <c r="W6" s="187" t="s">
@@ -17325,94 +17443,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="263"/>
-      <c r="B1" s="263"/>
-      <c r="C1" s="227"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="227"/>
-      <c r="G1" s="227"/>
-      <c r="H1" s="227"/>
-      <c r="I1" s="227"/>
-      <c r="J1" s="227"/>
-      <c r="K1" s="227"/>
-      <c r="L1" s="227"/>
-      <c r="M1" s="227"/>
-      <c r="N1" s="227"/>
-      <c r="O1" s="227"/>
-      <c r="P1" s="227"/>
-      <c r="Q1" s="263"/>
+      <c r="A1" s="262"/>
+      <c r="B1" s="262"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="262"/>
+      <c r="E1" s="262"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="226"/>
+      <c r="K1" s="226"/>
+      <c r="L1" s="226"/>
+      <c r="M1" s="226"/>
+      <c r="N1" s="226"/>
+      <c r="O1" s="226"/>
+      <c r="P1" s="226"/>
+      <c r="Q1" s="262"/>
     </row>
     <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="227"/>
-      <c r="B2" s="262" t="s">
+      <c r="A2" s="226"/>
+      <c r="B2" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="227"/>
-      <c r="D2" s="227"/>
-      <c r="E2" s="271" t="s">
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="270" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="227"/>
-      <c r="G2" s="272" t="s">
+      <c r="F2" s="226"/>
+      <c r="G2" s="271" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="227"/>
-      <c r="I2" s="227"/>
-      <c r="J2" s="227"/>
-      <c r="K2" s="227"/>
-      <c r="L2" s="227"/>
-      <c r="M2" s="227"/>
-      <c r="N2" s="227"/>
-      <c r="O2" s="227"/>
-      <c r="P2" s="227"/>
-      <c r="Q2" s="227"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
+      <c r="J2" s="226"/>
+      <c r="K2" s="226"/>
+      <c r="L2" s="226"/>
+      <c r="M2" s="226"/>
+      <c r="N2" s="226"/>
+      <c r="O2" s="226"/>
+      <c r="P2" s="226"/>
+      <c r="Q2" s="226"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="227"/>
-      <c r="B3" s="263"/>
-      <c r="C3" s="227"/>
-      <c r="D3" s="227"/>
-      <c r="E3" s="263"/>
-      <c r="F3" s="227"/>
-      <c r="G3" s="227"/>
-      <c r="H3" s="227"/>
-      <c r="I3" s="227"/>
-      <c r="J3" s="227"/>
-      <c r="K3" s="227"/>
-      <c r="L3" s="227"/>
-      <c r="M3" s="227"/>
-      <c r="N3" s="227"/>
-      <c r="O3" s="227"/>
-      <c r="P3" s="227"/>
-      <c r="Q3" s="227"/>
+      <c r="A3" s="226"/>
+      <c r="B3" s="262"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="262"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
+      <c r="J3" s="226"/>
+      <c r="K3" s="226"/>
+      <c r="L3" s="226"/>
+      <c r="M3" s="226"/>
+      <c r="N3" s="226"/>
+      <c r="O3" s="226"/>
+      <c r="P3" s="226"/>
+      <c r="Q3" s="226"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="227"/>
-      <c r="B4" s="264"/>
-      <c r="C4" s="227"/>
-      <c r="D4" s="227"/>
-      <c r="E4" s="270" t="s">
+      <c r="A4" s="226"/>
+      <c r="B4" s="263"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="269" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="227"/>
-      <c r="H4" s="227"/>
-      <c r="I4" s="227"/>
-      <c r="J4" s="227"/>
-      <c r="K4" s="227"/>
-      <c r="L4" s="227"/>
-      <c r="M4" s="227"/>
-      <c r="N4" s="227"/>
-      <c r="O4" s="227"/>
-      <c r="P4" s="227"/>
-      <c r="Q4" s="227"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
+      <c r="L4" s="226"/>
+      <c r="M4" s="226"/>
+      <c r="N4" s="226"/>
+      <c r="O4" s="226"/>
+      <c r="P4" s="226"/>
+      <c r="Q4" s="226"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="227"/>
+      <c r="A5" s="226"/>
       <c r="B5" s="11"/>
       <c r="C5" s="34"/>
-      <c r="D5" s="227"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="35" t="s">
         <v>104</v>
       </c>
@@ -17449,13 +17567,13 @@
       <c r="P5" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="Q5" s="227"/>
+      <c r="Q5" s="226"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="227"/>
+      <c r="A6" s="226"/>
       <c r="B6" s="11"/>
       <c r="C6" s="34"/>
-      <c r="D6" s="227"/>
+      <c r="D6" s="226"/>
       <c r="E6" s="47">
         <v>0</v>
       </c>
@@ -17494,55 +17612,55 @@
       <c r="P6" s="47">
         <v>150</v>
       </c>
-      <c r="Q6" s="227"/>
+      <c r="Q6" s="226"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="227"/>
-      <c r="B7" s="265"/>
-      <c r="C7" s="227"/>
-      <c r="D7" s="227"/>
-      <c r="E7" s="263"/>
-      <c r="F7" s="227"/>
-      <c r="G7" s="227"/>
-      <c r="H7" s="227"/>
-      <c r="I7" s="227"/>
-      <c r="J7" s="227"/>
-      <c r="K7" s="227"/>
-      <c r="L7" s="227"/>
-      <c r="M7" s="227"/>
-      <c r="N7" s="227"/>
-      <c r="O7" s="227"/>
-      <c r="P7" s="227"/>
-      <c r="Q7" s="227"/>
+      <c r="A7" s="226"/>
+      <c r="B7" s="264"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="262"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
+      <c r="L7" s="226"/>
+      <c r="M7" s="226"/>
+      <c r="N7" s="226"/>
+      <c r="O7" s="226"/>
+      <c r="P7" s="226"/>
+      <c r="Q7" s="226"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="227"/>
-      <c r="B8" s="264" t="s">
+      <c r="A8" s="226"/>
+      <c r="B8" s="263" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="227"/>
-      <c r="D8" s="227"/>
-      <c r="E8" s="266" t="s">
+      <c r="C8" s="226"/>
+      <c r="D8" s="226"/>
+      <c r="E8" s="265" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="227"/>
-      <c r="G8" s="227"/>
-      <c r="H8" s="227"/>
-      <c r="I8" s="227"/>
-      <c r="J8" s="227"/>
-      <c r="K8" s="227"/>
-      <c r="L8" s="227"/>
-      <c r="M8" s="227"/>
-      <c r="N8" s="227"/>
-      <c r="O8" s="227"/>
-      <c r="P8" s="227"/>
-      <c r="Q8" s="227"/>
+      <c r="F8" s="226"/>
+      <c r="G8" s="226"/>
+      <c r="H8" s="226"/>
+      <c r="I8" s="226"/>
+      <c r="J8" s="226"/>
+      <c r="K8" s="226"/>
+      <c r="L8" s="226"/>
+      <c r="M8" s="226"/>
+      <c r="N8" s="226"/>
+      <c r="O8" s="226"/>
+      <c r="P8" s="226"/>
+      <c r="Q8" s="226"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="227"/>
+      <c r="A9" s="226"/>
       <c r="B9" s="11"/>
       <c r="C9" s="54"/>
-      <c r="D9" s="227"/>
+      <c r="D9" s="226"/>
       <c r="E9" s="55">
         <v>1</v>
       </c>
@@ -17577,13 +17695,13 @@
       <c r="P9" s="59">
         <v>1</v>
       </c>
-      <c r="Q9" s="227"/>
+      <c r="Q9" s="226"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="227"/>
+      <c r="A10" s="226"/>
       <c r="B10" s="11"/>
       <c r="C10" s="54"/>
-      <c r="D10" s="227"/>
+      <c r="D10" s="226"/>
       <c r="E10" s="55">
         <v>2</v>
       </c>
@@ -17618,13 +17736,13 @@
       <c r="P10" s="59">
         <v>1.5</v>
       </c>
-      <c r="Q10" s="227"/>
+      <c r="Q10" s="226"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="227"/>
+      <c r="A11" s="226"/>
       <c r="B11" s="11"/>
       <c r="C11" s="54"/>
-      <c r="D11" s="227"/>
+      <c r="D11" s="226"/>
       <c r="E11" s="55">
         <v>3</v>
       </c>
@@ -17659,17 +17777,17 @@
       <c r="P11" s="59">
         <v>2</v>
       </c>
-      <c r="Q11" s="227"/>
+      <c r="Q11" s="226"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="227"/>
+      <c r="A12" s="226"/>
       <c r="B12" s="11" t="s">
         <v>161</v>
       </c>
       <c r="C12" s="54">
         <v>1</v>
       </c>
-      <c r="D12" s="227"/>
+      <c r="D12" s="226"/>
       <c r="E12" s="11" t="s">
         <v>162</v>
       </c>
@@ -17706,17 +17824,17 @@
       <c r="P12" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="Q12" s="227"/>
+      <c r="Q12" s="226"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="227"/>
+      <c r="A13" s="226"/>
       <c r="B13" s="11" t="s">
         <v>174</v>
       </c>
       <c r="C13" s="54">
         <v>1</v>
       </c>
-      <c r="D13" s="227"/>
+      <c r="D13" s="226"/>
       <c r="E13" s="55">
         <v>1</v>
       </c>
@@ -17764,17 +17882,17 @@
         <f t="shared" ref="P13:P15" si="5">P$6*P9</f>
         <v>150</v>
       </c>
-      <c r="Q13" s="227"/>
+      <c r="Q13" s="226"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="227"/>
+      <c r="A14" s="226"/>
       <c r="B14" s="11" t="s">
         <v>176</v>
       </c>
       <c r="C14" s="54">
         <v>1</v>
       </c>
-      <c r="D14" s="227"/>
+      <c r="D14" s="226"/>
       <c r="E14" s="55">
         <v>2</v>
       </c>
@@ -17819,13 +17937,13 @@
         <f t="shared" si="5"/>
         <v>225</v>
       </c>
-      <c r="Q14" s="227"/>
+      <c r="Q14" s="226"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="227"/>
+      <c r="A15" s="226"/>
       <c r="B15" s="11"/>
       <c r="C15" s="34"/>
-      <c r="D15" s="227"/>
+      <c r="D15" s="226"/>
       <c r="E15" s="55">
         <v>3</v>
       </c>
@@ -17870,55 +17988,55 @@
         <f t="shared" si="5"/>
         <v>300</v>
       </c>
-      <c r="Q15" s="227"/>
+      <c r="Q15" s="226"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="227"/>
-      <c r="B16" s="265"/>
-      <c r="C16" s="227"/>
-      <c r="D16" s="227"/>
-      <c r="E16" s="263"/>
-      <c r="F16" s="227"/>
-      <c r="G16" s="227"/>
-      <c r="H16" s="227"/>
-      <c r="I16" s="227"/>
-      <c r="J16" s="227"/>
-      <c r="K16" s="227"/>
-      <c r="L16" s="227"/>
-      <c r="M16" s="227"/>
+      <c r="A16" s="226"/>
+      <c r="B16" s="264"/>
+      <c r="C16" s="226"/>
+      <c r="D16" s="226"/>
+      <c r="E16" s="262"/>
+      <c r="F16" s="226"/>
+      <c r="G16" s="226"/>
+      <c r="H16" s="226"/>
+      <c r="I16" s="226"/>
+      <c r="J16" s="226"/>
+      <c r="K16" s="226"/>
+      <c r="L16" s="226"/>
+      <c r="M16" s="226"/>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
-      <c r="Q16" s="227"/>
+      <c r="Q16" s="226"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="227"/>
-      <c r="B17" s="264" t="s">
+      <c r="A17" s="226"/>
+      <c r="B17" s="263" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="227"/>
-      <c r="D17" s="227"/>
-      <c r="E17" s="268" t="s">
+      <c r="C17" s="226"/>
+      <c r="D17" s="226"/>
+      <c r="E17" s="267" t="s">
         <v>183</v>
       </c>
-      <c r="F17" s="227"/>
-      <c r="G17" s="227"/>
-      <c r="H17" s="227"/>
-      <c r="I17" s="227"/>
-      <c r="J17" s="227"/>
-      <c r="K17" s="227"/>
-      <c r="L17" s="227"/>
-      <c r="M17" s="227"/>
-      <c r="N17" s="227"/>
-      <c r="O17" s="227"/>
-      <c r="P17" s="227"/>
-      <c r="Q17" s="227"/>
+      <c r="F17" s="226"/>
+      <c r="G17" s="226"/>
+      <c r="H17" s="226"/>
+      <c r="I17" s="226"/>
+      <c r="J17" s="226"/>
+      <c r="K17" s="226"/>
+      <c r="L17" s="226"/>
+      <c r="M17" s="226"/>
+      <c r="N17" s="226"/>
+      <c r="O17" s="226"/>
+      <c r="P17" s="226"/>
+      <c r="Q17" s="226"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="227"/>
+      <c r="A18" s="226"/>
       <c r="B18" s="11"/>
       <c r="C18" s="34"/>
-      <c r="D18" s="227"/>
+      <c r="D18" s="226"/>
       <c r="E18" s="42">
         <v>1</v>
       </c>
@@ -17947,13 +18065,13 @@
       <c r="P18" s="78">
         <v>2</v>
       </c>
-      <c r="Q18" s="227"/>
+      <c r="Q18" s="226"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="227"/>
+      <c r="A19" s="226"/>
       <c r="B19" s="11"/>
       <c r="C19" s="34"/>
-      <c r="D19" s="227"/>
+      <c r="D19" s="226"/>
       <c r="E19" s="42">
         <v>2</v>
       </c>
@@ -17982,13 +18100,13 @@
       <c r="P19" s="78">
         <v>3</v>
       </c>
-      <c r="Q19" s="227"/>
+      <c r="Q19" s="226"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="227"/>
+      <c r="A20" s="226"/>
       <c r="B20" s="11"/>
       <c r="C20" s="34"/>
-      <c r="D20" s="227"/>
+      <c r="D20" s="226"/>
       <c r="E20" s="42">
         <v>3</v>
       </c>
@@ -18017,13 +18135,13 @@
       <c r="P20" s="78">
         <v>4</v>
       </c>
-      <c r="Q20" s="227"/>
+      <c r="Q20" s="226"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="227"/>
+      <c r="A21" s="226"/>
       <c r="B21" s="11"/>
       <c r="C21" s="34"/>
-      <c r="D21" s="227"/>
+      <c r="D21" s="226"/>
       <c r="E21" s="20" t="s">
         <v>205</v>
       </c>
@@ -18058,13 +18176,13 @@
       <c r="P21" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="Q21" s="227"/>
+      <c r="Q21" s="226"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="227"/>
+      <c r="A22" s="226"/>
       <c r="B22" s="11"/>
       <c r="C22" s="34"/>
-      <c r="D22" s="227"/>
+      <c r="D22" s="226"/>
       <c r="E22" s="42">
         <v>1</v>
       </c>
@@ -18109,13 +18227,13 @@
         <f t="shared" ref="P22:P24" si="15">P$6*P18</f>
         <v>300</v>
       </c>
-      <c r="Q22" s="227"/>
+      <c r="Q22" s="226"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="227"/>
+      <c r="A23" s="226"/>
       <c r="B23" s="11"/>
       <c r="C23" s="34"/>
-      <c r="D23" s="227"/>
+      <c r="D23" s="226"/>
       <c r="E23" s="42">
         <v>2</v>
       </c>
@@ -18160,13 +18278,13 @@
         <f t="shared" si="15"/>
         <v>450</v>
       </c>
-      <c r="Q23" s="227"/>
+      <c r="Q23" s="226"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="227"/>
+      <c r="A24" s="226"/>
       <c r="B24" s="11"/>
       <c r="C24" s="34"/>
-      <c r="D24" s="227"/>
+      <c r="D24" s="226"/>
       <c r="E24" s="42">
         <v>3</v>
       </c>
@@ -18211,55 +18329,55 @@
         <f t="shared" si="15"/>
         <v>600</v>
       </c>
-      <c r="Q24" s="227"/>
+      <c r="Q24" s="226"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="227"/>
-      <c r="B25" s="265"/>
-      <c r="C25" s="227"/>
-      <c r="D25" s="227"/>
-      <c r="E25" s="263"/>
-      <c r="F25" s="227"/>
-      <c r="G25" s="227"/>
-      <c r="H25" s="227"/>
-      <c r="I25" s="227"/>
-      <c r="J25" s="227"/>
-      <c r="K25" s="227"/>
-      <c r="L25" s="227"/>
-      <c r="M25" s="227"/>
+      <c r="A25" s="226"/>
+      <c r="B25" s="264"/>
+      <c r="C25" s="226"/>
+      <c r="D25" s="226"/>
+      <c r="E25" s="262"/>
+      <c r="F25" s="226"/>
+      <c r="G25" s="226"/>
+      <c r="H25" s="226"/>
+      <c r="I25" s="226"/>
+      <c r="J25" s="226"/>
+      <c r="K25" s="226"/>
+      <c r="L25" s="226"/>
+      <c r="M25" s="226"/>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
-      <c r="Q25" s="227"/>
+      <c r="Q25" s="226"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="227"/>
-      <c r="B26" s="264" t="s">
+      <c r="A26" s="226"/>
+      <c r="B26" s="263" t="s">
         <v>216</v>
       </c>
-      <c r="C26" s="227"/>
-      <c r="D26" s="227"/>
-      <c r="E26" s="269" t="s">
+      <c r="C26" s="226"/>
+      <c r="D26" s="226"/>
+      <c r="E26" s="268" t="s">
         <v>217</v>
       </c>
-      <c r="F26" s="227"/>
-      <c r="G26" s="227"/>
-      <c r="H26" s="227"/>
-      <c r="I26" s="227"/>
-      <c r="J26" s="227"/>
-      <c r="K26" s="227"/>
-      <c r="L26" s="227"/>
-      <c r="M26" s="227"/>
-      <c r="N26" s="227"/>
-      <c r="O26" s="227"/>
-      <c r="P26" s="227"/>
-      <c r="Q26" s="227"/>
+      <c r="F26" s="226"/>
+      <c r="G26" s="226"/>
+      <c r="H26" s="226"/>
+      <c r="I26" s="226"/>
+      <c r="J26" s="226"/>
+      <c r="K26" s="226"/>
+      <c r="L26" s="226"/>
+      <c r="M26" s="226"/>
+      <c r="N26" s="226"/>
+      <c r="O26" s="226"/>
+      <c r="P26" s="226"/>
+      <c r="Q26" s="226"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="227"/>
+      <c r="A27" s="226"/>
       <c r="B27" s="11"/>
       <c r="C27" s="34"/>
-      <c r="D27" s="227"/>
+      <c r="D27" s="226"/>
       <c r="E27" s="72">
         <v>1</v>
       </c>
@@ -18282,13 +18400,13 @@
       </c>
       <c r="O27" s="92"/>
       <c r="P27" s="91"/>
-      <c r="Q27" s="227"/>
+      <c r="Q27" s="226"/>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="227"/>
+      <c r="A28" s="226"/>
       <c r="B28" s="11"/>
       <c r="C28" s="34"/>
-      <c r="D28" s="227"/>
+      <c r="D28" s="226"/>
       <c r="E28" s="72">
         <v>2</v>
       </c>
@@ -18311,13 +18429,13 @@
       </c>
       <c r="O28" s="92"/>
       <c r="P28" s="91"/>
-      <c r="Q28" s="227"/>
+      <c r="Q28" s="226"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="227"/>
+      <c r="A29" s="226"/>
       <c r="B29" s="11"/>
       <c r="C29" s="34"/>
-      <c r="D29" s="227"/>
+      <c r="D29" s="226"/>
       <c r="E29" s="72">
         <v>3</v>
       </c>
@@ -18340,13 +18458,13 @@
       </c>
       <c r="O29" s="92"/>
       <c r="P29" s="91"/>
-      <c r="Q29" s="227"/>
+      <c r="Q29" s="226"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="227"/>
+      <c r="A30" s="226"/>
       <c r="B30" s="11"/>
       <c r="C30" s="34"/>
-      <c r="D30" s="227"/>
+      <c r="D30" s="226"/>
       <c r="E30" s="3" t="s">
         <v>227</v>
       </c>
@@ -18381,13 +18499,13 @@
       <c r="P30" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="Q30" s="227"/>
+      <c r="Q30" s="226"/>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="227"/>
+      <c r="A31" s="226"/>
       <c r="B31" s="11"/>
       <c r="C31" s="34"/>
-      <c r="D31" s="227"/>
+      <c r="D31" s="226"/>
       <c r="E31" s="72">
         <v>1</v>
       </c>
@@ -18432,13 +18550,13 @@
         <f t="shared" ref="P31:P33" si="25">P$6*P27</f>
         <v>0</v>
       </c>
-      <c r="Q31" s="227"/>
+      <c r="Q31" s="226"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="227"/>
+      <c r="A32" s="226"/>
       <c r="B32" s="11"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="227"/>
+      <c r="D32" s="226"/>
       <c r="E32" s="72">
         <v>2</v>
       </c>
@@ -18483,13 +18601,13 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="227"/>
+      <c r="Q32" s="226"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="227"/>
+      <c r="A33" s="226"/>
       <c r="B33" s="11"/>
       <c r="C33" s="34"/>
-      <c r="D33" s="227"/>
+      <c r="D33" s="226"/>
       <c r="E33" s="72">
         <v>3</v>
       </c>
@@ -18534,55 +18652,55 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="Q33" s="227"/>
+      <c r="Q33" s="226"/>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="227"/>
-      <c r="B34" s="265"/>
-      <c r="C34" s="227"/>
-      <c r="D34" s="227"/>
-      <c r="E34" s="263"/>
-      <c r="F34" s="227"/>
-      <c r="G34" s="227"/>
-      <c r="H34" s="227"/>
-      <c r="I34" s="227"/>
-      <c r="J34" s="227"/>
-      <c r="K34" s="227"/>
-      <c r="L34" s="227"/>
-      <c r="M34" s="227"/>
+      <c r="A34" s="226"/>
+      <c r="B34" s="264"/>
+      <c r="C34" s="226"/>
+      <c r="D34" s="226"/>
+      <c r="E34" s="262"/>
+      <c r="F34" s="226"/>
+      <c r="G34" s="226"/>
+      <c r="H34" s="226"/>
+      <c r="I34" s="226"/>
+      <c r="J34" s="226"/>
+      <c r="K34" s="226"/>
+      <c r="L34" s="226"/>
+      <c r="M34" s="226"/>
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
-      <c r="Q34" s="227"/>
+      <c r="Q34" s="226"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="227"/>
-      <c r="B35" s="264" t="s">
+      <c r="A35" s="226"/>
+      <c r="B35" s="263" t="s">
         <v>246</v>
       </c>
-      <c r="C35" s="227"/>
-      <c r="D35" s="227"/>
-      <c r="E35" s="267" t="s">
+      <c r="C35" s="226"/>
+      <c r="D35" s="226"/>
+      <c r="E35" s="266" t="s">
         <v>247</v>
       </c>
-      <c r="F35" s="227"/>
-      <c r="G35" s="227"/>
-      <c r="H35" s="227"/>
-      <c r="I35" s="227"/>
-      <c r="J35" s="227"/>
-      <c r="K35" s="227"/>
-      <c r="L35" s="227"/>
-      <c r="M35" s="227"/>
-      <c r="N35" s="227"/>
-      <c r="O35" s="227"/>
-      <c r="P35" s="227"/>
-      <c r="Q35" s="227"/>
+      <c r="F35" s="226"/>
+      <c r="G35" s="226"/>
+      <c r="H35" s="226"/>
+      <c r="I35" s="226"/>
+      <c r="J35" s="226"/>
+      <c r="K35" s="226"/>
+      <c r="L35" s="226"/>
+      <c r="M35" s="226"/>
+      <c r="N35" s="226"/>
+      <c r="O35" s="226"/>
+      <c r="P35" s="226"/>
+      <c r="Q35" s="226"/>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="227"/>
+      <c r="A36" s="226"/>
       <c r="B36" s="11"/>
       <c r="C36" s="34"/>
-      <c r="D36" s="227"/>
+      <c r="D36" s="226"/>
       <c r="E36" s="102">
         <v>1</v>
       </c>
@@ -18605,13 +18723,13 @@
       </c>
       <c r="O36" s="104"/>
       <c r="P36" s="103"/>
-      <c r="Q36" s="227"/>
+      <c r="Q36" s="226"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="227"/>
+      <c r="A37" s="226"/>
       <c r="B37" s="11"/>
       <c r="C37" s="34"/>
-      <c r="D37" s="227"/>
+      <c r="D37" s="226"/>
       <c r="E37" s="102">
         <v>2</v>
       </c>
@@ -18634,13 +18752,13 @@
       </c>
       <c r="O37" s="104"/>
       <c r="P37" s="103"/>
-      <c r="Q37" s="227"/>
+      <c r="Q37" s="226"/>
     </row>
     <row r="38" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="227"/>
+      <c r="A38" s="226"/>
       <c r="B38" s="11"/>
       <c r="C38" s="34"/>
-      <c r="D38" s="227"/>
+      <c r="D38" s="226"/>
       <c r="E38" s="102">
         <v>3</v>
       </c>
@@ -18663,13 +18781,13 @@
       </c>
       <c r="O38" s="104"/>
       <c r="P38" s="103"/>
-      <c r="Q38" s="227"/>
+      <c r="Q38" s="226"/>
     </row>
     <row r="39" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="227"/>
+      <c r="A39" s="226"/>
       <c r="B39" s="11"/>
       <c r="C39" s="34"/>
-      <c r="D39" s="227"/>
+      <c r="D39" s="226"/>
       <c r="E39" s="105" t="s">
         <v>257</v>
       </c>
@@ -18704,13 +18822,13 @@
       <c r="P39" s="105" t="s">
         <v>270</v>
       </c>
-      <c r="Q39" s="227"/>
+      <c r="Q39" s="226"/>
     </row>
     <row r="40" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="227"/>
+      <c r="A40" s="226"/>
       <c r="B40" s="11"/>
       <c r="C40" s="34"/>
-      <c r="D40" s="227"/>
+      <c r="D40" s="226"/>
       <c r="E40" s="102">
         <v>1</v>
       </c>
@@ -18755,13 +18873,13 @@
         <f t="shared" ref="P40:P42" si="35">P$6*P36</f>
         <v>0</v>
       </c>
-      <c r="Q40" s="227"/>
+      <c r="Q40" s="226"/>
     </row>
     <row r="41" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="227"/>
+      <c r="A41" s="226"/>
       <c r="B41" s="11"/>
       <c r="C41" s="34"/>
-      <c r="D41" s="227"/>
+      <c r="D41" s="226"/>
       <c r="E41" s="102">
         <v>2</v>
       </c>
@@ -18806,13 +18924,13 @@
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="Q41" s="227"/>
+      <c r="Q41" s="226"/>
     </row>
     <row r="42" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="227"/>
+      <c r="A42" s="226"/>
       <c r="B42" s="11"/>
       <c r="C42" s="34"/>
-      <c r="D42" s="227"/>
+      <c r="D42" s="226"/>
       <c r="E42" s="102">
         <v>3</v>
       </c>
@@ -18857,13 +18975,13 @@
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="227"/>
+      <c r="Q42" s="226"/>
     </row>
     <row r="43" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="227"/>
+      <c r="A43" s="226"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
-      <c r="D43" s="227"/>
+      <c r="D43" s="226"/>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
@@ -18876,7 +18994,7 @@
       <c r="N43" s="15"/>
       <c r="O43" s="15"/>
       <c r="P43" s="15"/>
-      <c r="Q43" s="227"/>
+      <c r="Q43" s="226"/>
     </row>
   </sheetData>
   <mergeCells count="28">
@@ -18919,7 +19037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -18950,24 +19068,24 @@
       <c r="B1" s="216">
         <v>1.5</v>
       </c>
-      <c r="C1" s="273" t="s">
+      <c r="C1" s="272" t="s">
         <v>417</v>
       </c>
-      <c r="D1" s="274"/>
-      <c r="E1" s="274"/>
-      <c r="F1" s="274"/>
-      <c r="G1" s="274"/>
-      <c r="H1" s="274"/>
-      <c r="I1" s="275"/>
-      <c r="J1" s="273" t="s">
+      <c r="D1" s="273"/>
+      <c r="E1" s="273"/>
+      <c r="F1" s="273"/>
+      <c r="G1" s="273"/>
+      <c r="H1" s="273"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="272" t="s">
         <v>418</v>
       </c>
-      <c r="K1" s="274"/>
-      <c r="L1" s="274"/>
-      <c r="M1" s="274"/>
-      <c r="N1" s="274"/>
-      <c r="O1" s="274"/>
-      <c r="P1" s="275"/>
+      <c r="K1" s="273"/>
+      <c r="L1" s="273"/>
+      <c r="M1" s="273"/>
+      <c r="N1" s="273"/>
+      <c r="O1" s="273"/>
+      <c r="P1" s="274"/>
     </row>
     <row r="2" spans="1:16" ht="27" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="215" t="s">
@@ -20644,60 +20762,60 @@
   </cols>
   <sheetData>
     <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="244" t="s">
+      <c r="A26" s="243" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="227"/>
-      <c r="C26" s="227"/>
+      <c r="B26" s="226"/>
+      <c r="C26" s="226"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="243"/>
-      <c r="B27" s="227"/>
+      <c r="A27" s="242"/>
+      <c r="B27" s="226"/>
       <c r="C27" s="50"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="243"/>
-      <c r="B28" s="227"/>
+      <c r="A28" s="242"/>
+      <c r="B28" s="226"/>
       <c r="C28" s="51"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="243"/>
-      <c r="B29" s="227"/>
+      <c r="A29" s="242"/>
+      <c r="B29" s="226"/>
       <c r="C29" s="121"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="243"/>
-      <c r="B30" s="227"/>
+      <c r="A30" s="242"/>
+      <c r="B30" s="226"/>
       <c r="C30" s="53"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="243"/>
-      <c r="B31" s="227"/>
+      <c r="A31" s="242"/>
+      <c r="B31" s="226"/>
       <c r="C31" s="53"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="241"/>
-      <c r="B32" s="227"/>
+      <c r="A32" s="240"/>
+      <c r="B32" s="226"/>
       <c r="C32" s="121"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="240"/>
-      <c r="B33" s="227"/>
+      <c r="A33" s="239"/>
+      <c r="B33" s="226"/>
       <c r="C33" s="53"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="240"/>
-      <c r="B34" s="227"/>
+      <c r="A34" s="239"/>
+      <c r="B34" s="226"/>
       <c r="C34" s="53"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="240"/>
-      <c r="B35" s="227"/>
+      <c r="A35" s="239"/>
+      <c r="B35" s="226"/>
       <c r="C35" s="53"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="240"/>
-      <c r="B36" s="227"/>
+      <c r="A36" s="239"/>
+      <c r="B36" s="226"/>
       <c r="C36" s="53"/>
     </row>
   </sheetData>

</xml_diff>